<commit_message>
coding sheep sim inputs
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3ED61-2BCA-4AFA-BDE2-AAFF8B2F4FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF4503B-79A8-421E-860B-9CA68057B53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -187,7 +187,7 @@
     <definedName name="yield_by_lmu" localSheetId="5">Crop!$I$238:$N$250</definedName>
     <definedName name="yield_penalty" localSheetId="5">Crop!$H$84:$J$96</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6245,6 +6245,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="16" borderId="15" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -6288,7 +6289,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Calculations" xfId="10" xr:uid="{449B9FA0-BCFF-41FE-A9C5-7F4DFD2D1D3B}"/>
@@ -15878,21 +15878,21 @@
       <c r="E46" s="140"/>
       <c r="F46" s="142"/>
       <c r="G46" s="151"/>
-      <c r="H46" s="444" t="s">
+      <c r="H46" s="445" t="s">
         <v>164</v>
       </c>
-      <c r="I46" s="445"/>
-      <c r="J46" s="445"/>
-      <c r="K46" s="445"/>
-      <c r="L46" s="445"/>
-      <c r="M46" s="445"/>
-      <c r="N46" s="445"/>
-      <c r="O46" s="445"/>
-      <c r="P46" s="445"/>
-      <c r="Q46" s="445"/>
-      <c r="R46" s="445"/>
-      <c r="S46" s="445"/>
-      <c r="T46" s="446"/>
+      <c r="I46" s="446"/>
+      <c r="J46" s="446"/>
+      <c r="K46" s="446"/>
+      <c r="L46" s="446"/>
+      <c r="M46" s="446"/>
+      <c r="N46" s="446"/>
+      <c r="O46" s="446"/>
+      <c r="P46" s="446"/>
+      <c r="Q46" s="446"/>
+      <c r="R46" s="446"/>
+      <c r="S46" s="446"/>
+      <c r="T46" s="447"/>
       <c r="U46" s="151"/>
       <c r="V46" s="142"/>
       <c r="W46" s="122"/>
@@ -15906,19 +15906,19 @@
       <c r="E47" s="140"/>
       <c r="F47" s="142"/>
       <c r="G47" s="151"/>
-      <c r="H47" s="447"/>
-      <c r="I47" s="448"/>
-      <c r="J47" s="448"/>
-      <c r="K47" s="448"/>
-      <c r="L47" s="448"/>
-      <c r="M47" s="448"/>
-      <c r="N47" s="448"/>
-      <c r="O47" s="448"/>
-      <c r="P47" s="448"/>
-      <c r="Q47" s="448"/>
-      <c r="R47" s="448"/>
-      <c r="S47" s="448"/>
-      <c r="T47" s="449"/>
+      <c r="H47" s="448"/>
+      <c r="I47" s="449"/>
+      <c r="J47" s="449"/>
+      <c r="K47" s="449"/>
+      <c r="L47" s="449"/>
+      <c r="M47" s="449"/>
+      <c r="N47" s="449"/>
+      <c r="O47" s="449"/>
+      <c r="P47" s="449"/>
+      <c r="Q47" s="449"/>
+      <c r="R47" s="449"/>
+      <c r="S47" s="449"/>
+      <c r="T47" s="450"/>
       <c r="U47" s="151"/>
       <c r="V47" s="142"/>
       <c r="W47" s="122"/>
@@ -15932,19 +15932,19 @@
       <c r="E48" s="140"/>
       <c r="F48" s="142"/>
       <c r="G48" s="151"/>
-      <c r="H48" s="447"/>
-      <c r="I48" s="448"/>
-      <c r="J48" s="448"/>
-      <c r="K48" s="448"/>
-      <c r="L48" s="448"/>
-      <c r="M48" s="448"/>
-      <c r="N48" s="448"/>
-      <c r="O48" s="448"/>
-      <c r="P48" s="448"/>
-      <c r="Q48" s="448"/>
-      <c r="R48" s="448"/>
-      <c r="S48" s="448"/>
-      <c r="T48" s="449"/>
+      <c r="H48" s="448"/>
+      <c r="I48" s="449"/>
+      <c r="J48" s="449"/>
+      <c r="K48" s="449"/>
+      <c r="L48" s="449"/>
+      <c r="M48" s="449"/>
+      <c r="N48" s="449"/>
+      <c r="O48" s="449"/>
+      <c r="P48" s="449"/>
+      <c r="Q48" s="449"/>
+      <c r="R48" s="449"/>
+      <c r="S48" s="449"/>
+      <c r="T48" s="450"/>
       <c r="U48" s="151"/>
       <c r="V48" s="142"/>
       <c r="W48" s="122"/>
@@ -15958,19 +15958,19 @@
       <c r="E49" s="140"/>
       <c r="F49" s="142"/>
       <c r="G49" s="151"/>
-      <c r="H49" s="450"/>
-      <c r="I49" s="451"/>
-      <c r="J49" s="451"/>
-      <c r="K49" s="451"/>
-      <c r="L49" s="451"/>
-      <c r="M49" s="451"/>
-      <c r="N49" s="451"/>
-      <c r="O49" s="451"/>
-      <c r="P49" s="451"/>
-      <c r="Q49" s="451"/>
-      <c r="R49" s="451"/>
-      <c r="S49" s="451"/>
-      <c r="T49" s="452"/>
+      <c r="H49" s="451"/>
+      <c r="I49" s="452"/>
+      <c r="J49" s="452"/>
+      <c r="K49" s="452"/>
+      <c r="L49" s="452"/>
+      <c r="M49" s="452"/>
+      <c r="N49" s="452"/>
+      <c r="O49" s="452"/>
+      <c r="P49" s="452"/>
+      <c r="Q49" s="452"/>
+      <c r="R49" s="452"/>
+      <c r="S49" s="452"/>
+      <c r="T49" s="453"/>
       <c r="U49" s="151"/>
       <c r="V49" s="142"/>
       <c r="W49" s="122"/>
@@ -30547,9 +30547,9 @@
       <c r="I318" s="252"/>
       <c r="J318" s="252"/>
       <c r="K318" s="139"/>
-      <c r="L318" s="453"/>
-      <c r="M318" s="454"/>
-      <c r="N318" s="454"/>
+      <c r="L318" s="454"/>
+      <c r="M318" s="455"/>
+      <c r="N318" s="455"/>
       <c r="O318" s="139"/>
       <c r="P318" s="139"/>
       <c r="Q318" s="139"/>
@@ -36101,8 +36101,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AP506"/>
   <sheetViews>
-    <sheetView topLeftCell="A478" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K121" sqref="K121"/>
+    <sheetView tabSelected="1" topLeftCell="A349" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S382" sqref="S382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="12" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -47530,7 +47530,7 @@
       <c r="E397" s="13"/>
       <c r="F397" s="13"/>
       <c r="G397" s="13"/>
-      <c r="H397" s="455"/>
+      <c r="H397" s="456"/>
       <c r="I397" s="13"/>
       <c r="J397" s="13"/>
       <c r="K397" s="18"/>
@@ -47558,7 +47558,7 @@
       <c r="E398" s="13"/>
       <c r="F398" s="13"/>
       <c r="G398" s="13"/>
-      <c r="H398" s="455"/>
+      <c r="H398" s="456"/>
       <c r="I398" s="13"/>
       <c r="J398" s="19" t="s">
         <v>42</v>
@@ -47592,7 +47592,7 @@
       <c r="G399" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H399" s="455"/>
+      <c r="H399" s="456"/>
       <c r="I399" s="13"/>
       <c r="J399" s="19" t="s">
         <v>67</v>
@@ -51434,7 +51434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7487BF92-A04F-4C5C-BC2B-11327DDC945F}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -51453,7 +51453,7 @@
       <c r="E1" t="s">
         <v>524</v>
       </c>
-      <c r="F1" s="458" t="s">
+      <c r="F1" s="444" t="s">
         <v>520</v>
       </c>
       <c r="I1" t="s">
@@ -51482,7 +51482,7 @@
       <c r="E2" t="s">
         <v>524</v>
       </c>
-      <c r="F2" s="458" t="s">
+      <c r="F2" s="444" t="s">
         <v>521</v>
       </c>
       <c r="I2" t="s">
@@ -53631,10 +53631,10 @@
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
-      <c r="F68" s="456" t="s">
+      <c r="F68" s="457" t="s">
         <v>377</v>
       </c>
-      <c r="G68" s="457"/>
+      <c r="G68" s="458"/>
       <c r="H68" s="19"/>
       <c r="I68" s="19" t="s">
         <v>378</v>
@@ -54466,8 +54466,8 @@
       <c r="B96" s="2"/>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="456"/>
-      <c r="F96" s="457"/>
+      <c r="E96" s="457"/>
+      <c r="F96" s="458"/>
       <c r="G96" s="19" t="s">
         <v>385</v>
       </c>

</xml_diff>

<commit_message>
changes to crop, start sheep pyomo, add mort functions sheep
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49D4D11-EB83-4E73-A432-3FE2C1E17D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103EE347-B64F-4D71-8AB0-377DF75A0EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <definedName name="fixed_control" localSheetId="5">Crop!$G$95:$R$119</definedName>
     <definedName name="fixed_fert" localSheetId="5">Crop!$G$95:$J$119</definedName>
     <definedName name="fixed_fert_passes" localSheetId="5">Crop!$L$95:$O$119</definedName>
-    <definedName name="fixed_rotphases">Crop!$G$156:$L$161</definedName>
+    <definedName name="fixed_rotphases">Crop!$G$155:$L$161</definedName>
     <definedName name="FOOatGrazing" localSheetId="4">Annual!$L$120</definedName>
     <definedName name="FOOatSeeding" localSheetId="4">Annual!$J$113</definedName>
     <definedName name="FOODryH" localSheetId="4">Annual!$M$293:$M$302</definedName>
@@ -123,7 +123,7 @@
     <definedName name="number_crop_gear" localSheetId="8">Mach!$B$5</definedName>
     <definedName name="option" localSheetId="8">Mach!$B$3</definedName>
     <definedName name="overdraw_limit" localSheetId="10">Finance!$B$2</definedName>
-    <definedName name="overheads">General!$I$24:$J$33</definedName>
+    <definedName name="overheads">General!$I$49:$J$58</definedName>
     <definedName name="own_seed">Crop!$P$373:$P$390</definedName>
     <definedName name="PastDecay" localSheetId="4">Annual!$J$68</definedName>
     <definedName name="PGRScalarH" localSheetId="4">Annual!$M$212:$M$221</definedName>
@@ -152,6 +152,7 @@
     <definedName name="SA.PGR" localSheetId="4">Annual!#REF!</definedName>
     <definedName name="SA.PGRLMU" localSheetId="4">Annual!#REF!</definedName>
     <definedName name="SA.PGRPer" localSheetId="4">Annual!#REF!</definedName>
+    <definedName name="season_info">General!$I$24:$K$25</definedName>
     <definedName name="seed_info">Crop!$G$405:$Q$423</definedName>
     <definedName name="seed_period_lengths" localSheetId="5">Crop!$I$13:$I$16</definedName>
     <definedName name="seed_prep">Labour!$S$97:$T$100</definedName>
@@ -194,7 +195,7 @@
     <definedName name="yield_penalty" localSheetId="5">Crop!$H$24:$J$36</definedName>
     <definedName name="yields" localSheetId="5">Crop!$M$155:$M$161</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -266,7 +267,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{44D2834B-F5A5-4B3F-8A7A-AF2F7CF0521F}">
+    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{468F4AA6-F6F7-4C76-99C7-3D4020558FE1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+this is probability when all season types are included. This is altered in the code if only a subset of seasons are included
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J49" authorId="0" shapeId="0" xr:uid="{44D2834B-F5A5-4B3F-8A7A-AF2F7CF0521F}">
       <text>
         <r>
           <rPr>
@@ -2995,7 +3021,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="526">
   <si>
     <t>«</t>
   </si>
@@ -4587,6 +4613,24 @@
   <si>
     <t>fert passes</t>
   </si>
+  <si>
+    <t>Season Types</t>
+  </si>
+  <si>
+    <t>season 1</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>Note: add to the table below when the inputs for other seasons exist</t>
+  </si>
+  <si>
+    <t>included</t>
+  </si>
+  <si>
+    <t>Do you wan steady state model?</t>
+  </si>
 </sst>
 </file>
 
@@ -4606,7 +4650,7 @@
     <numFmt numFmtId="174" formatCode="0.000"/>
     <numFmt numFmtId="175" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4787,6 +4831,13 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="21">
@@ -5192,7 +5243,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5222,8 +5273,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="20" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="29" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="469">
+  <cellXfs count="474">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6351,6 +6403,37 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="26" fillId="20" borderId="24" xfId="12" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="24" xfId="12"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="16" borderId="15" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -6388,51 +6471,34 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="26" fillId="20" borderId="24" xfId="12" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="24" xfId="12"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="10" borderId="9" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="7" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="7" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="7" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Calculations" xfId="10" xr:uid="{449B9FA0-BCFF-41FE-A9C5-7F4DFD2D1D3B}"/>
     <cellStyle name="Formula 1" xfId="11" xr:uid="{F8CEB686-1EA8-43D0-A731-F4582AD6DEDB}"/>
     <cellStyle name="IndexSelectBackground" xfId="7" xr:uid="{D65E80AD-CB0E-4369-AB4D-3C50EADF821F}"/>
@@ -6444,6 +6510,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{0C3493F0-E759-4D93-8160-530DBAD973D6}"/>
     <cellStyle name="Normal 3" xfId="5" xr:uid="{0FB42827-6271-4A4D-87D5-7577D9F5FC01}"/>
+    <cellStyle name="Percent" xfId="13" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="2" xr:uid="{FE2D1058-BCB6-47B5-B4CE-77F02A915649}"/>
     <cellStyle name="WorksheetBackground" xfId="6" xr:uid="{F1D7B2CD-A7D3-44D4-9C6E-58E9948FB1C9}"/>
   </cellStyles>
@@ -11444,10 +11511,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AB1FD0-C06F-43E2-AD4D-7EBD7CDF886A}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:Z38"/>
+  <dimension ref="A2:Z63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24:J33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11535,6 +11602,7 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="326"/>
       <c r="B14" s="327"/>
@@ -11631,7 +11699,7 @@
       </c>
       <c r="F17" s="333"/>
       <c r="G17" s="334" t="s">
-        <v>384</v>
+        <v>520</v>
       </c>
       <c r="H17" s="333"/>
       <c r="I17" s="333"/>
@@ -11660,9 +11728,7 @@
       <c r="D18" s="332"/>
       <c r="E18" s="337"/>
       <c r="F18" s="333"/>
-      <c r="G18" s="333" t="s">
-        <v>385</v>
-      </c>
+      <c r="G18" s="333"/>
       <c r="H18" s="333"/>
       <c r="I18" s="333"/>
       <c r="J18" s="333"/>
@@ -11690,14 +11756,12 @@
       <c r="D19" s="332"/>
       <c r="E19" s="337"/>
       <c r="F19" s="333"/>
-      <c r="G19" s="339">
-        <v>38576.728726851848</v>
-      </c>
-      <c r="H19" s="333" t="s">
-        <v>386</v>
-      </c>
+      <c r="G19" s="339"/>
+      <c r="H19" s="333"/>
       <c r="I19" s="333"/>
-      <c r="J19" s="333"/>
+      <c r="J19" s="333" t="s">
+        <v>523</v>
+      </c>
       <c r="K19" s="333"/>
       <c r="L19" s="333"/>
       <c r="M19" s="333"/>
@@ -11814,9 +11878,7 @@
       <c r="J23" s="337"/>
       <c r="K23" s="343"/>
       <c r="L23" s="344"/>
-      <c r="M23" s="344" t="s">
-        <v>388</v>
-      </c>
+      <c r="M23" s="344"/>
       <c r="N23" s="344"/>
       <c r="O23" s="344"/>
       <c r="P23" s="344"/>
@@ -11842,11 +11904,15 @@
       <c r="H24" s="337"/>
       <c r="I24" s="337"/>
       <c r="J24" s="343" t="s">
-        <v>387</v>
-      </c>
-      <c r="K24" s="343"/>
+        <v>522</v>
+      </c>
+      <c r="K24" s="343" t="s">
+        <v>524</v>
+      </c>
       <c r="L24" s="344"/>
-      <c r="M24" s="344"/>
+      <c r="M24" s="469" t="s">
+        <v>525</v>
+      </c>
       <c r="N24" s="344"/>
       <c r="O24" s="344"/>
       <c r="P24" s="344"/>
@@ -11871,15 +11937,17 @@
       <c r="G25" s="99"/>
       <c r="H25" s="349"/>
       <c r="I25" s="363" t="s">
-        <v>390</v>
-      </c>
-      <c r="J25" s="350">
-        <v>1500</v>
-      </c>
-      <c r="K25" s="351"/>
+        <v>521</v>
+      </c>
+      <c r="J25" s="471">
+        <v>1</v>
+      </c>
+      <c r="K25" s="470" t="b">
+        <v>1</v>
+      </c>
       <c r="L25" s="351"/>
-      <c r="M25" s="352">
-        <v>1500</v>
+      <c r="M25" s="470" t="b">
+        <v>1</v>
       </c>
       <c r="N25" s="351"/>
       <c r="O25" s="351"/>
@@ -11904,17 +11972,11 @@
       <c r="F26" s="345"/>
       <c r="G26" s="99"/>
       <c r="H26" s="349"/>
-      <c r="I26" s="363" t="s">
-        <v>391</v>
-      </c>
-      <c r="J26" s="350">
-        <v>15000</v>
-      </c>
+      <c r="I26" s="351"/>
+      <c r="J26" s="472"/>
       <c r="K26" s="351"/>
       <c r="L26" s="351"/>
-      <c r="M26" s="352">
-        <v>5000</v>
-      </c>
+      <c r="M26" s="351"/>
       <c r="N26" s="351"/>
       <c r="O26" s="351"/>
       <c r="P26" s="351"/>
@@ -11938,17 +12000,11 @@
       <c r="F27" s="345"/>
       <c r="G27" s="99"/>
       <c r="H27" s="349"/>
-      <c r="I27" s="363" t="s">
-        <v>392</v>
-      </c>
-      <c r="J27" s="350">
-        <v>2000</v>
-      </c>
+      <c r="I27" s="351"/>
+      <c r="J27" s="472"/>
       <c r="K27" s="351"/>
       <c r="L27" s="351"/>
-      <c r="M27" s="352">
-        <v>2000</v>
-      </c>
+      <c r="M27" s="351"/>
       <c r="N27" s="351"/>
       <c r="O27" s="351"/>
       <c r="P27" s="351"/>
@@ -11972,17 +12028,11 @@
       <c r="F28" s="345"/>
       <c r="G28" s="99"/>
       <c r="H28" s="349"/>
-      <c r="I28" s="363" t="s">
-        <v>393</v>
-      </c>
-      <c r="J28" s="350">
-        <v>5000</v>
-      </c>
+      <c r="I28" s="351"/>
+      <c r="J28" s="472"/>
       <c r="K28" s="351"/>
       <c r="L28" s="351"/>
-      <c r="M28" s="352">
-        <v>3000</v>
-      </c>
+      <c r="M28" s="351"/>
       <c r="N28" s="351"/>
       <c r="O28" s="351"/>
       <c r="P28" s="351"/>
@@ -12006,17 +12056,11 @@
       <c r="F29" s="345"/>
       <c r="G29" s="99"/>
       <c r="H29" s="349"/>
-      <c r="I29" s="363" t="s">
-        <v>394</v>
-      </c>
-      <c r="J29" s="350">
-        <v>50000</v>
-      </c>
+      <c r="I29" s="351"/>
+      <c r="J29" s="472"/>
       <c r="K29" s="351"/>
       <c r="L29" s="351"/>
-      <c r="M29" s="352">
-        <v>20000</v>
-      </c>
+      <c r="M29" s="351"/>
       <c r="N29" s="351"/>
       <c r="O29" s="351"/>
       <c r="P29" s="351"/>
@@ -12040,17 +12084,11 @@
       <c r="F30" s="345"/>
       <c r="G30" s="99"/>
       <c r="H30" s="349"/>
-      <c r="I30" s="363" t="s">
-        <v>395</v>
-      </c>
-      <c r="J30" s="350">
-        <v>1500</v>
-      </c>
+      <c r="I30" s="351"/>
+      <c r="J30" s="472"/>
       <c r="K30" s="351"/>
       <c r="L30" s="351"/>
-      <c r="M30" s="352">
-        <v>1500</v>
-      </c>
+      <c r="M30" s="351"/>
       <c r="N30" s="351"/>
       <c r="O30" s="351"/>
       <c r="P30" s="351"/>
@@ -12074,17 +12112,11 @@
       <c r="F31" s="345"/>
       <c r="G31" s="99"/>
       <c r="H31" s="349"/>
-      <c r="I31" s="363" t="s">
-        <v>396</v>
-      </c>
-      <c r="J31" s="350">
-        <v>10000</v>
-      </c>
+      <c r="I31" s="351"/>
+      <c r="J31" s="472"/>
       <c r="K31" s="351"/>
       <c r="L31" s="351"/>
-      <c r="M31" s="352">
-        <v>5000</v>
-      </c>
+      <c r="M31" s="351"/>
       <c r="N31" s="351"/>
       <c r="O31" s="351"/>
       <c r="P31" s="351"/>
@@ -12108,17 +12140,11 @@
       <c r="F32" s="353"/>
       <c r="G32" s="99"/>
       <c r="H32" s="349"/>
-      <c r="I32" s="363" t="s">
-        <v>397</v>
-      </c>
-      <c r="J32" s="350">
-        <v>7500</v>
-      </c>
+      <c r="I32" s="351"/>
+      <c r="J32" s="472"/>
       <c r="K32" s="351"/>
       <c r="L32" s="351"/>
-      <c r="M32" s="352">
-        <v>3000</v>
-      </c>
+      <c r="M32" s="351"/>
       <c r="N32" s="351"/>
       <c r="O32" s="351"/>
       <c r="P32" s="351"/>
@@ -12142,15 +12168,11 @@
       <c r="F33" s="353"/>
       <c r="G33" s="99"/>
       <c r="H33" s="349"/>
-      <c r="I33" s="363" t="s">
-        <v>334</v>
-      </c>
-      <c r="J33" s="350">
-        <v>6000</v>
-      </c>
+      <c r="I33" s="351"/>
+      <c r="J33" s="472"/>
       <c r="K33" s="351"/>
       <c r="L33" s="351"/>
-      <c r="M33" s="352"/>
+      <c r="M33" s="351"/>
       <c r="N33" s="351"/>
       <c r="O33" s="351"/>
       <c r="P33" s="351"/>
@@ -12175,7 +12197,7 @@
       <c r="G34" s="349"/>
       <c r="H34" s="349"/>
       <c r="I34" s="349"/>
-      <c r="J34" s="355"/>
+      <c r="J34" s="473"/>
       <c r="K34" s="351"/>
       <c r="L34" s="351"/>
       <c r="M34" s="355"/>
@@ -12205,16 +12227,13 @@
       </c>
       <c r="H35" s="349"/>
       <c r="I35" s="349"/>
-      <c r="J35" s="356">
-        <f>SUM(J25:J33)</f>
-        <v>98500</v>
-      </c>
-      <c r="K35" s="351"/>
-      <c r="L35" s="351"/>
-      <c r="M35" s="357">
-        <f>SUM(M25:M32)</f>
-        <v>41000</v>
-      </c>
+      <c r="J35" s="349">
+        <f>SUM(J25:J34)</f>
+        <v>1</v>
+      </c>
+      <c r="K35" s="349"/>
+      <c r="L35" s="349"/>
+      <c r="M35" s="349"/>
       <c r="N35" s="351"/>
       <c r="O35" s="351"/>
       <c r="P35" s="351"/>
@@ -12266,7 +12285,7 @@
       <c r="F37" s="360"/>
       <c r="G37" s="361" t="str">
         <f>G17</f>
-        <v>FINANCE - ANNUAL OVERHEADS</v>
+        <v>Season Types</v>
       </c>
       <c r="H37" s="360"/>
       <c r="I37" s="360"/>
@@ -12318,7 +12337,791 @@
       <c r="Y38" s="328"/>
       <c r="Z38" s="328"/>
     </row>
+    <row r="39" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="326"/>
+      <c r="B39" s="327"/>
+      <c r="C39" s="327"/>
+      <c r="D39" s="327"/>
+      <c r="E39" s="327"/>
+      <c r="F39" s="327"/>
+      <c r="G39" s="327"/>
+      <c r="H39" s="328"/>
+      <c r="I39" s="328"/>
+      <c r="J39" s="328"/>
+      <c r="K39" s="328"/>
+      <c r="L39" s="328"/>
+      <c r="M39" s="328"/>
+      <c r="N39" s="328"/>
+      <c r="O39" s="328"/>
+      <c r="P39" s="328"/>
+      <c r="Q39" s="328"/>
+      <c r="R39" s="328"/>
+      <c r="S39" s="328"/>
+      <c r="T39" s="328"/>
+      <c r="U39" s="328"/>
+      <c r="V39" s="328"/>
+      <c r="W39" s="328"/>
+      <c r="X39" s="327"/>
+      <c r="Y39" s="327"/>
+      <c r="Z39" s="327"/>
+    </row>
+    <row r="40" spans="1:26" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="326"/>
+      <c r="B40" s="327"/>
+      <c r="C40" s="327"/>
+      <c r="D40" s="327"/>
+      <c r="E40" s="327"/>
+      <c r="F40" s="327"/>
+      <c r="G40" s="327"/>
+      <c r="H40" s="328"/>
+      <c r="I40" s="328"/>
+      <c r="J40" s="328"/>
+      <c r="K40" s="328"/>
+      <c r="L40" s="328"/>
+      <c r="M40" s="328"/>
+      <c r="N40" s="328"/>
+      <c r="O40" s="328"/>
+      <c r="P40" s="328"/>
+      <c r="Q40" s="328"/>
+      <c r="R40" s="328"/>
+      <c r="S40" s="328"/>
+      <c r="T40" s="328"/>
+      <c r="U40" s="328"/>
+      <c r="V40" s="328"/>
+      <c r="W40" s="328"/>
+      <c r="X40" s="327"/>
+      <c r="Y40" s="327"/>
+      <c r="Z40" s="327"/>
+    </row>
+    <row r="41" spans="1:26" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="326"/>
+      <c r="B41" s="327"/>
+      <c r="C41" s="329" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="329"/>
+      <c r="E41" s="329"/>
+      <c r="F41" s="329"/>
+      <c r="G41" s="329"/>
+      <c r="H41" s="329"/>
+      <c r="I41" s="329"/>
+      <c r="J41" s="329"/>
+      <c r="K41" s="330"/>
+      <c r="L41" s="330"/>
+      <c r="M41" s="330"/>
+      <c r="N41" s="330"/>
+      <c r="O41" s="330"/>
+      <c r="P41" s="330"/>
+      <c r="Q41" s="330"/>
+      <c r="R41" s="330"/>
+      <c r="S41" s="330"/>
+      <c r="T41" s="330"/>
+      <c r="U41" s="330"/>
+      <c r="V41" s="330"/>
+      <c r="W41" s="331"/>
+      <c r="X41" s="328"/>
+      <c r="Y41" s="328"/>
+      <c r="Z41" s="328"/>
+    </row>
+    <row r="42" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="326"/>
+      <c r="B42" s="327"/>
+      <c r="C42" s="332"/>
+      <c r="D42" s="332"/>
+      <c r="E42" s="332" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="333"/>
+      <c r="G42" s="334" t="s">
+        <v>384</v>
+      </c>
+      <c r="H42" s="333"/>
+      <c r="I42" s="333"/>
+      <c r="J42" s="333"/>
+      <c r="K42" s="333"/>
+      <c r="L42" s="333"/>
+      <c r="M42" s="333"/>
+      <c r="N42" s="333"/>
+      <c r="O42" s="333"/>
+      <c r="P42" s="333"/>
+      <c r="Q42" s="333"/>
+      <c r="R42" s="333"/>
+      <c r="S42" s="335"/>
+      <c r="T42" s="333"/>
+      <c r="U42" s="335"/>
+      <c r="V42" s="335"/>
+      <c r="W42" s="336"/>
+      <c r="X42" s="328"/>
+      <c r="Y42" s="328"/>
+      <c r="Z42" s="328"/>
+    </row>
+    <row r="43" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="326"/>
+      <c r="B43" s="327"/>
+      <c r="C43" s="332"/>
+      <c r="D43" s="332"/>
+      <c r="E43" s="337"/>
+      <c r="F43" s="333"/>
+      <c r="G43" s="333" t="s">
+        <v>385</v>
+      </c>
+      <c r="H43" s="333"/>
+      <c r="I43" s="333"/>
+      <c r="J43" s="333"/>
+      <c r="K43" s="333"/>
+      <c r="L43" s="333"/>
+      <c r="M43" s="333"/>
+      <c r="N43" s="333"/>
+      <c r="O43" s="333"/>
+      <c r="P43" s="333"/>
+      <c r="Q43" s="333"/>
+      <c r="R43" s="333"/>
+      <c r="S43" s="335"/>
+      <c r="T43" s="338"/>
+      <c r="U43" s="335"/>
+      <c r="V43" s="335"/>
+      <c r="W43" s="336"/>
+      <c r="X43" s="328"/>
+      <c r="Y43" s="328"/>
+      <c r="Z43" s="328"/>
+    </row>
+    <row r="44" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="326"/>
+      <c r="B44" s="327"/>
+      <c r="C44" s="337"/>
+      <c r="D44" s="332"/>
+      <c r="E44" s="337"/>
+      <c r="F44" s="333"/>
+      <c r="G44" s="339">
+        <v>38576.728726851848</v>
+      </c>
+      <c r="H44" s="333" t="s">
+        <v>386</v>
+      </c>
+      <c r="I44" s="333"/>
+      <c r="J44" s="333"/>
+      <c r="K44" s="333"/>
+      <c r="L44" s="333"/>
+      <c r="M44" s="333"/>
+      <c r="N44" s="333"/>
+      <c r="O44" s="333"/>
+      <c r="P44" s="333"/>
+      <c r="Q44" s="333"/>
+      <c r="R44" s="333"/>
+      <c r="S44" s="335"/>
+      <c r="T44" s="338"/>
+      <c r="U44" s="335"/>
+      <c r="V44" s="335"/>
+      <c r="W44" s="336"/>
+      <c r="X44" s="328"/>
+      <c r="Y44" s="328"/>
+      <c r="Z44" s="328"/>
+    </row>
+    <row r="45" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="326"/>
+      <c r="B45" s="327"/>
+      <c r="C45" s="340">
+        <v>0</v>
+      </c>
+      <c r="D45" s="332"/>
+      <c r="E45" s="337"/>
+      <c r="F45" s="333"/>
+      <c r="G45" s="341"/>
+      <c r="H45" s="333"/>
+      <c r="I45" s="333"/>
+      <c r="J45" s="333"/>
+      <c r="K45" s="333"/>
+      <c r="L45" s="333"/>
+      <c r="M45" s="333"/>
+      <c r="N45" s="333"/>
+      <c r="O45" s="333"/>
+      <c r="P45" s="333"/>
+      <c r="Q45" s="333"/>
+      <c r="R45" s="333"/>
+      <c r="S45" s="335"/>
+      <c r="T45" s="338"/>
+      <c r="U45" s="335"/>
+      <c r="V45" s="335"/>
+      <c r="W45" s="336"/>
+      <c r="X45" s="328"/>
+      <c r="Y45" s="328"/>
+      <c r="Z45" s="328"/>
+    </row>
+    <row r="46" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="326"/>
+      <c r="B46" s="327"/>
+      <c r="C46" s="337"/>
+      <c r="D46" s="337"/>
+      <c r="E46" s="337"/>
+      <c r="F46" s="337"/>
+      <c r="G46" s="337"/>
+      <c r="H46" s="337"/>
+      <c r="I46" s="337"/>
+      <c r="J46" s="342"/>
+      <c r="K46" s="342"/>
+      <c r="L46" s="342"/>
+      <c r="M46" s="342"/>
+      <c r="N46" s="342"/>
+      <c r="O46" s="342"/>
+      <c r="P46" s="342"/>
+      <c r="Q46" s="342"/>
+      <c r="R46" s="342"/>
+      <c r="S46" s="342"/>
+      <c r="T46" s="342"/>
+      <c r="U46" s="342"/>
+      <c r="V46" s="342"/>
+      <c r="W46" s="336"/>
+      <c r="X46" s="328"/>
+      <c r="Y46" s="328"/>
+      <c r="Z46" s="328"/>
+    </row>
+    <row r="47" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="326"/>
+      <c r="B47" s="327"/>
+      <c r="C47" s="337"/>
+      <c r="D47" s="337"/>
+      <c r="E47" s="337"/>
+      <c r="F47" s="337"/>
+      <c r="G47" s="337"/>
+      <c r="H47" s="337"/>
+      <c r="I47" s="337"/>
+      <c r="J47" s="337"/>
+      <c r="K47" s="337"/>
+      <c r="L47" s="342"/>
+      <c r="M47" s="342"/>
+      <c r="N47" s="342"/>
+      <c r="O47" s="342"/>
+      <c r="P47" s="342"/>
+      <c r="Q47" s="342"/>
+      <c r="R47" s="342"/>
+      <c r="S47" s="342"/>
+      <c r="T47" s="342"/>
+      <c r="U47" s="342"/>
+      <c r="V47" s="342"/>
+      <c r="W47" s="336"/>
+      <c r="X47" s="328"/>
+      <c r="Y47" s="328"/>
+      <c r="Z47" s="328"/>
+    </row>
+    <row r="48" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="326"/>
+      <c r="B48" s="327"/>
+      <c r="C48" s="337"/>
+      <c r="D48" s="337"/>
+      <c r="E48" s="337"/>
+      <c r="F48" s="337"/>
+      <c r="G48" s="337"/>
+      <c r="H48" s="337"/>
+      <c r="I48" s="337"/>
+      <c r="J48" s="337"/>
+      <c r="K48" s="343"/>
+      <c r="L48" s="344"/>
+      <c r="M48" s="344" t="s">
+        <v>388</v>
+      </c>
+      <c r="N48" s="344"/>
+      <c r="O48" s="344"/>
+      <c r="P48" s="344"/>
+      <c r="Q48" s="344"/>
+      <c r="R48" s="344"/>
+      <c r="S48" s="342"/>
+      <c r="T48" s="342"/>
+      <c r="U48" s="342"/>
+      <c r="V48" s="342"/>
+      <c r="W48" s="336"/>
+      <c r="X48" s="328"/>
+      <c r="Y48" s="328"/>
+      <c r="Z48" s="328"/>
+    </row>
+    <row r="49" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="326"/>
+      <c r="B49" s="327"/>
+      <c r="C49" s="337"/>
+      <c r="D49" s="337"/>
+      <c r="E49" s="337"/>
+      <c r="F49" s="337"/>
+      <c r="G49" s="337"/>
+      <c r="H49" s="337"/>
+      <c r="I49" s="337"/>
+      <c r="J49" s="343" t="s">
+        <v>387</v>
+      </c>
+      <c r="K49" s="343"/>
+      <c r="L49" s="344"/>
+      <c r="M49" s="344"/>
+      <c r="N49" s="344"/>
+      <c r="O49" s="344"/>
+      <c r="P49" s="344"/>
+      <c r="Q49" s="344"/>
+      <c r="R49" s="344"/>
+      <c r="S49" s="342"/>
+      <c r="T49" s="342"/>
+      <c r="U49" s="342"/>
+      <c r="V49" s="342"/>
+      <c r="W49" s="336"/>
+      <c r="X49" s="328"/>
+      <c r="Y49" s="328"/>
+      <c r="Z49" s="328"/>
+    </row>
+    <row r="50" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="326"/>
+      <c r="B50" s="327"/>
+      <c r="C50" s="337"/>
+      <c r="D50" s="337"/>
+      <c r="E50" s="337"/>
+      <c r="F50" s="345"/>
+      <c r="G50" s="99"/>
+      <c r="H50" s="349"/>
+      <c r="I50" s="363" t="s">
+        <v>390</v>
+      </c>
+      <c r="J50" s="350">
+        <v>1500</v>
+      </c>
+      <c r="K50" s="351"/>
+      <c r="L50" s="351"/>
+      <c r="M50" s="352">
+        <v>1500</v>
+      </c>
+      <c r="N50" s="351"/>
+      <c r="O50" s="351"/>
+      <c r="P50" s="351"/>
+      <c r="Q50" s="351"/>
+      <c r="R50" s="351"/>
+      <c r="S50" s="351"/>
+      <c r="T50" s="351"/>
+      <c r="U50" s="351"/>
+      <c r="V50" s="348"/>
+      <c r="W50" s="336"/>
+      <c r="X50" s="328"/>
+      <c r="Y50" s="328"/>
+      <c r="Z50" s="328"/>
+    </row>
+    <row r="51" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="326"/>
+      <c r="B51" s="327"/>
+      <c r="C51" s="337"/>
+      <c r="D51" s="337"/>
+      <c r="E51" s="337"/>
+      <c r="F51" s="345"/>
+      <c r="G51" s="99"/>
+      <c r="H51" s="349"/>
+      <c r="I51" s="363" t="s">
+        <v>391</v>
+      </c>
+      <c r="J51" s="350">
+        <v>15000</v>
+      </c>
+      <c r="K51" s="351"/>
+      <c r="L51" s="351"/>
+      <c r="M51" s="352">
+        <v>5000</v>
+      </c>
+      <c r="N51" s="351"/>
+      <c r="O51" s="351"/>
+      <c r="P51" s="351"/>
+      <c r="Q51" s="351"/>
+      <c r="R51" s="351"/>
+      <c r="S51" s="351"/>
+      <c r="T51" s="351"/>
+      <c r="U51" s="351"/>
+      <c r="V51" s="348"/>
+      <c r="W51" s="336"/>
+      <c r="X51" s="328"/>
+      <c r="Y51" s="328"/>
+      <c r="Z51" s="328"/>
+    </row>
+    <row r="52" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="326"/>
+      <c r="B52" s="327"/>
+      <c r="C52" s="337"/>
+      <c r="D52" s="337"/>
+      <c r="E52" s="337"/>
+      <c r="F52" s="345"/>
+      <c r="G52" s="99"/>
+      <c r="H52" s="349"/>
+      <c r="I52" s="363" t="s">
+        <v>392</v>
+      </c>
+      <c r="J52" s="350">
+        <v>2000</v>
+      </c>
+      <c r="K52" s="351"/>
+      <c r="L52" s="351"/>
+      <c r="M52" s="352">
+        <v>2000</v>
+      </c>
+      <c r="N52" s="351"/>
+      <c r="O52" s="351"/>
+      <c r="P52" s="351"/>
+      <c r="Q52" s="351"/>
+      <c r="R52" s="351"/>
+      <c r="S52" s="351"/>
+      <c r="T52" s="351"/>
+      <c r="U52" s="351"/>
+      <c r="V52" s="348"/>
+      <c r="W52" s="336"/>
+      <c r="X52" s="328"/>
+      <c r="Y52" s="328"/>
+      <c r="Z52" s="328"/>
+    </row>
+    <row r="53" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="326"/>
+      <c r="B53" s="327"/>
+      <c r="C53" s="337"/>
+      <c r="D53" s="337"/>
+      <c r="E53" s="337"/>
+      <c r="F53" s="345"/>
+      <c r="G53" s="99"/>
+      <c r="H53" s="349"/>
+      <c r="I53" s="363" t="s">
+        <v>393</v>
+      </c>
+      <c r="J53" s="350">
+        <v>5000</v>
+      </c>
+      <c r="K53" s="351"/>
+      <c r="L53" s="351"/>
+      <c r="M53" s="352">
+        <v>3000</v>
+      </c>
+      <c r="N53" s="351"/>
+      <c r="O53" s="351"/>
+      <c r="P53" s="351"/>
+      <c r="Q53" s="351"/>
+      <c r="R53" s="351"/>
+      <c r="S53" s="351"/>
+      <c r="T53" s="351"/>
+      <c r="U53" s="351"/>
+      <c r="V53" s="348"/>
+      <c r="W53" s="336"/>
+      <c r="X53" s="328"/>
+      <c r="Y53" s="328"/>
+      <c r="Z53" s="328"/>
+    </row>
+    <row r="54" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="326"/>
+      <c r="B54" s="327"/>
+      <c r="C54" s="337"/>
+      <c r="D54" s="337"/>
+      <c r="E54" s="337"/>
+      <c r="F54" s="345"/>
+      <c r="G54" s="99"/>
+      <c r="H54" s="349"/>
+      <c r="I54" s="363" t="s">
+        <v>394</v>
+      </c>
+      <c r="J54" s="350">
+        <v>50000</v>
+      </c>
+      <c r="K54" s="351"/>
+      <c r="L54" s="351"/>
+      <c r="M54" s="352">
+        <v>20000</v>
+      </c>
+      <c r="N54" s="351"/>
+      <c r="O54" s="351"/>
+      <c r="P54" s="351"/>
+      <c r="Q54" s="351"/>
+      <c r="R54" s="351"/>
+      <c r="S54" s="351"/>
+      <c r="T54" s="351"/>
+      <c r="U54" s="351"/>
+      <c r="V54" s="348"/>
+      <c r="W54" s="336"/>
+      <c r="X54" s="328"/>
+      <c r="Y54" s="328"/>
+      <c r="Z54" s="328"/>
+    </row>
+    <row r="55" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="326"/>
+      <c r="B55" s="327"/>
+      <c r="C55" s="337"/>
+      <c r="D55" s="337"/>
+      <c r="E55" s="337"/>
+      <c r="F55" s="345"/>
+      <c r="G55" s="99"/>
+      <c r="H55" s="349"/>
+      <c r="I55" s="363" t="s">
+        <v>395</v>
+      </c>
+      <c r="J55" s="350">
+        <v>1500</v>
+      </c>
+      <c r="K55" s="351"/>
+      <c r="L55" s="351"/>
+      <c r="M55" s="352">
+        <v>1500</v>
+      </c>
+      <c r="N55" s="351"/>
+      <c r="O55" s="351"/>
+      <c r="P55" s="351"/>
+      <c r="Q55" s="351"/>
+      <c r="R55" s="351"/>
+      <c r="S55" s="351"/>
+      <c r="T55" s="351"/>
+      <c r="U55" s="351"/>
+      <c r="V55" s="348"/>
+      <c r="W55" s="336"/>
+      <c r="X55" s="328"/>
+      <c r="Y55" s="328"/>
+      <c r="Z55" s="328"/>
+    </row>
+    <row r="56" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="326"/>
+      <c r="B56" s="327"/>
+      <c r="C56" s="337"/>
+      <c r="D56" s="337"/>
+      <c r="E56" s="337"/>
+      <c r="F56" s="345"/>
+      <c r="G56" s="99"/>
+      <c r="H56" s="349"/>
+      <c r="I56" s="363" t="s">
+        <v>396</v>
+      </c>
+      <c r="J56" s="350">
+        <v>10000</v>
+      </c>
+      <c r="K56" s="351"/>
+      <c r="L56" s="351"/>
+      <c r="M56" s="352">
+        <v>5000</v>
+      </c>
+      <c r="N56" s="351"/>
+      <c r="O56" s="351"/>
+      <c r="P56" s="351"/>
+      <c r="Q56" s="351"/>
+      <c r="R56" s="351"/>
+      <c r="S56" s="351"/>
+      <c r="T56" s="351"/>
+      <c r="U56" s="351"/>
+      <c r="V56" s="348"/>
+      <c r="W56" s="336"/>
+      <c r="X56" s="328"/>
+      <c r="Y56" s="328"/>
+      <c r="Z56" s="328"/>
+    </row>
+    <row r="57" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="326"/>
+      <c r="B57" s="327"/>
+      <c r="C57" s="337"/>
+      <c r="D57" s="337"/>
+      <c r="E57" s="337"/>
+      <c r="F57" s="353"/>
+      <c r="G57" s="99"/>
+      <c r="H57" s="349"/>
+      <c r="I57" s="363" t="s">
+        <v>397</v>
+      </c>
+      <c r="J57" s="350">
+        <v>7500</v>
+      </c>
+      <c r="K57" s="351"/>
+      <c r="L57" s="351"/>
+      <c r="M57" s="352">
+        <v>3000</v>
+      </c>
+      <c r="N57" s="351"/>
+      <c r="O57" s="351"/>
+      <c r="P57" s="351"/>
+      <c r="Q57" s="351"/>
+      <c r="R57" s="351"/>
+      <c r="S57" s="351"/>
+      <c r="T57" s="351"/>
+      <c r="U57" s="351"/>
+      <c r="V57" s="348"/>
+      <c r="W57" s="336"/>
+      <c r="X57" s="328"/>
+      <c r="Y57" s="328"/>
+      <c r="Z57" s="328"/>
+    </row>
+    <row r="58" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="326"/>
+      <c r="B58" s="327"/>
+      <c r="C58" s="337"/>
+      <c r="D58" s="337"/>
+      <c r="E58" s="337"/>
+      <c r="F58" s="353"/>
+      <c r="G58" s="99"/>
+      <c r="H58" s="349"/>
+      <c r="I58" s="363" t="s">
+        <v>334</v>
+      </c>
+      <c r="J58" s="350">
+        <v>6000</v>
+      </c>
+      <c r="K58" s="351"/>
+      <c r="L58" s="351"/>
+      <c r="M58" s="352"/>
+      <c r="N58" s="351"/>
+      <c r="O58" s="351"/>
+      <c r="P58" s="351"/>
+      <c r="Q58" s="351"/>
+      <c r="R58" s="351"/>
+      <c r="S58" s="351"/>
+      <c r="T58" s="351"/>
+      <c r="U58" s="351"/>
+      <c r="V58" s="348"/>
+      <c r="W58" s="336"/>
+      <c r="X58" s="328"/>
+      <c r="Y58" s="328"/>
+      <c r="Z58" s="328"/>
+    </row>
+    <row r="59" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="326"/>
+      <c r="B59" s="327"/>
+      <c r="C59" s="337"/>
+      <c r="D59" s="337"/>
+      <c r="E59" s="337"/>
+      <c r="F59" s="354"/>
+      <c r="G59" s="349"/>
+      <c r="H59" s="349"/>
+      <c r="I59" s="349"/>
+      <c r="J59" s="355"/>
+      <c r="K59" s="351"/>
+      <c r="L59" s="351"/>
+      <c r="M59" s="355"/>
+      <c r="N59" s="351"/>
+      <c r="O59" s="351"/>
+      <c r="P59" s="351"/>
+      <c r="Q59" s="351"/>
+      <c r="R59" s="351"/>
+      <c r="S59" s="351"/>
+      <c r="T59" s="351"/>
+      <c r="U59" s="351"/>
+      <c r="V59" s="348"/>
+      <c r="W59" s="336"/>
+      <c r="X59" s="328"/>
+      <c r="Y59" s="328"/>
+      <c r="Z59" s="328"/>
+    </row>
+    <row r="60" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="326"/>
+      <c r="B60" s="327"/>
+      <c r="C60" s="337"/>
+      <c r="D60" s="337"/>
+      <c r="E60" s="337"/>
+      <c r="F60" s="354"/>
+      <c r="G60" s="349" t="s">
+        <v>398</v>
+      </c>
+      <c r="H60" s="349"/>
+      <c r="I60" s="349"/>
+      <c r="J60" s="356">
+        <f>SUM(J50:J58)</f>
+        <v>98500</v>
+      </c>
+      <c r="K60" s="351"/>
+      <c r="L60" s="351"/>
+      <c r="M60" s="357">
+        <f>SUM(M50:M57)</f>
+        <v>41000</v>
+      </c>
+      <c r="N60" s="351"/>
+      <c r="O60" s="351"/>
+      <c r="P60" s="351"/>
+      <c r="Q60" s="351"/>
+      <c r="R60" s="351"/>
+      <c r="S60" s="351"/>
+      <c r="T60" s="351"/>
+      <c r="U60" s="351"/>
+      <c r="V60" s="348"/>
+      <c r="W60" s="336"/>
+      <c r="X60" s="328"/>
+      <c r="Y60" s="328"/>
+      <c r="Z60" s="328"/>
+    </row>
+    <row r="61" spans="1:26" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="326"/>
+      <c r="B61" s="327"/>
+      <c r="C61" s="337"/>
+      <c r="D61" s="337"/>
+      <c r="E61" s="337"/>
+      <c r="F61" s="353"/>
+      <c r="G61" s="358"/>
+      <c r="H61" s="358"/>
+      <c r="I61" s="358"/>
+      <c r="J61" s="359"/>
+      <c r="K61" s="359"/>
+      <c r="L61" s="359"/>
+      <c r="M61" s="359"/>
+      <c r="N61" s="359"/>
+      <c r="O61" s="359"/>
+      <c r="P61" s="359"/>
+      <c r="Q61" s="359"/>
+      <c r="R61" s="359"/>
+      <c r="S61" s="359"/>
+      <c r="T61" s="359"/>
+      <c r="U61" s="359"/>
+      <c r="V61" s="348"/>
+      <c r="W61" s="336"/>
+      <c r="X61" s="328"/>
+      <c r="Y61" s="328"/>
+      <c r="Z61" s="328"/>
+    </row>
+    <row r="62" spans="1:26" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="326"/>
+      <c r="B62" s="327"/>
+      <c r="C62" s="360"/>
+      <c r="D62" s="360"/>
+      <c r="E62" s="360"/>
+      <c r="F62" s="360"/>
+      <c r="G62" s="361" t="str">
+        <f>G42</f>
+        <v>FINANCE - ANNUAL OVERHEADS</v>
+      </c>
+      <c r="H62" s="360"/>
+      <c r="I62" s="360"/>
+      <c r="J62" s="360"/>
+      <c r="K62" s="360"/>
+      <c r="L62" s="360"/>
+      <c r="M62" s="360"/>
+      <c r="N62" s="360"/>
+      <c r="O62" s="360"/>
+      <c r="P62" s="360"/>
+      <c r="Q62" s="360"/>
+      <c r="R62" s="360"/>
+      <c r="S62" s="360"/>
+      <c r="T62" s="360"/>
+      <c r="U62" s="360"/>
+      <c r="V62" s="360"/>
+      <c r="W62" s="362" t="s">
+        <v>24</v>
+      </c>
+      <c r="X62" s="328"/>
+      <c r="Y62" s="328"/>
+      <c r="Z62" s="328"/>
+    </row>
+    <row r="63" spans="1:26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="326"/>
+      <c r="B63" s="327"/>
+      <c r="C63" s="327"/>
+      <c r="D63" s="327"/>
+      <c r="E63" s="327"/>
+      <c r="F63" s="328"/>
+      <c r="G63" s="328"/>
+      <c r="H63" s="328"/>
+      <c r="I63" s="328"/>
+      <c r="J63" s="328"/>
+      <c r="K63" s="328"/>
+      <c r="L63" s="328"/>
+      <c r="M63" s="328"/>
+      <c r="N63" s="328"/>
+      <c r="O63" s="328"/>
+      <c r="P63" s="328"/>
+      <c r="Q63" s="328"/>
+      <c r="R63" s="328"/>
+      <c r="S63" s="328"/>
+      <c r="T63" s="328"/>
+      <c r="U63" s="328"/>
+      <c r="V63" s="328"/>
+      <c r="W63" s="328"/>
+      <c r="X63" s="328"/>
+      <c r="Y63" s="328"/>
+      <c r="Z63" s="328"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -16083,21 +16886,21 @@
       <c r="E46" s="139"/>
       <c r="F46" s="141"/>
       <c r="G46" s="150"/>
-      <c r="H46" s="442" t="s">
+      <c r="H46" s="453" t="s">
         <v>163</v>
       </c>
-      <c r="I46" s="443"/>
-      <c r="J46" s="443"/>
-      <c r="K46" s="443"/>
-      <c r="L46" s="443"/>
-      <c r="M46" s="443"/>
-      <c r="N46" s="443"/>
-      <c r="O46" s="443"/>
-      <c r="P46" s="443"/>
-      <c r="Q46" s="443"/>
-      <c r="R46" s="443"/>
-      <c r="S46" s="443"/>
-      <c r="T46" s="444"/>
+      <c r="I46" s="454"/>
+      <c r="J46" s="454"/>
+      <c r="K46" s="454"/>
+      <c r="L46" s="454"/>
+      <c r="M46" s="454"/>
+      <c r="N46" s="454"/>
+      <c r="O46" s="454"/>
+      <c r="P46" s="454"/>
+      <c r="Q46" s="454"/>
+      <c r="R46" s="454"/>
+      <c r="S46" s="454"/>
+      <c r="T46" s="455"/>
       <c r="U46" s="150"/>
       <c r="V46" s="141"/>
       <c r="W46" s="121"/>
@@ -16111,19 +16914,19 @@
       <c r="E47" s="139"/>
       <c r="F47" s="141"/>
       <c r="G47" s="150"/>
-      <c r="H47" s="445"/>
-      <c r="I47" s="446"/>
-      <c r="J47" s="446"/>
-      <c r="K47" s="446"/>
-      <c r="L47" s="446"/>
-      <c r="M47" s="446"/>
-      <c r="N47" s="446"/>
-      <c r="O47" s="446"/>
-      <c r="P47" s="446"/>
-      <c r="Q47" s="446"/>
-      <c r="R47" s="446"/>
-      <c r="S47" s="446"/>
-      <c r="T47" s="447"/>
+      <c r="H47" s="456"/>
+      <c r="I47" s="457"/>
+      <c r="J47" s="457"/>
+      <c r="K47" s="457"/>
+      <c r="L47" s="457"/>
+      <c r="M47" s="457"/>
+      <c r="N47" s="457"/>
+      <c r="O47" s="457"/>
+      <c r="P47" s="457"/>
+      <c r="Q47" s="457"/>
+      <c r="R47" s="457"/>
+      <c r="S47" s="457"/>
+      <c r="T47" s="458"/>
       <c r="U47" s="150"/>
       <c r="V47" s="141"/>
       <c r="W47" s="121"/>
@@ -16137,19 +16940,19 @@
       <c r="E48" s="139"/>
       <c r="F48" s="141"/>
       <c r="G48" s="150"/>
-      <c r="H48" s="445"/>
-      <c r="I48" s="446"/>
-      <c r="J48" s="446"/>
-      <c r="K48" s="446"/>
-      <c r="L48" s="446"/>
-      <c r="M48" s="446"/>
-      <c r="N48" s="446"/>
-      <c r="O48" s="446"/>
-      <c r="P48" s="446"/>
-      <c r="Q48" s="446"/>
-      <c r="R48" s="446"/>
-      <c r="S48" s="446"/>
-      <c r="T48" s="447"/>
+      <c r="H48" s="456"/>
+      <c r="I48" s="457"/>
+      <c r="J48" s="457"/>
+      <c r="K48" s="457"/>
+      <c r="L48" s="457"/>
+      <c r="M48" s="457"/>
+      <c r="N48" s="457"/>
+      <c r="O48" s="457"/>
+      <c r="P48" s="457"/>
+      <c r="Q48" s="457"/>
+      <c r="R48" s="457"/>
+      <c r="S48" s="457"/>
+      <c r="T48" s="458"/>
       <c r="U48" s="150"/>
       <c r="V48" s="141"/>
       <c r="W48" s="121"/>
@@ -16163,19 +16966,19 @@
       <c r="E49" s="139"/>
       <c r="F49" s="141"/>
       <c r="G49" s="150"/>
-      <c r="H49" s="448"/>
-      <c r="I49" s="449"/>
-      <c r="J49" s="449"/>
-      <c r="K49" s="449"/>
-      <c r="L49" s="449"/>
-      <c r="M49" s="449"/>
-      <c r="N49" s="449"/>
-      <c r="O49" s="449"/>
-      <c r="P49" s="449"/>
-      <c r="Q49" s="449"/>
-      <c r="R49" s="449"/>
-      <c r="S49" s="449"/>
-      <c r="T49" s="450"/>
+      <c r="H49" s="459"/>
+      <c r="I49" s="460"/>
+      <c r="J49" s="460"/>
+      <c r="K49" s="460"/>
+      <c r="L49" s="460"/>
+      <c r="M49" s="460"/>
+      <c r="N49" s="460"/>
+      <c r="O49" s="460"/>
+      <c r="P49" s="460"/>
+      <c r="Q49" s="460"/>
+      <c r="R49" s="460"/>
+      <c r="S49" s="460"/>
+      <c r="T49" s="461"/>
       <c r="U49" s="150"/>
       <c r="V49" s="141"/>
       <c r="W49" s="121"/>
@@ -30752,9 +31555,9 @@
       <c r="I318" s="251"/>
       <c r="J318" s="251"/>
       <c r="K318" s="138"/>
-      <c r="L318" s="451"/>
-      <c r="M318" s="452"/>
-      <c r="N318" s="452"/>
+      <c r="L318" s="462"/>
+      <c r="M318" s="463"/>
+      <c r="N318" s="463"/>
       <c r="O318" s="138"/>
       <c r="P318" s="138"/>
       <c r="Q318" s="138"/>
@@ -36306,8 +37109,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AU479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H182" sqref="H182"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G156" sqref="G156:L161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="12" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -39180,18 +39983,18 @@
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
-      <c r="H93" s="467" t="s">
+      <c r="H93" s="466" t="s">
         <v>518</v>
       </c>
-      <c r="I93" s="467"/>
-      <c r="J93" s="467"/>
+      <c r="I93" s="466"/>
+      <c r="J93" s="466"/>
       <c r="K93" s="420"/>
       <c r="L93" s="441"/>
-      <c r="M93" s="462" t="s">
+      <c r="M93" s="465" t="s">
         <v>380</v>
       </c>
-      <c r="N93" s="462"/>
-      <c r="O93" s="462"/>
+      <c r="N93" s="465"/>
+      <c r="O93" s="465"/>
       <c r="P93" s="441"/>
       <c r="Q93" s="441"/>
       <c r="R93" s="441"/>
@@ -39255,8 +40058,8 @@
       <c r="J95" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="K95" s="463"/>
-      <c r="L95" s="463"/>
+      <c r="K95" s="448"/>
+      <c r="L95" s="448"/>
       <c r="M95" s="20" t="s">
         <v>475</v>
       </c>
@@ -39298,10 +40101,10 @@
         <v>0</v>
       </c>
       <c r="L96" s="4" t="str">
-        <f>G96</f>
+        <f t="shared" ref="L96:L119" si="0">G96</f>
         <v>b</v>
       </c>
-      <c r="M96" s="468">
+      <c r="M96" s="452">
         <f>1/4</f>
         <v>0.25</v>
       </c>
@@ -39342,19 +40145,19 @@
         <v>0</v>
       </c>
       <c r="L97" s="4" t="str">
-        <f>G97</f>
+        <f t="shared" si="0"/>
         <v>f</v>
       </c>
-      <c r="M97" s="468">
-        <f t="shared" ref="M97:M119" si="0">1/4</f>
+      <c r="M97" s="452">
+        <f t="shared" ref="M97:M119" si="1">1/4</f>
         <v>0.25</v>
       </c>
       <c r="N97" s="422">
-        <f t="shared" ref="N97:O119" si="1">IF(I97&gt;0,1,0)</f>
+        <f t="shared" ref="N97:O119" si="2">IF(I97&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="O97" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S97" s="32"/>
@@ -39386,19 +40189,19 @@
         <v>0</v>
       </c>
       <c r="L98" s="4" t="str">
-        <f>G98</f>
+        <f t="shared" si="0"/>
         <v>h</v>
       </c>
-      <c r="M98" s="468">
-        <f t="shared" si="0"/>
+      <c r="M98" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N98" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O98" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S98" s="32"/>
@@ -39430,19 +40233,19 @@
         <v>0</v>
       </c>
       <c r="L99" s="4" t="str">
-        <f>G99</f>
+        <f t="shared" si="0"/>
         <v>i</v>
       </c>
-      <c r="M99" s="468">
-        <f t="shared" si="0"/>
+      <c r="M99" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N99" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O99" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S99" s="32"/>
@@ -39474,19 +40277,19 @@
         <v>0</v>
       </c>
       <c r="L100" s="4" t="str">
-        <f>G100</f>
+        <f t="shared" si="0"/>
         <v>k</v>
       </c>
-      <c r="M100" s="468">
-        <f t="shared" si="0"/>
+      <c r="M100" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N100" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O100" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S100" s="32"/>
@@ -39518,19 +40321,19 @@
         <v>0</v>
       </c>
       <c r="L101" s="4" t="str">
-        <f>G101</f>
+        <f t="shared" si="0"/>
         <v>l</v>
       </c>
-      <c r="M101" s="468">
-        <f t="shared" si="0"/>
+      <c r="M101" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N101" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O101" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S101" s="32"/>
@@ -39562,19 +40365,19 @@
         <v>0</v>
       </c>
       <c r="L102" s="4" t="str">
-        <f>G102</f>
+        <f t="shared" si="0"/>
         <v>o</v>
       </c>
-      <c r="M102" s="468">
-        <f t="shared" si="0"/>
+      <c r="M102" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N102" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O102" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S102" s="32"/>
@@ -39606,19 +40409,19 @@
         <v>0</v>
       </c>
       <c r="L103" s="4" t="str">
-        <f>G103</f>
+        <f t="shared" si="0"/>
         <v>of</v>
       </c>
-      <c r="M103" s="468">
-        <f t="shared" si="0"/>
+      <c r="M103" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N103" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O103" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S103" s="32"/>
@@ -39650,19 +40453,19 @@
         <v>0</v>
       </c>
       <c r="L104" s="4" t="str">
-        <f>G104</f>
+        <f t="shared" si="0"/>
         <v>r</v>
       </c>
-      <c r="M104" s="468">
-        <f t="shared" si="0"/>
+      <c r="M104" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N104" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O104" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S104" s="32"/>
@@ -39694,19 +40497,19 @@
         <v>0</v>
       </c>
       <c r="L105" s="4" t="str">
-        <f>G105</f>
+        <f t="shared" si="0"/>
         <v>v</v>
       </c>
-      <c r="M105" s="468">
-        <f t="shared" si="0"/>
+      <c r="M105" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N105" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O105" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S105" s="32"/>
@@ -39738,19 +40541,19 @@
         <v>0</v>
       </c>
       <c r="L106" s="4" t="str">
-        <f>G106</f>
+        <f t="shared" si="0"/>
         <v>w</v>
       </c>
-      <c r="M106" s="468">
-        <f t="shared" si="0"/>
+      <c r="M106" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N106" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O106" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S106" s="32"/>
@@ -39782,19 +40585,19 @@
         <v>0</v>
       </c>
       <c r="L107" s="4" t="str">
-        <f>G107</f>
+        <f t="shared" si="0"/>
         <v>z</v>
       </c>
-      <c r="M107" s="468">
-        <f t="shared" si="0"/>
+      <c r="M107" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N107" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O107" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S107" s="32"/>
@@ -39827,19 +40630,19 @@
       </c>
       <c r="K108" s="23"/>
       <c r="L108" s="4" t="str">
-        <f>G108</f>
+        <f t="shared" si="0"/>
         <v>ar</v>
       </c>
-      <c r="M108" s="468">
-        <f t="shared" si="0"/>
+      <c r="M108" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N108" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O108" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S108" s="32"/>
@@ -39872,19 +40675,19 @@
       </c>
       <c r="K109" s="23"/>
       <c r="L109" s="4" t="str">
-        <f>G109</f>
+        <f t="shared" si="0"/>
         <v>m</v>
       </c>
-      <c r="M109" s="468">
-        <f t="shared" si="0"/>
+      <c r="M109" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N109" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O109" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S109" s="32"/>
@@ -39916,19 +40719,19 @@
         <v>12</v>
       </c>
       <c r="L110" s="4" t="str">
-        <f>G110</f>
+        <f t="shared" si="0"/>
         <v>j</v>
       </c>
-      <c r="M110" s="468">
-        <f t="shared" si="0"/>
+      <c r="M110" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N110" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O110" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S110" s="32"/>
@@ -39960,19 +40763,19 @@
         <v>17</v>
       </c>
       <c r="L111" s="4" t="str">
-        <f>G111</f>
+        <f t="shared" si="0"/>
         <v>jr</v>
       </c>
-      <c r="M111" s="468">
-        <f t="shared" si="0"/>
+      <c r="M111" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N111" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O111" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S111" s="32"/>
@@ -40005,19 +40808,19 @@
       </c>
       <c r="K112" s="23"/>
       <c r="L112" s="4" t="str">
-        <f>G112</f>
+        <f t="shared" si="0"/>
         <v>s</v>
       </c>
-      <c r="M112" s="468">
-        <f t="shared" si="0"/>
+      <c r="M112" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N112" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O112" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S112" s="32"/>
@@ -40050,19 +40853,19 @@
       </c>
       <c r="K113" s="23"/>
       <c r="L113" s="4" t="str">
-        <f>G113</f>
+        <f t="shared" si="0"/>
         <v>sr</v>
       </c>
-      <c r="M113" s="468">
-        <f t="shared" si="0"/>
+      <c r="M113" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N113" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O113" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S113" s="32"/>
@@ -40095,19 +40898,19 @@
       </c>
       <c r="K114" s="23"/>
       <c r="L114" s="4" t="str">
-        <f>G114</f>
+        <f t="shared" si="0"/>
         <v>t</v>
       </c>
-      <c r="M114" s="468">
-        <f t="shared" si="0"/>
+      <c r="M114" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N114" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O114" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S114" s="32"/>
@@ -40140,19 +40943,19 @@
       </c>
       <c r="K115" s="23"/>
       <c r="L115" s="4" t="str">
-        <f>G115</f>
+        <f t="shared" si="0"/>
         <v>tr</v>
       </c>
-      <c r="M115" s="468">
-        <f t="shared" si="0"/>
+      <c r="M115" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N115" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O115" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S115" s="32"/>
@@ -40185,19 +40988,19 @@
       </c>
       <c r="K116" s="23"/>
       <c r="L116" s="4" t="str">
-        <f>G116</f>
+        <f t="shared" si="0"/>
         <v>u</v>
       </c>
-      <c r="M116" s="468">
-        <f t="shared" si="0"/>
+      <c r="M116" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N116" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O116" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S116" s="32"/>
@@ -40230,19 +41033,19 @@
       </c>
       <c r="K117" s="22"/>
       <c r="L117" s="4" t="str">
-        <f>G117</f>
+        <f t="shared" si="0"/>
         <v>ur</v>
       </c>
-      <c r="M117" s="468">
-        <f t="shared" si="0"/>
+      <c r="M117" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N117" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O117" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S117" s="32"/>
@@ -40275,19 +41078,19 @@
       </c>
       <c r="K118" s="22"/>
       <c r="L118" s="4" t="str">
-        <f>G118</f>
+        <f t="shared" si="0"/>
         <v>x</v>
       </c>
-      <c r="M118" s="468">
-        <f t="shared" si="0"/>
+      <c r="M118" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N118" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O118" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S118" s="32"/>
@@ -40319,19 +41122,19 @@
         <v>17</v>
       </c>
       <c r="L119" s="4" t="str">
-        <f>G119</f>
+        <f t="shared" si="0"/>
         <v>xr</v>
       </c>
-      <c r="M119" s="468">
-        <f t="shared" si="0"/>
+      <c r="M119" s="452">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="N119" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O119" s="422">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S119" s="32"/>
@@ -41287,10 +42090,10 @@
       <c r="F149" s="9"/>
       <c r="G149" s="14"/>
       <c r="H149" s="9"/>
-      <c r="I149" s="457" t="s">
+      <c r="I149" s="443" t="s">
         <v>491</v>
       </c>
-      <c r="J149" s="456" t="b">
+      <c r="J149" s="442" t="b">
         <v>0</v>
       </c>
       <c r="K149" s="9"/>
@@ -41397,7 +42200,7 @@
       <c r="K152" s="441"/>
       <c r="L152" s="441"/>
       <c r="M152" s="441"/>
-      <c r="N152" s="458" t="s">
+      <c r="N152" s="444" t="s">
         <v>506</v>
       </c>
       <c r="O152" s="441"/>
@@ -41478,13 +42281,13 @@
       <c r="P154" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="Q154" s="461" t="s">
+      <c r="Q154" s="447" t="s">
         <v>501</v>
       </c>
-      <c r="R154" s="461" t="s">
+      <c r="R154" s="447" t="s">
         <v>501</v>
       </c>
-      <c r="S154" s="461" t="s">
+      <c r="S154" s="447" t="s">
         <v>501</v>
       </c>
       <c r="T154" s="441" t="s">
@@ -41598,12 +42401,12 @@
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
       <c r="F156" s="22"/>
-      <c r="G156" s="459"/>
-      <c r="H156" s="459"/>
-      <c r="I156" s="459"/>
-      <c r="J156" s="459"/>
-      <c r="K156" s="459"/>
-      <c r="L156" s="460" t="s">
+      <c r="G156" s="445"/>
+      <c r="H156" s="445"/>
+      <c r="I156" s="445"/>
+      <c r="J156" s="445"/>
+      <c r="K156" s="445"/>
+      <c r="L156" s="446" t="s">
         <v>92</v>
       </c>
       <c r="M156" s="422">
@@ -41644,15 +42447,15 @@
         <v>1</v>
       </c>
       <c r="Y156" s="422">
-        <f t="shared" ref="Y156:AA156" si="2">IF(U156&gt;0,1,0)</f>
+        <f t="shared" ref="Y156:AA156" si="3">IF(U156&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="Z156" s="422">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA156" s="422">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB156" s="12"/>
@@ -41667,12 +42470,12 @@
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
       <c r="F157" s="22"/>
-      <c r="G157" s="459"/>
-      <c r="H157" s="459"/>
-      <c r="I157" s="459"/>
-      <c r="J157" s="459"/>
-      <c r="K157" s="459"/>
-      <c r="L157" s="460" t="s">
+      <c r="G157" s="445"/>
+      <c r="H157" s="445"/>
+      <c r="I157" s="445"/>
+      <c r="J157" s="445"/>
+      <c r="K157" s="445"/>
+      <c r="L157" s="446" t="s">
         <v>91</v>
       </c>
       <c r="M157" s="422">
@@ -41709,19 +42512,19 @@
         <v>0</v>
       </c>
       <c r="X157" s="422">
-        <f t="shared" ref="X157:X161" si="3">IF(T157&gt;0,1,0)</f>
+        <f t="shared" ref="X157:X161" si="4">IF(T157&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="Y157" s="422">
-        <f t="shared" ref="Y157:Y161" si="4">IF(U157&gt;0,1,0)</f>
+        <f t="shared" ref="Y157:Y161" si="5">IF(U157&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="Z157" s="422">
-        <f t="shared" ref="Z157:Z161" si="5">IF(V157&gt;0,1,0)</f>
+        <f t="shared" ref="Z157:Z161" si="6">IF(V157&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="AA157" s="422">
-        <f t="shared" ref="AA157:AA161" si="6">IF(W157&gt;0,1,0)</f>
+        <f t="shared" ref="AA157:AA161" si="7">IF(W157&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="AB157" s="12"/>
@@ -41736,12 +42539,12 @@
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
       <c r="F158" s="22"/>
-      <c r="G158" s="459"/>
-      <c r="H158" s="459"/>
-      <c r="I158" s="459"/>
-      <c r="J158" s="459"/>
-      <c r="K158" s="459"/>
-      <c r="L158" s="460" t="s">
+      <c r="G158" s="445"/>
+      <c r="H158" s="445"/>
+      <c r="I158" s="445"/>
+      <c r="J158" s="445"/>
+      <c r="K158" s="445"/>
+      <c r="L158" s="446" t="s">
         <v>93</v>
       </c>
       <c r="M158" s="422">
@@ -41778,19 +42581,19 @@
         <v>0</v>
       </c>
       <c r="X158" s="422">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="Y158" s="422">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="Y158" s="422">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="Z158" s="422">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA158" s="422">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB158" s="12"/>
@@ -41805,12 +42608,12 @@
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
       <c r="F159" s="22"/>
-      <c r="G159" s="459"/>
-      <c r="H159" s="459"/>
-      <c r="I159" s="459"/>
-      <c r="J159" s="459"/>
-      <c r="K159" s="459"/>
-      <c r="L159" s="460" t="s">
+      <c r="G159" s="445"/>
+      <c r="H159" s="445"/>
+      <c r="I159" s="445"/>
+      <c r="J159" s="445"/>
+      <c r="K159" s="445"/>
+      <c r="L159" s="446" t="s">
         <v>471</v>
       </c>
       <c r="M159" s="422">
@@ -41847,19 +42650,19 @@
         <v>0</v>
       </c>
       <c r="X159" s="422">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="Y159" s="422">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="Y159" s="422">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="Z159" s="422">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA159" s="422">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB159" s="12"/>
@@ -41874,12 +42677,12 @@
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
       <c r="F160" s="22"/>
-      <c r="G160" s="459"/>
-      <c r="H160" s="459"/>
-      <c r="I160" s="459"/>
-      <c r="J160" s="459"/>
-      <c r="K160" s="459"/>
-      <c r="L160" s="460" t="s">
+      <c r="G160" s="445"/>
+      <c r="H160" s="445"/>
+      <c r="I160" s="445"/>
+      <c r="J160" s="445"/>
+      <c r="K160" s="445"/>
+      <c r="L160" s="446" t="s">
         <v>81</v>
       </c>
       <c r="M160" s="422">
@@ -41916,19 +42719,19 @@
         <v>0</v>
       </c>
       <c r="X160" s="422">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="Y160" s="422">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="Y160" s="422">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="Z160" s="422">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA160" s="422">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB160" s="12"/>
@@ -41943,12 +42746,12 @@
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
       <c r="F161" s="22"/>
-      <c r="G161" s="459"/>
-      <c r="H161" s="459"/>
-      <c r="I161" s="459"/>
-      <c r="J161" s="459"/>
-      <c r="K161" s="459"/>
-      <c r="L161" s="460" t="s">
+      <c r="G161" s="445"/>
+      <c r="H161" s="445"/>
+      <c r="I161" s="445"/>
+      <c r="J161" s="445"/>
+      <c r="K161" s="445"/>
+      <c r="L161" s="446" t="s">
         <v>79</v>
       </c>
       <c r="M161" s="422">
@@ -41985,19 +42788,19 @@
         <v>0</v>
       </c>
       <c r="X161" s="422">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="Y161" s="422">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="Y161" s="422">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="Z161" s="422">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA161" s="422">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB161" s="12"/>
@@ -42349,7 +43152,7 @@
       <c r="F172" s="9"/>
       <c r="G172" s="14"/>
       <c r="H172" s="9"/>
-      <c r="I172" s="457"/>
+      <c r="I172" s="443"/>
       <c r="J172" s="9"/>
       <c r="K172" s="9"/>
       <c r="L172" s="9"/>
@@ -42440,7 +43243,7 @@
       <c r="K175" s="441"/>
       <c r="L175" s="441"/>
       <c r="M175" s="441"/>
-      <c r="N175" s="458"/>
+      <c r="N175" s="444"/>
       <c r="O175" s="441"/>
       <c r="P175" s="441"/>
       <c r="Q175" s="441"/>
@@ -45347,7 +46150,7 @@
       <c r="D261" s="13"/>
       <c r="E261" s="13"/>
       <c r="F261" s="30"/>
-      <c r="H261" s="464" t="s">
+      <c r="H261" s="449" t="s">
         <v>514</v>
       </c>
       <c r="I261" s="427">
@@ -45384,7 +46187,7 @@
       <c r="D262" s="13"/>
       <c r="E262" s="13"/>
       <c r="F262" s="30"/>
-      <c r="H262" s="465" t="s">
+      <c r="H262" s="450" t="s">
         <v>515</v>
       </c>
       <c r="I262" s="427">
@@ -45421,7 +46224,7 @@
       <c r="D263" s="13"/>
       <c r="E263" s="13"/>
       <c r="F263" s="30"/>
-      <c r="H263" s="465" t="s">
+      <c r="H263" s="450" t="s">
         <v>73</v>
       </c>
       <c r="I263" s="427">
@@ -45458,7 +46261,7 @@
       <c r="D264" s="13"/>
       <c r="E264" s="13"/>
       <c r="F264" s="30"/>
-      <c r="H264" s="465" t="s">
+      <c r="H264" s="450" t="s">
         <v>516</v>
       </c>
       <c r="I264" s="427">
@@ -45495,7 +46298,7 @@
       <c r="D265" s="13"/>
       <c r="E265" s="13"/>
       <c r="F265" s="30"/>
-      <c r="H265" s="466" t="s">
+      <c r="H265" s="451" t="s">
         <v>76</v>
       </c>
       <c r="I265" s="427">
@@ -45532,7 +46335,7 @@
       <c r="D266" s="13"/>
       <c r="E266" s="13"/>
       <c r="F266" s="30"/>
-      <c r="H266" s="466" t="s">
+      <c r="H266" s="451" t="s">
         <v>75</v>
       </c>
       <c r="I266" s="427">
@@ -45569,7 +46372,7 @@
       <c r="D267" s="13"/>
       <c r="E267" s="13"/>
       <c r="F267" s="30"/>
-      <c r="H267" s="466" t="s">
+      <c r="H267" s="451" t="s">
         <v>74</v>
       </c>
       <c r="I267" s="427">
@@ -46047,7 +46850,7 @@
       <c r="D283" s="13"/>
       <c r="E283" s="13"/>
       <c r="F283" s="30"/>
-      <c r="H283" s="464" t="s">
+      <c r="H283" s="449" t="s">
         <v>514</v>
       </c>
       <c r="I283" s="46">
@@ -46085,7 +46888,7 @@
       <c r="D284" s="13"/>
       <c r="E284" s="13"/>
       <c r="F284" s="30"/>
-      <c r="H284" s="465" t="s">
+      <c r="H284" s="450" t="s">
         <v>515</v>
       </c>
       <c r="I284" s="46">
@@ -46123,7 +46926,7 @@
       <c r="D285" s="13"/>
       <c r="E285" s="13"/>
       <c r="F285" s="30"/>
-      <c r="H285" s="465" t="s">
+      <c r="H285" s="450" t="s">
         <v>73</v>
       </c>
       <c r="I285" s="46">
@@ -46161,7 +46964,7 @@
       <c r="D286" s="13"/>
       <c r="E286" s="13"/>
       <c r="F286" s="30"/>
-      <c r="H286" s="465" t="s">
+      <c r="H286" s="450" t="s">
         <v>516</v>
       </c>
       <c r="I286" s="46">
@@ -47456,7 +48259,7 @@
       <c r="G327" s="23"/>
       <c r="H327" s="23"/>
       <c r="I327" s="23" t="str">
-        <f t="shared" ref="I327:I334" si="7">I350</f>
+        <f t="shared" ref="I327:I334" si="8">I350</f>
         <v>pre seeding</v>
       </c>
       <c r="J327" s="294">
@@ -47491,7 +48294,7 @@
       <c r="G328" s="23"/>
       <c r="H328" s="23"/>
       <c r="I328" s="23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>at seeding</v>
       </c>
       <c r="J328" s="294">
@@ -47526,7 +48329,7 @@
       <c r="G329" s="23"/>
       <c r="H329" s="23"/>
       <c r="I329" s="23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>post seeding</v>
       </c>
       <c r="J329" s="294">
@@ -47561,7 +48364,7 @@
       <c r="G330" s="23"/>
       <c r="H330" s="23"/>
       <c r="I330" s="23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>cereal</v>
       </c>
       <c r="J330" s="294">
@@ -47596,7 +48399,7 @@
       <c r="G331" s="31"/>
       <c r="H331" s="31"/>
       <c r="I331" s="23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>oilseed</v>
       </c>
       <c r="J331" s="294">
@@ -47631,7 +48434,7 @@
       <c r="G332" s="23"/>
       <c r="H332" s="23"/>
       <c r="I332" s="23" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>pulse</v>
       </c>
       <c r="J332" s="294">
@@ -47666,7 +48469,7 @@
       <c r="G333" s="23"/>
       <c r="H333" s="23"/>
       <c r="I333" s="23" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J333" s="294">
@@ -47701,7 +48504,7 @@
       <c r="G334" s="23"/>
       <c r="H334" s="23"/>
       <c r="I334" s="23" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
       <c r="J334" s="294">
@@ -48177,7 +48980,7 @@
       <c r="G350" s="23"/>
       <c r="H350" s="23"/>
       <c r="I350" s="23" t="str">
-        <f>I306</f>
+        <f t="shared" ref="I350:I355" si="9">I306</f>
         <v>pre seeding</v>
       </c>
       <c r="J350" s="295">
@@ -48215,7 +49018,7 @@
       <c r="G351" s="23"/>
       <c r="H351" s="23"/>
       <c r="I351" s="23" t="str">
-        <f>I307</f>
+        <f t="shared" si="9"/>
         <v>at seeding</v>
       </c>
       <c r="J351" s="295">
@@ -48253,7 +49056,7 @@
       <c r="G352" s="23"/>
       <c r="H352" s="23"/>
       <c r="I352" s="23" t="str">
-        <f>I308</f>
+        <f t="shared" si="9"/>
         <v>post seeding</v>
       </c>
       <c r="J352" s="295">
@@ -48291,7 +49094,7 @@
       <c r="G353" s="23"/>
       <c r="H353" s="23"/>
       <c r="I353" s="23" t="str">
-        <f>I309</f>
+        <f t="shared" si="9"/>
         <v>cereal</v>
       </c>
       <c r="J353" s="295">
@@ -48329,7 +49132,7 @@
       <c r="G354" s="23"/>
       <c r="H354" s="23"/>
       <c r="I354" s="23" t="str">
-        <f>I310</f>
+        <f t="shared" si="9"/>
         <v>oilseed</v>
       </c>
       <c r="J354" s="295">
@@ -48362,7 +49165,7 @@
       <c r="G355" s="23"/>
       <c r="H355" s="23"/>
       <c r="I355" s="23" t="str">
-        <f>I311</f>
+        <f t="shared" si="9"/>
         <v>pulse</v>
       </c>
       <c r="J355" s="295">
@@ -48812,7 +49615,7 @@
       <c r="E370" s="13"/>
       <c r="F370" s="13"/>
       <c r="G370" s="13"/>
-      <c r="H370" s="453"/>
+      <c r="H370" s="464"/>
       <c r="I370" s="13"/>
       <c r="J370" s="13"/>
       <c r="K370" s="18"/>
@@ -48840,7 +49643,7 @@
       <c r="E371" s="13"/>
       <c r="F371" s="13"/>
       <c r="G371" s="13"/>
-      <c r="H371" s="453"/>
+      <c r="H371" s="464"/>
       <c r="I371" s="13"/>
       <c r="J371" s="19" t="s">
         <v>42</v>
@@ -48874,7 +49677,7 @@
       <c r="G372" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="H372" s="453"/>
+      <c r="H372" s="464"/>
       <c r="I372" s="13"/>
       <c r="J372" s="19" t="s">
         <v>67</v>
@@ -54915,10 +55718,10 @@
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
-      <c r="F68" s="454" t="s">
+      <c r="F68" s="467" t="s">
         <v>366</v>
       </c>
-      <c r="G68" s="455"/>
+      <c r="G68" s="468"/>
       <c r="H68" s="19"/>
       <c r="I68" s="19" t="s">
         <v>367</v>
@@ -55750,8 +56553,8 @@
       <c r="B96" s="2"/>
       <c r="C96" s="13"/>
       <c r="D96" s="13"/>
-      <c r="E96" s="454"/>
-      <c r="F96" s="455"/>
+      <c r="E96" s="467"/>
+      <c r="F96" s="468"/>
       <c r="G96" s="19" t="s">
         <v>374</v>
       </c>

</xml_diff>

<commit_message>
fix couple of sheep errors and do initial numbers and some fvp stuff
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78425C1F-96FD-4647-B274-671A745E7CF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F481B2-C603-4760-BDCE-D96D95BA6408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -2873,7 +2873,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="527">
   <si>
     <t>«</t>
   </si>
@@ -4482,6 +4482,9 @@
   </si>
   <si>
     <t>Current rotations represented below:</t>
+  </si>
+  <si>
+    <t>*season type will have to be added. Note sheep use the first slice to determine the break of season</t>
   </si>
 </sst>
 </file>
@@ -6820,9 +6823,9 @@
       <sheetName val="Mach 1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="26">
           <cell r="I26" t="str">
@@ -6885,7 +6888,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="35">
           <cell r="B35">
@@ -13052,9 +13055,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB23067-7440-4A35-B3C1-23A2B3B50502}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13063,12 +13068,12 @@
     <col min="3" max="16384" width="8.88671875" style="97"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="98" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="102" t="s">
         <v>116</v>
       </c>
@@ -13079,7 +13084,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="99">
         <v>0</v>
       </c>
@@ -13091,7 +13096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="99">
         <v>1</v>
       </c>
@@ -13102,8 +13107,11 @@
         <f t="shared" ref="C5:C12" si="0">B6-B5</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" s="97" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="99">
         <v>2</v>
       </c>
@@ -13115,7 +13123,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="99">
         <v>3</v>
       </c>
@@ -13127,7 +13135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="99">
         <v>4</v>
       </c>
@@ -13139,7 +13147,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="99">
         <v>5</v>
       </c>
@@ -13151,7 +13159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="99">
         <v>6</v>
       </c>
@@ -13163,7 +13171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="99">
         <v>7</v>
       </c>
@@ -13175,7 +13183,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="99">
         <v>8</v>
       </c>
@@ -13187,7 +13195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="99">
         <v>9</v>
       </c>
@@ -13199,7 +13207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="99">
         <v>10</v>
       </c>
@@ -37032,8 +37040,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AU487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A336" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L362" sqref="L362"/>
+    <sheetView topLeftCell="A159" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H296" sqref="H296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="12" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
small changes to pp (including adding sire onhand) and more dubugging of numbers
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E55CCAA-EDC6-48E2-8B65-6FA14761497F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5698D2CD-AA46-4E25-8C0B-5D532F7FFA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -154,6 +154,7 @@
     <definedName name="spray_prep">Labour!$P$97:$Q$100</definedName>
     <definedName name="sprayer_crop_allocation" localSheetId="8">Mach!$B$39</definedName>
     <definedName name="start_harvest_crops" localSheetId="5">Crop!$H$64:$I$75</definedName>
+    <definedName name="steady_state">General!$M$25</definedName>
     <definedName name="step_size">Stubble!$H$88</definedName>
     <definedName name="storage_cost_date">'Sup Feed'!$K$32</definedName>
     <definedName name="storage_grain">'[1]Sup Feed'!$I$26:$N$28</definedName>
@@ -12291,8 +12292,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:Z63"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16393,7 +16394,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:BD427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+    <sheetView topLeftCell="A194" workbookViewId="0">
       <selection activeCell="O223" sqref="O223:O226"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to pasture & harvest time
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CB6493-ECFD-4F69-91D0-F0D0996D9325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE89F559-FD4E-4DD3-82DD-81D1771ACDFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27645" windowHeight="15360" activeTab="4" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="990" yWindow="150" windowWidth="27645" windowHeight="15360" activeTab="4" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -905,6 +905,31 @@
           </rPr>
           <t xml:space="preserve">
 Note APa doesn't exist therefore only necessary option is CPa</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T264" authorId="1" shapeId="0" xr:uid="{C6CAF181-37E2-4F82-A4EA-A528C123A019}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the range of digestibility of the top 25% of the feed compared with the bottom 25%. Which is roughly the 10 to 90 percentile range (because the average of the top 25% is roughly the 10 percentile value)
+Value is to be for a low FOO sward. Increasing FOO increases the range in digestibility. The high end remains the same but the low end is reduced.</t>
         </r>
       </text>
     </comment>
@@ -3734,9 +3759,6 @@
     <t>digestibility if deferred</t>
   </si>
   <si>
-    <t>of sward</t>
-  </si>
-  <si>
     <t>senescing feed relative</t>
   </si>
   <si>
@@ -3747,9 +3769,6 @@
   </si>
   <si>
     <t>1 month</t>
-  </si>
-  <si>
-    <t>components</t>
   </si>
   <si>
     <t>to green diet digestibility</t>
@@ -4566,6 +4585,12 @@
       <t>-potentially this could come from the the simulation-ev_cutoff_p6f</t>
     </r>
   </si>
+  <si>
+    <t>of sward components</t>
+  </si>
+  <si>
+    <t>(low FOO)</t>
+  </si>
 </sst>
 </file>
 
@@ -5178,7 +5203,7 @@
     <xf numFmtId="0" fontId="23" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="473">
+  <cellXfs count="474">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -6315,6 +6340,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="16" fillId="8" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Calculations" xfId="6" xr:uid="{449B9FA0-BCFF-41FE-A9C5-7F4DFD2D1D3B}"/>
@@ -7377,7 +7405,7 @@
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -7693,7 +7721,7 @@
       <c r="G29" s="242"/>
       <c r="H29" s="242"/>
       <c r="I29" s="242" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="J29" s="443">
         <v>1</v>
@@ -8212,7 +8240,7 @@
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
@@ -8501,7 +8529,7 @@
         <v>126</v>
       </c>
       <c r="H58" s="243" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I58" s="240"/>
       <c r="J58" s="241"/>
@@ -9365,14 +9393,14 @@
       <c r="E88" s="16"/>
       <c r="F88" s="25"/>
       <c r="G88" s="26" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H88" s="444">
         <v>1</v>
       </c>
       <c r="I88" s="54"/>
       <c r="K88" s="348" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="L88" s="445">
         <v>0.05</v>
@@ -9548,7 +9576,7 @@
       <c r="K94" s="53"/>
       <c r="L94" s="53"/>
       <c r="M94" s="33" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N94" s="33"/>
       <c r="O94" s="55"/>
@@ -9574,7 +9602,7 @@
       <c r="G95" s="33"/>
       <c r="H95" s="33"/>
       <c r="I95" s="55" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J95" s="244"/>
       <c r="K95" s="53"/>
@@ -9582,7 +9610,7 @@
       <c r="M95" s="33"/>
       <c r="N95" s="33"/>
       <c r="O95" s="55" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="P95" s="31"/>
       <c r="Q95" s="31"/>
@@ -9922,7 +9950,7 @@
       <c r="K105" s="53"/>
       <c r="L105" s="53"/>
       <c r="M105" s="33" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="N105" s="33"/>
       <c r="O105" s="55"/>
@@ -9948,7 +9976,7 @@
       <c r="G106" s="33"/>
       <c r="H106" s="33"/>
       <c r="I106" s="55" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J106" s="53"/>
       <c r="K106" s="53"/>
@@ -9956,7 +9984,7 @@
       <c r="M106" s="33"/>
       <c r="N106" s="33"/>
       <c r="O106" s="55" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="P106" s="31"/>
       <c r="Q106" s="31"/>
@@ -10294,7 +10322,7 @@
       <c r="E116" s="16"/>
       <c r="F116" s="25"/>
       <c r="G116" s="33" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H116" s="33"/>
       <c r="I116" s="54"/>
@@ -10326,19 +10354,19 @@
       <c r="G117" s="33"/>
       <c r="H117" s="33"/>
       <c r="I117" s="158" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J117" s="448" t="s">
+        <v>433</v>
+      </c>
+      <c r="K117" s="448" t="s">
+        <v>434</v>
+      </c>
+      <c r="L117" s="448" t="s">
         <v>435</v>
       </c>
-      <c r="K117" s="448" t="s">
+      <c r="M117" s="448" t="s">
         <v>436</v>
-      </c>
-      <c r="L117" s="448" t="s">
-        <v>437</v>
-      </c>
-      <c r="M117" s="448" t="s">
-        <v>438</v>
       </c>
       <c r="N117" s="56"/>
       <c r="O117" s="56"/>
@@ -10710,7 +10738,7 @@
       <c r="E127" s="16"/>
       <c r="F127" s="25"/>
       <c r="G127" s="33" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H127" s="33"/>
       <c r="I127" s="54"/>
@@ -10742,19 +10770,19 @@
       <c r="G128" s="33"/>
       <c r="H128" s="33"/>
       <c r="I128" s="158" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J128" s="448" t="s">
+        <v>433</v>
+      </c>
+      <c r="K128" s="448" t="s">
+        <v>434</v>
+      </c>
+      <c r="L128" s="448" t="s">
         <v>435</v>
       </c>
-      <c r="K128" s="448" t="s">
+      <c r="M128" s="448" t="s">
         <v>436</v>
-      </c>
-      <c r="L128" s="448" t="s">
-        <v>437</v>
-      </c>
-      <c r="M128" s="448" t="s">
-        <v>438</v>
       </c>
       <c r="N128" s="56"/>
       <c r="O128" s="56"/>
@@ -11126,7 +11154,7 @@
       <c r="E138" s="16"/>
       <c r="F138" s="25"/>
       <c r="G138" s="33" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H138" s="33"/>
       <c r="I138" s="54"/>
@@ -11164,10 +11192,10 @@
         <v>81</v>
       </c>
       <c r="K139" s="448" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L139" s="448" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="M139" s="56"/>
       <c r="N139" s="56"/>
@@ -11532,7 +11560,7 @@
       <c r="E149" s="16"/>
       <c r="F149" s="25"/>
       <c r="G149" s="33" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H149" s="33"/>
       <c r="I149" s="54"/>
@@ -11570,10 +11598,10 @@
         <v>81</v>
       </c>
       <c r="K150" s="448" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L150" s="448" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="M150" s="56"/>
       <c r="N150" s="56"/>
@@ -12267,10 +12295,10 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G3" s="74" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H3" s="74" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -12432,7 +12460,7 @@
       </c>
       <c r="F17" s="282"/>
       <c r="G17" s="283" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H17" s="282"/>
       <c r="I17" s="282"/>
@@ -12493,7 +12521,7 @@
       <c r="H19" s="282"/>
       <c r="I19" s="282"/>
       <c r="J19" s="282" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K19" s="282"/>
       <c r="L19" s="282"/>
@@ -12637,14 +12665,14 @@
       <c r="H24" s="286"/>
       <c r="I24" s="286"/>
       <c r="J24" s="292" t="s">
+        <v>498</v>
+      </c>
+      <c r="K24" s="292" t="s">
         <v>500</v>
-      </c>
-      <c r="K24" s="292" t="s">
-        <v>502</v>
       </c>
       <c r="L24" s="293"/>
       <c r="M24" s="375" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="N24" s="293"/>
       <c r="O24" s="293"/>
@@ -12670,7 +12698,7 @@
       <c r="G25" s="74"/>
       <c r="H25" s="298"/>
       <c r="I25" s="309" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="J25" s="380">
         <v>1</v>
@@ -12956,7 +12984,7 @@
       <c r="E35" s="286"/>
       <c r="F35" s="302"/>
       <c r="G35" s="298" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H35" s="298"/>
       <c r="I35" s="298"/>
@@ -13166,7 +13194,7 @@
       </c>
       <c r="F42" s="282"/>
       <c r="G42" s="283" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H42" s="282"/>
       <c r="I42" s="282"/>
@@ -13196,7 +13224,7 @@
       <c r="E43" s="286"/>
       <c r="F43" s="282"/>
       <c r="G43" s="282" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H43" s="282"/>
       <c r="I43" s="282"/>
@@ -13229,7 +13257,7 @@
         <v>38576.728726851848</v>
       </c>
       <c r="H44" s="282" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I44" s="282"/>
       <c r="J44" s="282"/>
@@ -13350,7 +13378,7 @@
       <c r="K48" s="292"/>
       <c r="L48" s="293"/>
       <c r="M48" s="293" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N48" s="293"/>
       <c r="O48" s="293"/>
@@ -13377,7 +13405,7 @@
       <c r="H49" s="286"/>
       <c r="I49" s="286"/>
       <c r="J49" s="292" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K49" s="292"/>
       <c r="L49" s="293"/>
@@ -13406,7 +13434,7 @@
       <c r="G50" s="74"/>
       <c r="H50" s="298"/>
       <c r="I50" s="309" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J50" s="385">
         <v>1500</v>
@@ -13440,7 +13468,7 @@
       <c r="G51" s="74"/>
       <c r="H51" s="298"/>
       <c r="I51" s="309" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J51" s="385">
         <v>15000</v>
@@ -13474,7 +13502,7 @@
       <c r="G52" s="74"/>
       <c r="H52" s="298"/>
       <c r="I52" s="309" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J52" s="385">
         <v>2000</v>
@@ -13508,7 +13536,7 @@
       <c r="G53" s="74"/>
       <c r="H53" s="298"/>
       <c r="I53" s="309" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J53" s="385">
         <v>5000</v>
@@ -13542,7 +13570,7 @@
       <c r="G54" s="74"/>
       <c r="H54" s="298"/>
       <c r="I54" s="309" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J54" s="385">
         <v>50000</v>
@@ -13576,7 +13604,7 @@
       <c r="G55" s="74"/>
       <c r="H55" s="298"/>
       <c r="I55" s="309" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J55" s="385">
         <v>1500</v>
@@ -13610,7 +13638,7 @@
       <c r="G56" s="74"/>
       <c r="H56" s="298"/>
       <c r="I56" s="309" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J56" s="385">
         <v>10000</v>
@@ -13644,7 +13672,7 @@
       <c r="G57" s="74"/>
       <c r="H57" s="298"/>
       <c r="I57" s="309" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J57" s="385">
         <v>7500</v>
@@ -13678,7 +13706,7 @@
       <c r="G58" s="74"/>
       <c r="H58" s="298"/>
       <c r="I58" s="309" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J58" s="385">
         <v>6000</v>
@@ -13736,7 +13764,7 @@
       <c r="E60" s="286"/>
       <c r="F60" s="302"/>
       <c r="G60" s="298" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H60" s="298"/>
       <c r="I60" s="298"/>
@@ -13916,7 +13944,7 @@
         <v>28</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -14155,7 +14183,7 @@
       </c>
       <c r="F4" s="282"/>
       <c r="G4" s="283" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H4" s="282"/>
       <c r="I4" s="282"/>
@@ -14185,7 +14213,7 @@
       <c r="E5" s="286"/>
       <c r="F5" s="282"/>
       <c r="G5" s="282" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H5" s="282"/>
       <c r="I5" s="282"/>
@@ -14219,7 +14247,7 @@
       </c>
       <c r="H6" s="282"/>
       <c r="I6" s="282" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J6" s="282"/>
       <c r="K6" s="282"/>
@@ -14336,10 +14364,10 @@
       <c r="H10" s="286"/>
       <c r="I10" s="286"/>
       <c r="J10" s="292" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K10" s="292" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L10" s="293"/>
       <c r="M10" s="293"/>
@@ -14424,10 +14452,10 @@
       <c r="H13" s="295"/>
       <c r="I13" s="295"/>
       <c r="J13" s="296" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K13" s="296" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L13" s="296"/>
       <c r="M13" s="296"/>
@@ -14454,7 +14482,7 @@
       <c r="F14" s="294"/>
       <c r="H14" s="298"/>
       <c r="I14" s="311" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J14" s="388">
         <v>70</v>
@@ -14487,7 +14515,7 @@
       <c r="F15" s="294"/>
       <c r="H15" s="298"/>
       <c r="I15" s="311" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J15" s="388">
         <v>4760</v>
@@ -14496,10 +14524,10 @@
         <v>6752</v>
       </c>
       <c r="L15" s="298" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M15" s="298" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="N15" s="311"/>
       <c r="O15" s="299"/>
@@ -14524,7 +14552,7 @@
       <c r="F16" s="294"/>
       <c r="H16" s="298"/>
       <c r="I16" s="311" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J16" s="388">
         <v>30</v>
@@ -14533,7 +14561,7 @@
         <v>30</v>
       </c>
       <c r="L16" s="298" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="M16" s="311"/>
       <c r="N16" s="311"/>
@@ -14559,7 +14587,7 @@
       <c r="F17" s="294"/>
       <c r="H17" s="298"/>
       <c r="I17" s="311" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J17" s="2">
         <f>J15/EXP(J16*LN(1.2))</f>
@@ -14570,7 +14598,7 @@
         <v>28.444287013806314</v>
       </c>
       <c r="L17" s="298" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="M17" s="311"/>
       <c r="N17" s="311"/>
@@ -14596,7 +14624,7 @@
       <c r="F18" s="302"/>
       <c r="H18" s="298"/>
       <c r="I18" s="312" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J18" s="389">
         <v>3.6</v>
@@ -14779,7 +14807,7 @@
       </c>
       <c r="F24" s="282"/>
       <c r="G24" s="283" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H24" s="282"/>
       <c r="I24" s="282"/>
@@ -14809,7 +14837,7 @@
       <c r="E25" s="286"/>
       <c r="F25" s="282"/>
       <c r="G25" s="282" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H25" s="282"/>
       <c r="I25" s="282"/>
@@ -15229,7 +15257,7 @@
       </c>
       <c r="F39" s="282"/>
       <c r="G39" s="283" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H39" s="282"/>
       <c r="I39" s="282"/>
@@ -15262,7 +15290,7 @@
       <c r="E40" s="286"/>
       <c r="F40" s="282"/>
       <c r="G40" s="282" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H40" s="316"/>
       <c r="I40" s="282"/>
@@ -15330,7 +15358,7 @@
       <c r="E42" s="286"/>
       <c r="F42" s="282"/>
       <c r="G42" s="310" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H42" s="316"/>
       <c r="I42" s="282"/>
@@ -15431,7 +15459,7 @@
       <c r="I45" s="320"/>
       <c r="J45" s="292"/>
       <c r="K45" s="292" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L45" s="292"/>
       <c r="M45" s="291"/>
@@ -15464,7 +15492,7 @@
       <c r="I46" s="320"/>
       <c r="J46" s="291"/>
       <c r="K46" s="291" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L46" s="291"/>
       <c r="M46" s="291"/>
@@ -15524,7 +15552,7 @@
       <c r="E48" s="286"/>
       <c r="F48" s="294"/>
       <c r="G48" s="327" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H48" s="323"/>
       <c r="I48" s="324"/>
@@ -15580,10 +15608,10 @@
       <c r="F50" s="294"/>
       <c r="G50" s="329"/>
       <c r="H50" s="329" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I50" s="329" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J50" s="329"/>
       <c r="K50" s="329"/>
@@ -15605,7 +15633,7 @@
       <c r="E51" s="286"/>
       <c r="F51" s="294"/>
       <c r="G51" s="341" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H51" s="391">
         <v>0.1</v>
@@ -15614,7 +15642,7 @@
         <v>0.2</v>
       </c>
       <c r="J51" s="329" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K51" s="393">
         <f>H51*60</f>
@@ -15625,7 +15653,7 @@
         <v>12</v>
       </c>
       <c r="M51" s="329" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="Q51" s="329"/>
       <c r="R51" s="329"/>
@@ -15649,7 +15677,7 @@
       <c r="E52" s="286"/>
       <c r="F52" s="294"/>
       <c r="G52" s="341" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H52" s="391">
         <v>0.1</v>
@@ -15658,7 +15686,7 @@
         <v>0.1</v>
       </c>
       <c r="J52" s="329" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K52" s="393">
         <f>H52*60</f>
@@ -15669,7 +15697,7 @@
         <v>6</v>
       </c>
       <c r="M52" s="329" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="Q52" s="329"/>
       <c r="R52" s="329"/>
@@ -15693,7 +15721,7 @@
       <c r="E53" s="286"/>
       <c r="F53" s="294"/>
       <c r="G53" s="341" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H53" s="391">
         <v>2</v>
@@ -15702,7 +15730,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="329" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K53" s="329"/>
       <c r="L53" s="329"/>
@@ -15736,7 +15764,7 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="J54" s="329" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K54" s="329"/>
       <c r="L54" s="329"/>
@@ -15769,12 +15797,12 @@
       <c r="L55" s="332"/>
       <c r="M55" s="332"/>
       <c r="N55" s="336" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="O55" s="332"/>
       <c r="P55" s="332"/>
       <c r="Q55" s="329" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="R55" s="333"/>
       <c r="V55" s="334"/>
@@ -15819,26 +15847,26 @@
       <c r="E57" s="286"/>
       <c r="F57" s="301"/>
       <c r="H57" s="335" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="K57" s="332"/>
       <c r="L57" s="332"/>
       <c r="M57" s="332"/>
       <c r="N57" s="332" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O57" s="394">
         <v>0.2</v>
       </c>
       <c r="P57" s="337" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="Q57" s="396">
         <f>O57*60</f>
         <v>12</v>
       </c>
       <c r="R57" s="332" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="V57" s="334"/>
       <c r="W57" s="285"/>
@@ -15863,13 +15891,13 @@
       <c r="L58" s="332"/>
       <c r="M58" s="332"/>
       <c r="N58" s="331" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="O58" s="395">
         <v>2</v>
       </c>
       <c r="P58" s="337" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="Q58" s="332"/>
       <c r="R58" s="332"/>
@@ -15915,10 +15943,10 @@
       <c r="E60" s="286"/>
       <c r="F60" s="301"/>
       <c r="H60" s="326" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I60" s="331" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L60" s="332"/>
       <c r="M60" s="332"/>
@@ -15938,7 +15966,7 @@
       <c r="AA60" s="277"/>
       <c r="AB60" s="277"/>
       <c r="AC60" s="323" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15952,20 +15980,20 @@
         <v>117</v>
       </c>
       <c r="H61" s="331" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="I61" s="331" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="M61" s="332"/>
       <c r="N61" s="332" t="s">
         <v>117</v>
       </c>
       <c r="O61" s="332" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="P61" s="338" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="Q61" s="332"/>
       <c r="U61" s="333"/>
@@ -16230,7 +16258,7 @@
       <c r="AA68" s="277"/>
       <c r="AB68" s="277"/>
       <c r="AC68" s="323" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="69" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16263,7 +16291,7 @@
       <c r="AA69" s="277"/>
       <c r="AB69" s="277"/>
       <c r="AC69" s="323" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16301,7 +16329,7 @@
       <c r="AA70" s="277"/>
       <c r="AB70" s="277"/>
       <c r="AC70" s="323" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16334,7 +16362,7 @@
       <c r="AA71" s="277"/>
       <c r="AB71" s="277"/>
       <c r="AC71" s="323" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -16348,8 +16376,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:BD427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="K167" sqref="K167:O171"/>
+    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="S269" sqref="S269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -20317,7 +20345,7 @@
       <c r="F110" s="114"/>
       <c r="G110" s="116"/>
       <c r="H110" s="116" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I110" s="116"/>
       <c r="J110" s="176">
@@ -20431,7 +20459,7 @@
       <c r="F112" s="114"/>
       <c r="G112" s="116"/>
       <c r="H112" s="116" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I112" s="116"/>
       <c r="J112" s="346">
@@ -20439,7 +20467,7 @@
       </c>
       <c r="K112" s="116"/>
       <c r="L112" s="116" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="M112" s="116"/>
       <c r="N112" s="116"/>
@@ -20489,7 +20517,7 @@
       <c r="F113" s="114"/>
       <c r="G113" s="116"/>
       <c r="H113" s="344" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I113" s="116"/>
       <c r="J113" s="345">
@@ -20498,7 +20526,7 @@
       </c>
       <c r="K113" s="116"/>
       <c r="L113" s="116" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="M113" s="116"/>
       <c r="N113" s="116"/>
@@ -21085,7 +21113,7 @@
       </c>
       <c r="R123" s="191"/>
       <c r="S123" s="189" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="T123" s="123"/>
       <c r="U123" s="123"/>
@@ -21441,7 +21469,7 @@
       <c r="I132" s="98"/>
       <c r="J132" s="98"/>
       <c r="K132" s="106" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L132" s="98"/>
       <c r="M132" s="98"/>
@@ -21471,7 +21499,7 @@
       <c r="I133" s="106"/>
       <c r="J133" s="106"/>
       <c r="K133" s="80" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="L133" s="106"/>
       <c r="M133" s="106"/>
@@ -21591,7 +21619,7 @@
         <v>200</v>
       </c>
       <c r="M137" s="170" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="N137" s="170" t="s">
         <v>201</v>
@@ -21725,7 +21753,7 @@
         <v>23</v>
       </c>
       <c r="M140" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N140" s="347">
         <f>IF(AND(O140=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q140)</f>
@@ -21770,7 +21798,7 @@
         <v>91</v>
       </c>
       <c r="M141" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N141" s="347">
         <f>IF(AND(O141=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q141)</f>
@@ -21815,7 +21843,7 @@
         <v>92</v>
       </c>
       <c r="M142" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N142" s="347">
         <f>IF(AND(O142=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q142)</f>
@@ -21860,7 +21888,7 @@
         <v>204</v>
       </c>
       <c r="M143" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N143" s="347">
         <f>IF(AND(O143=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q143)</f>
@@ -21899,13 +21927,13 @@
         <v>203</v>
       </c>
       <c r="K144" s="172" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L144" s="172" t="s">
         <v>91</v>
       </c>
       <c r="M144" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N144" s="347">
         <f>IF(AND(O144=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q144)</f>
@@ -21944,13 +21972,13 @@
         <v>203</v>
       </c>
       <c r="K145" s="172" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L145" s="172" t="s">
         <v>92</v>
       </c>
       <c r="M145" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N145" s="347">
         <f>IF(AND(O145=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q145)</f>
@@ -21989,13 +22017,13 @@
         <v>203</v>
       </c>
       <c r="K146" s="172" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L146" s="172" t="s">
         <v>93</v>
       </c>
       <c r="M146" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N146" s="347">
         <f>IF(AND(O146=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q146)</f>
@@ -22034,13 +22062,13 @@
         <v>203</v>
       </c>
       <c r="K147" s="172" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L147" s="172" t="s">
         <v>204</v>
       </c>
       <c r="M147" s="172" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N147" s="347">
         <f>IF(AND(O147=1,(Date_Destocking&lt;'Feed Budget'!$B$4)),0,$Q147)</f>
@@ -22337,7 +22365,7 @@
       </c>
       <c r="F154" s="89"/>
       <c r="G154" s="90" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H154" s="91"/>
       <c r="I154" s="91"/>
@@ -22717,7 +22745,7 @@
       <c r="U160" s="111"/>
       <c r="V160" s="111"/>
       <c r="W160" s="136" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="X160" s="136"/>
       <c r="Y160" s="111"/>
@@ -24150,7 +24178,7 @@
       </c>
       <c r="F178" s="89"/>
       <c r="G178" s="90" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H178" s="91"/>
       <c r="I178" s="91"/>
@@ -24530,7 +24558,7 @@
       <c r="U184" s="111"/>
       <c r="V184" s="111"/>
       <c r="W184" s="136" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="X184" s="136"/>
       <c r="Y184" s="111"/>
@@ -24895,7 +24923,7 @@
         <v>50</v>
       </c>
       <c r="Y188" s="116" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="Z188" s="116"/>
       <c r="AA188" s="116"/>
@@ -27113,7 +27141,7 @@
       <c r="F223" s="114"/>
       <c r="G223" s="123"/>
       <c r="H223" s="123" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I223" s="139"/>
       <c r="J223" s="123"/>
@@ -27225,7 +27253,7 @@
       <c r="F225" s="114"/>
       <c r="G225" s="123"/>
       <c r="H225" s="123" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I225" s="139"/>
       <c r="J225" s="123"/>
@@ -27281,7 +27309,7 @@
       <c r="F226" s="114"/>
       <c r="G226" s="123"/>
       <c r="H226" s="123" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I226" s="139"/>
       <c r="J226" s="123"/>
@@ -29513,15 +29541,15 @@
       </c>
       <c r="S265" s="110"/>
       <c r="T265" s="110" t="s">
-        <v>258</v>
+        <v>530</v>
       </c>
       <c r="U265" s="110"/>
       <c r="V265" s="111" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="W265" s="111"/>
       <c r="X265" s="111" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y265" s="110"/>
       <c r="Z265" s="94"/>
@@ -29582,19 +29610,19 @@
         <v>71</v>
       </c>
       <c r="P266" s="170" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q266" s="111"/>
       <c r="R266" s="111" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="S266" s="111"/>
       <c r="T266" s="111" t="s">
-        <v>263</v>
+        <v>531</v>
       </c>
       <c r="U266" s="111"/>
       <c r="V266" s="111" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="W266" s="111"/>
       <c r="X266" s="111"/>
@@ -29892,7 +29920,7 @@
       </c>
       <c r="Q270" s="116"/>
       <c r="R270" s="135">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="S270" s="116"/>
       <c r="T270" s="133">
@@ -29969,7 +29997,7 @@
       </c>
       <c r="Q271" s="116"/>
       <c r="R271" s="135">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="S271" s="116"/>
       <c r="T271" s="133">
@@ -30743,7 +30771,7 @@
       </c>
       <c r="F283" s="89"/>
       <c r="G283" s="90" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H283" s="91"/>
       <c r="I283" s="91"/>
@@ -30797,7 +30825,7 @@
       <c r="E284" s="96"/>
       <c r="F284" s="97"/>
       <c r="G284" s="98" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H284" s="98"/>
       <c r="I284" s="98"/>
@@ -30967,7 +30995,7 @@
         <v>214</v>
       </c>
       <c r="K287" s="213" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L287" s="110"/>
       <c r="M287" s="110"/>
@@ -30976,7 +31004,7 @@
         <v>214</v>
       </c>
       <c r="P287" s="213" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Q287" s="110"/>
       <c r="R287" s="110"/>
@@ -31025,14 +31053,14 @@
       <c r="I288" s="96"/>
       <c r="J288" s="96"/>
       <c r="K288" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L288" s="110"/>
       <c r="M288" s="110"/>
       <c r="N288" s="110"/>
       <c r="O288" s="96"/>
       <c r="P288" s="214" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Q288" s="110"/>
       <c r="R288" s="110"/>
@@ -31081,24 +31109,24 @@
       <c r="I289" s="111"/>
       <c r="J289" s="111"/>
       <c r="K289" s="136" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L289" s="136"/>
       <c r="M289" s="136"/>
       <c r="N289" s="111"/>
       <c r="O289" s="111"/>
       <c r="P289" s="136" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Q289" s="136"/>
       <c r="R289" s="136"/>
       <c r="S289" s="111"/>
       <c r="T289" s="136" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="U289" s="136"/>
       <c r="V289" s="219" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W289" s="94"/>
       <c r="X289" s="132"/>
@@ -31137,41 +31165,41 @@
       <c r="E290" s="112"/>
       <c r="F290" s="96"/>
       <c r="G290" s="111" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H290" s="111" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I290" s="111" t="s">
         <v>208</v>
       </c>
       <c r="J290" s="111"/>
       <c r="K290" s="111" t="s">
+        <v>273</v>
+      </c>
+      <c r="L290" s="111" t="s">
+        <v>274</v>
+      </c>
+      <c r="M290" s="111" t="s">
         <v>275</v>
-      </c>
-      <c r="L290" s="111" t="s">
-        <v>276</v>
-      </c>
-      <c r="M290" s="111" t="s">
-        <v>277</v>
       </c>
       <c r="N290" s="111"/>
       <c r="O290" s="111"/>
       <c r="P290" s="111" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q290" s="111" t="s">
+        <v>274</v>
+      </c>
+      <c r="R290" s="111" t="s">
         <v>275</v>
-      </c>
-      <c r="Q290" s="111" t="s">
-        <v>276</v>
-      </c>
-      <c r="R290" s="111" t="s">
-        <v>277</v>
       </c>
       <c r="S290" s="111"/>
       <c r="T290" s="111" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="U290" s="111" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="V290" s="219"/>
       <c r="W290" s="94"/>
@@ -32135,7 +32163,7 @@
         <v>214</v>
       </c>
       <c r="I304" s="217" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J304" s="123"/>
       <c r="K304" s="141"/>
@@ -32189,7 +32217,7 @@
       <c r="G305" s="123"/>
       <c r="H305" s="217"/>
       <c r="I305" s="218" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J305" s="123"/>
       <c r="K305" s="141"/>
@@ -32295,7 +32323,7 @@
       <c r="E307" s="125"/>
       <c r="F307" s="125"/>
       <c r="G307" s="126" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H307" s="127"/>
       <c r="I307" s="127"/>
@@ -32491,7 +32519,7 @@
       </c>
       <c r="F312" s="89"/>
       <c r="G312" s="90" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H312" s="91"/>
       <c r="I312" s="91"/>
@@ -32519,7 +32547,7 @@
       <c r="E313" s="96"/>
       <c r="F313" s="97"/>
       <c r="G313" s="98" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H313" s="98"/>
       <c r="I313" s="98"/>
@@ -32765,14 +32793,14 @@
       <c r="E322" s="112"/>
       <c r="F322" s="114"/>
       <c r="G322" s="226" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H322" s="223"/>
       <c r="I322" s="223"/>
       <c r="J322" s="224"/>
       <c r="K322" s="225"/>
       <c r="L322" s="225" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="M322" s="142" t="s">
         <v>67</v>
@@ -32808,7 +32836,7 @@
       <c r="I323" s="223"/>
       <c r="J323" s="225"/>
       <c r="K323" s="227" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L323" s="238">
         <v>0</v>
@@ -33266,7 +33294,7 @@
       <c r="E336" s="125"/>
       <c r="F336" s="125"/>
       <c r="G336" s="126" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H336" s="127"/>
       <c r="I336" s="127"/>
@@ -33486,7 +33514,7 @@
       </c>
       <c r="F341" s="147"/>
       <c r="G341" s="148" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H341" s="147"/>
       <c r="I341" s="147"/>
@@ -33540,7 +33568,7 @@
       <c r="E342" s="96"/>
       <c r="F342" s="147"/>
       <c r="G342" s="147" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H342" s="150"/>
       <c r="I342" s="147"/>
@@ -33807,26 +33835,26 @@
       <c r="F347" s="96"/>
       <c r="G347" s="96"/>
       <c r="H347" s="96" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I347" s="96"/>
       <c r="J347" s="111" t="s">
+        <v>287</v>
+      </c>
+      <c r="K347" s="111" t="s">
+        <v>288</v>
+      </c>
+      <c r="L347" s="111" t="s">
         <v>289</v>
       </c>
-      <c r="K347" s="111" t="s">
+      <c r="M347" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="L347" s="111" t="s">
+      <c r="N347" s="111" t="s">
+        <v>289</v>
+      </c>
+      <c r="O347" s="111" t="s">
         <v>291</v>
-      </c>
-      <c r="M347" s="111" t="s">
-        <v>292</v>
-      </c>
-      <c r="N347" s="111" t="s">
-        <v>291</v>
-      </c>
-      <c r="O347" s="111" t="s">
-        <v>293</v>
       </c>
       <c r="P347" s="111"/>
       <c r="Q347" s="111"/>
@@ -33875,22 +33903,22 @@
       <c r="H348" s="96"/>
       <c r="I348" s="96"/>
       <c r="J348" s="111" t="s">
+        <v>292</v>
+      </c>
+      <c r="K348" s="111" t="s">
+        <v>293</v>
+      </c>
+      <c r="L348" s="111" t="s">
         <v>294</v>
       </c>
-      <c r="K348" s="111" t="s">
+      <c r="M348" s="111" t="s">
         <v>295</v>
       </c>
-      <c r="L348" s="111" t="s">
+      <c r="N348" s="111" t="s">
         <v>296</v>
       </c>
-      <c r="M348" s="111" t="s">
+      <c r="O348" s="111" t="s">
         <v>297</v>
-      </c>
-      <c r="N348" s="111" t="s">
-        <v>298</v>
-      </c>
-      <c r="O348" s="111" t="s">
-        <v>299</v>
       </c>
       <c r="P348" s="111"/>
       <c r="Q348" s="111"/>
@@ -34780,7 +34808,7 @@
       <c r="E364" s="125"/>
       <c r="F364" s="125"/>
       <c r="G364" s="126" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H364" s="127"/>
       <c r="I364" s="127"/>
@@ -35051,7 +35079,7 @@
       </c>
       <c r="F369" s="147"/>
       <c r="G369" s="148" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H369" s="147"/>
       <c r="I369" s="147"/>
@@ -35105,7 +35133,7 @@
       <c r="E370" s="96"/>
       <c r="F370" s="147"/>
       <c r="G370" s="147" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H370" s="150"/>
       <c r="I370" s="147"/>
@@ -35374,7 +35402,7 @@
       <c r="H375" s="96"/>
       <c r="I375" s="96"/>
       <c r="J375" s="96" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K375" s="111"/>
       <c r="L375" s="111"/>
@@ -35428,7 +35456,7 @@
       <c r="H376" s="96"/>
       <c r="I376" s="96"/>
       <c r="J376" s="111" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K376" s="111" t="s">
         <v>180</v>
@@ -36130,7 +36158,7 @@
       <c r="F387" s="156"/>
       <c r="G387" s="120"/>
       <c r="H387" s="120" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I387" s="120"/>
       <c r="J387" s="118"/>
@@ -36339,7 +36367,7 @@
       <c r="E391" s="125"/>
       <c r="F391" s="125"/>
       <c r="G391" s="126" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H391" s="127"/>
       <c r="I391" s="127"/>
@@ -36611,7 +36639,7 @@
       </c>
       <c r="F396" s="89"/>
       <c r="G396" s="90" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H396" s="91"/>
       <c r="I396" s="91"/>
@@ -36665,7 +36693,7 @@
       <c r="E397" s="96"/>
       <c r="F397" s="97"/>
       <c r="G397" s="98" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H397" s="98"/>
       <c r="I397" s="98"/>
@@ -36777,7 +36805,7 @@
       <c r="E399" s="96"/>
       <c r="F399" s="104"/>
       <c r="G399" s="105" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H399" s="106"/>
       <c r="I399" s="106"/>
@@ -36889,13 +36917,13 @@
       <c r="K401" s="96"/>
       <c r="L401" s="110"/>
       <c r="M401" s="136" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="N401" s="136"/>
       <c r="O401" s="136"/>
       <c r="P401" s="136"/>
       <c r="Q401" s="193" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="R401" s="110"/>
       <c r="S401" s="110"/>
@@ -36944,10 +36972,10 @@
       <c r="J402" s="111"/>
       <c r="K402" s="111"/>
       <c r="L402" s="111" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="M402" s="136" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="N402" s="136"/>
       <c r="O402" s="136"/>
@@ -37002,19 +37030,19 @@
         <v>208</v>
       </c>
       <c r="L403" s="170" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="M403" s="170" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="N403" s="170" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="O403" s="170" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="P403" s="170" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q403" s="111"/>
       <c r="R403" s="111"/>
@@ -37805,7 +37833,7 @@
       <c r="E416" s="125"/>
       <c r="F416" s="125"/>
       <c r="G416" s="126" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H416" s="127"/>
       <c r="I416" s="127"/>
@@ -38219,8 +38247,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AU487"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G270" sqref="G270:P280"/>
+    <sheetView topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -38340,7 +38368,7 @@
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -38880,7 +38908,7 @@
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -39406,7 +39434,7 @@
       <c r="E41" s="16"/>
       <c r="F41" s="25"/>
       <c r="G41" s="364" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
@@ -39636,7 +39664,7 @@
       <c r="F48" s="25"/>
       <c r="G48" s="33"/>
       <c r="H48" s="362" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I48" s="410"/>
       <c r="J48" s="410"/>
@@ -39963,7 +39991,8 @@
       <c r="H58" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="I58" s="411">
+      <c r="I58" s="473">
+        <f>MIN(I65:I75)</f>
         <v>43794</v>
       </c>
       <c r="J58" s="34"/>
@@ -40553,7 +40582,7 @@
       <c r="F77" s="25"/>
       <c r="G77" s="33"/>
       <c r="H77" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I77" s="411">
         <v>43770</v>
@@ -40613,7 +40642,7 @@
       <c r="F79" s="25"/>
       <c r="G79" s="33"/>
       <c r="H79" s="34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I79" s="410">
         <v>15</v>
@@ -40672,7 +40701,7 @@
       <c r="E81" s="16"/>
       <c r="F81" s="25"/>
       <c r="G81" s="363" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I81" s="34"/>
       <c r="J81" s="34"/>
@@ -40702,7 +40731,7 @@
       <c r="F82" s="25"/>
       <c r="G82" s="33"/>
       <c r="H82" s="34" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I82" s="410">
         <v>7</v>
@@ -41197,7 +41226,7 @@
       <c r="F98" s="25"/>
       <c r="G98" s="33"/>
       <c r="H98" s="26" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I98" s="408">
         <v>1</v>
@@ -41485,7 +41514,7 @@
       </c>
       <c r="F107" s="12"/>
       <c r="G107" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
@@ -41517,7 +41546,7 @@
       <c r="G108" s="17"/>
       <c r="H108" s="12"/>
       <c r="I108" s="354" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J108" s="12"/>
       <c r="K108" s="12"/>
@@ -41547,7 +41576,7 @@
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
       <c r="I109" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J109" s="12"/>
       <c r="K109" s="12"/>
@@ -41634,14 +41663,14 @@
       <c r="F112" s="16"/>
       <c r="G112" s="16"/>
       <c r="H112" s="470" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I112" s="470"/>
       <c r="J112" s="470"/>
       <c r="K112" s="349"/>
       <c r="L112" s="366"/>
       <c r="M112" s="469" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="N112" s="469"/>
       <c r="O112" s="469"/>
@@ -42047,7 +42076,7 @@
       <c r="E122" s="16"/>
       <c r="F122" s="25"/>
       <c r="G122" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H122" s="412">
         <v>250</v>
@@ -42357,7 +42386,7 @@
       <c r="E129" s="16"/>
       <c r="F129" s="25"/>
       <c r="G129" s="26" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H129" s="412">
         <v>250</v>
@@ -42402,7 +42431,7 @@
       <c r="E130" s="16"/>
       <c r="F130" s="25"/>
       <c r="G130" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H130" s="412">
         <v>250</v>
@@ -42446,7 +42475,7 @@
       <c r="E131" s="16"/>
       <c r="F131" s="25"/>
       <c r="G131" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H131" s="412">
         <v>250</v>
@@ -42490,7 +42519,7 @@
       <c r="E132" s="16"/>
       <c r="F132" s="25"/>
       <c r="G132" s="26" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H132" s="412">
         <v>250</v>
@@ -42580,7 +42609,7 @@
       <c r="E134" s="16"/>
       <c r="F134" s="25"/>
       <c r="G134" s="26" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H134" s="412">
         <v>250</v>
@@ -42625,7 +42654,7 @@
       <c r="E135" s="16"/>
       <c r="F135" s="25"/>
       <c r="G135" s="26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H135" s="412">
         <v>250</v>
@@ -42670,7 +42699,7 @@
       <c r="E136" s="16"/>
       <c r="F136" s="25"/>
       <c r="G136" s="26" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H136" s="412">
         <v>250</v>
@@ -42715,7 +42744,7 @@
       <c r="E137" s="16"/>
       <c r="F137" s="25"/>
       <c r="G137" s="25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H137" s="412">
         <v>250</v>
@@ -42760,7 +42789,7 @@
       <c r="E138" s="16"/>
       <c r="F138" s="25"/>
       <c r="G138" s="25" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H138" s="412">
         <v>250</v>
@@ -42805,7 +42834,7 @@
       <c r="E139" s="16"/>
       <c r="F139" s="25"/>
       <c r="G139" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H139" s="412">
         <v>250</v>
@@ -43121,7 +43150,7 @@
       </c>
       <c r="F149" s="12"/>
       <c r="G149" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="H149" s="12"/>
       <c r="I149" s="12"/>
@@ -43183,7 +43212,7 @@
       </c>
       <c r="H151" s="12"/>
       <c r="I151" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J151" s="12"/>
       <c r="K151" s="12"/>
@@ -43471,7 +43500,7 @@
       <c r="E160" s="16"/>
       <c r="F160" s="25"/>
       <c r="G160" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H160" s="26" t="s">
         <v>74</v>
@@ -43749,14 +43778,14 @@
       </c>
       <c r="F168" s="12"/>
       <c r="G168" s="13" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H168" s="12"/>
       <c r="I168" s="12"/>
       <c r="J168" s="12"/>
       <c r="K168" s="12"/>
       <c r="L168" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="M168" s="12"/>
       <c r="N168" s="12"/>
@@ -43788,7 +43817,7 @@
       <c r="G169" s="17"/>
       <c r="H169" s="12"/>
       <c r="I169" s="368" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J169" s="417" t="b">
         <v>1</v>
@@ -43830,7 +43859,7 @@
       <c r="J170" s="12"/>
       <c r="K170" s="12"/>
       <c r="L170" s="32" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="M170" s="12"/>
       <c r="N170" s="12"/>
@@ -43867,7 +43896,7 @@
       <c r="J171" s="12"/>
       <c r="K171" s="12"/>
       <c r="L171" s="32" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="M171" s="12"/>
       <c r="N171" s="12"/>
@@ -43904,7 +43933,7 @@
       <c r="L172" s="366"/>
       <c r="M172" s="366"/>
       <c r="N172" s="369" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="O172" s="366"/>
       <c r="P172" s="366"/>
@@ -43934,7 +43963,7 @@
       <c r="G173" s="16"/>
       <c r="H173" s="16"/>
       <c r="I173" s="16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J173" s="16"/>
       <c r="K173" s="16"/>
@@ -43973,49 +44002,49 @@
       <c r="K174" s="16"/>
       <c r="L174" s="16"/>
       <c r="M174" s="366" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="N174" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="O174" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="P174" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q174" s="370" t="s">
         <v>477</v>
       </c>
-      <c r="O174" s="16" t="s">
+      <c r="R174" s="370" t="s">
         <v>477</v>
       </c>
-      <c r="P174" s="16" t="s">
+      <c r="S174" s="370" t="s">
         <v>477</v>
       </c>
-      <c r="Q174" s="370" t="s">
-        <v>479</v>
-      </c>
-      <c r="R174" s="370" t="s">
-        <v>479</v>
-      </c>
-      <c r="S174" s="370" t="s">
-        <v>479</v>
-      </c>
       <c r="T174" s="366" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="U174" s="366" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V174" s="366" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="W174" s="366" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="X174" s="366" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="Y174" s="366" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="Z174" s="366" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AA174" s="366" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="AB174" s="15"/>
       <c r="AC174" s="6"/>
@@ -44030,67 +44059,67 @@
       <c r="E175" s="16"/>
       <c r="F175" s="16"/>
       <c r="G175" s="22" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H175" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="I175" s="22" t="s">
+        <v>470</v>
+      </c>
+      <c r="J175" s="22" t="s">
+        <v>471</v>
+      </c>
+      <c r="K175" s="22" t="s">
+        <v>469</v>
+      </c>
+      <c r="L175" s="22" t="s">
+        <v>468</v>
+      </c>
+      <c r="M175" s="22" t="s">
         <v>474</v>
       </c>
-      <c r="I175" s="22" t="s">
-        <v>472</v>
-      </c>
-      <c r="J175" s="22" t="s">
-        <v>473</v>
-      </c>
-      <c r="K175" s="22" t="s">
-        <v>471</v>
-      </c>
-      <c r="L175" s="22" t="s">
-        <v>470</v>
-      </c>
-      <c r="M175" s="22" t="s">
-        <v>476</v>
-      </c>
       <c r="N175" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="O175" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="P175" s="22" t="s">
         <v>465</v>
       </c>
-      <c r="O175" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="P175" s="22" t="s">
-        <v>467</v>
-      </c>
       <c r="Q175" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="R175" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="S175" s="22" t="s">
         <v>451</v>
       </c>
-      <c r="R175" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="S175" s="22" t="s">
-        <v>453</v>
-      </c>
       <c r="T175" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="U175" s="23" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="V175" s="23" t="s">
         <v>73</v>
       </c>
       <c r="W175" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="X175" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="Y175" s="23" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="Z175" s="23" t="s">
         <v>73</v>
       </c>
       <c r="AA175" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AB175" s="15"/>
       <c r="AC175" s="6"/>
@@ -44184,7 +44213,7 @@
       <c r="E177" s="16"/>
       <c r="F177" s="25"/>
       <c r="G177" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H177" s="415" t="s">
         <v>23</v>
@@ -44266,7 +44295,7 @@
         <v>23</v>
       </c>
       <c r="H178" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I178" s="415" t="s">
         <v>23</v>
@@ -44342,10 +44371,10 @@
       <c r="E179" s="16"/>
       <c r="F179" s="25"/>
       <c r="G179" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H179" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I179" s="415" t="s">
         <v>91</v>
@@ -44421,10 +44450,10 @@
       <c r="E180" s="16"/>
       <c r="F180" s="25"/>
       <c r="G180" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H180" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I180" s="415" t="s">
         <v>92</v>
@@ -44500,10 +44529,10 @@
       <c r="E181" s="16"/>
       <c r="F181" s="25"/>
       <c r="G181" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H181" s="415" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I181" s="415" t="s">
         <v>92</v>
@@ -44881,7 +44910,7 @@
       </c>
       <c r="F191" s="12"/>
       <c r="G191" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H191" s="12"/>
       <c r="I191" s="12"/>
@@ -44941,7 +44970,7 @@
       <c r="G193" s="12"/>
       <c r="H193" s="12"/>
       <c r="I193" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="J193" s="12"/>
       <c r="K193" s="12"/>
@@ -45057,22 +45086,22 @@
       <c r="G197" s="16"/>
       <c r="H197" s="16"/>
       <c r="I197" s="16" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J197" s="16" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="K197" s="16" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L197" s="366" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="M197" s="366" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="N197" s="366" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="O197" s="16"/>
       <c r="P197" s="16"/>
@@ -45096,25 +45125,25 @@
       <c r="F198" s="16"/>
       <c r="G198" s="16"/>
       <c r="H198" s="16" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I198" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="J198" s="22" t="s">
+        <v>464</v>
+      </c>
+      <c r="K198" s="22" t="s">
         <v>465</v>
       </c>
-      <c r="J198" s="22" t="s">
-        <v>466</v>
-      </c>
-      <c r="K198" s="22" t="s">
-        <v>467</v>
-      </c>
       <c r="L198" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="M198" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="N198" s="22" t="s">
         <v>451</v>
-      </c>
-      <c r="M198" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="N198" s="22" t="s">
-        <v>453</v>
       </c>
       <c r="O198" s="22"/>
       <c r="P198" s="22"/>
@@ -45418,7 +45447,7 @@
       <c r="F206" s="25"/>
       <c r="G206" s="25"/>
       <c r="H206" s="25" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I206" s="412">
         <v>0</v>
@@ -45698,7 +45727,7 @@
       <c r="F213" s="25"/>
       <c r="G213" s="25"/>
       <c r="H213" s="26" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I213" s="412">
         <v>30</v>
@@ -45738,7 +45767,7 @@
       <c r="F214" s="25"/>
       <c r="G214" s="25"/>
       <c r="H214" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I214" s="412">
         <v>30</v>
@@ -45778,7 +45807,7 @@
       <c r="F215" s="25"/>
       <c r="G215" s="25"/>
       <c r="H215" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I215" s="412">
         <v>30</v>
@@ -45818,7 +45847,7 @@
       <c r="F216" s="25"/>
       <c r="G216" s="25"/>
       <c r="H216" s="26" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I216" s="412">
         <v>30</v>
@@ -45898,7 +45927,7 @@
       <c r="F218" s="25"/>
       <c r="G218" s="25"/>
       <c r="H218" s="26" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I218" s="412">
         <v>30</v>
@@ -45938,7 +45967,7 @@
       <c r="F219" s="25"/>
       <c r="G219" s="25"/>
       <c r="H219" s="26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I219" s="412">
         <v>30</v>
@@ -45978,7 +46007,7 @@
       <c r="F220" s="25"/>
       <c r="G220" s="25"/>
       <c r="H220" s="26" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I220" s="412">
         <v>30</v>
@@ -46018,7 +46047,7 @@
       <c r="F221" s="25"/>
       <c r="G221" s="25"/>
       <c r="H221" s="25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I221" s="412">
         <v>30</v>
@@ -46058,7 +46087,7 @@
       <c r="F222" s="25"/>
       <c r="G222" s="25"/>
       <c r="H222" s="25" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I222" s="412">
         <v>30</v>
@@ -46098,7 +46127,7 @@
       <c r="F223" s="25"/>
       <c r="G223" s="25"/>
       <c r="H223" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I223" s="412">
         <v>30</v>
@@ -46973,7 +47002,7 @@
       <c r="F249" s="32"/>
       <c r="H249" s="26"/>
       <c r="I249" s="26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J249" s="419">
         <v>0.06</v>
@@ -47328,7 +47357,7 @@
       </c>
       <c r="F261" s="12"/>
       <c r="G261" s="13" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H261" s="12"/>
       <c r="I261" s="12"/>
@@ -47891,7 +47920,7 @@
       <c r="F277" s="32"/>
       <c r="G277" s="221"/>
       <c r="H277" s="221" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I277" s="414">
         <v>0</v>
@@ -48251,7 +48280,7 @@
       </c>
       <c r="F288" s="12"/>
       <c r="G288" s="13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H288" s="12"/>
       <c r="I288" s="12"/>
@@ -48311,7 +48340,7 @@
       <c r="G290" s="12"/>
       <c r="H290" s="12"/>
       <c r="I290" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J290" s="12"/>
       <c r="K290" s="12"/>
@@ -48433,7 +48462,7 @@
       <c r="E294" s="16"/>
       <c r="F294" s="32"/>
       <c r="H294" s="372" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I294" s="417">
         <v>0</v>
@@ -48470,7 +48499,7 @@
       <c r="E295" s="16"/>
       <c r="F295" s="32"/>
       <c r="H295" s="373" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I295" s="417">
         <v>1</v>
@@ -48544,7 +48573,7 @@
       <c r="E297" s="16"/>
       <c r="F297" s="32"/>
       <c r="H297" s="373" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I297" s="417">
         <v>1</v>
@@ -49133,7 +49162,7 @@
       <c r="E316" s="16"/>
       <c r="F316" s="32"/>
       <c r="H316" s="372" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I316" s="418">
         <v>0.62</v>
@@ -49171,7 +49200,7 @@
       <c r="E317" s="16"/>
       <c r="F317" s="32"/>
       <c r="H317" s="373" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I317" s="418">
         <v>0.62</v>
@@ -49250,7 +49279,7 @@
       <c r="F319" s="32"/>
       <c r="G319" s="80"/>
       <c r="H319" s="373" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I319" s="418">
         <v>0.62</v>
@@ -49872,7 +49901,7 @@
       <c r="G339" s="26"/>
       <c r="H339" s="26"/>
       <c r="I339" s="33" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J339" s="418">
         <v>1</v>
@@ -49912,7 +49941,7 @@
       <c r="G340" s="26"/>
       <c r="H340" s="26"/>
       <c r="I340" s="33" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J340" s="418">
         <v>1</v>
@@ -49952,7 +49981,7 @@
       <c r="G341" s="26"/>
       <c r="H341" s="26"/>
       <c r="I341" s="33" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J341" s="418">
         <v>1</v>
@@ -49992,7 +50021,7 @@
       <c r="G342" s="26"/>
       <c r="H342" s="26"/>
       <c r="I342" s="33" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J342" s="418">
         <v>1</v>
@@ -50032,7 +50061,7 @@
       <c r="G343" s="26"/>
       <c r="H343" s="26"/>
       <c r="I343" s="33" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="J343" s="418">
         <v>1</v>
@@ -50072,7 +50101,7 @@
       <c r="G344" s="26"/>
       <c r="H344" s="26"/>
       <c r="I344" s="33" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J344" s="418">
         <v>1</v>
@@ -50315,7 +50344,7 @@
       </c>
       <c r="F352" s="12"/>
       <c r="G352" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H352" s="12"/>
       <c r="I352" s="12"/>
@@ -50346,7 +50375,7 @@
       <c r="F353" s="12"/>
       <c r="G353" s="17"/>
       <c r="H353" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I353" s="12"/>
       <c r="J353" s="12"/>
@@ -51193,7 +51222,7 @@
       </c>
       <c r="O380" s="22"/>
       <c r="P380" s="22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q380" s="23"/>
       <c r="R380" s="23"/>
@@ -51552,7 +51581,7 @@
       <c r="G389" s="48"/>
       <c r="H389" s="30"/>
       <c r="I389" s="26" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J389" s="425">
         <v>100</v>
@@ -51804,7 +51833,7 @@
       <c r="G395" s="49"/>
       <c r="H395" s="50"/>
       <c r="I395" s="70" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J395" s="425">
         <v>2</v>
@@ -51846,7 +51875,7 @@
       <c r="G396" s="49"/>
       <c r="H396" s="50"/>
       <c r="I396" s="70" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J396" s="425">
         <v>10</v>
@@ -51888,7 +51917,7 @@
       <c r="G397" s="49"/>
       <c r="H397" s="50"/>
       <c r="I397" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J397" s="425">
         <v>10</v>
@@ -51929,7 +51958,7 @@
       <c r="G398" s="49"/>
       <c r="H398" s="50"/>
       <c r="I398" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J398" s="425">
         <v>10</v>
@@ -52384,34 +52413,34 @@
         <v>39</v>
       </c>
       <c r="H413" s="52" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I413" s="52" t="s">
         <v>49</v>
       </c>
       <c r="J413" s="52" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K413" s="24" t="s">
         <v>50</v>
       </c>
       <c r="L413" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M413" s="24" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N413" s="24" t="s">
         <v>51</v>
       </c>
       <c r="O413" s="24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="P413" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q413" s="255" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="R413" s="52"/>
       <c r="S413" s="52"/>
@@ -52775,7 +52804,7 @@
       <c r="E422" s="16"/>
       <c r="F422" s="32"/>
       <c r="G422" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H422" s="428">
         <v>0</v>
@@ -53023,7 +53052,7 @@
       <c r="E428" s="16"/>
       <c r="F428" s="32"/>
       <c r="G428" s="253" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H428" s="428">
         <v>3000</v>
@@ -53064,7 +53093,7 @@
       <c r="E429" s="16"/>
       <c r="F429" s="32"/>
       <c r="G429" s="253" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H429" s="428">
         <v>3000</v>
@@ -53105,7 +53134,7 @@
       <c r="E430" s="16"/>
       <c r="F430" s="32"/>
       <c r="G430" s="254" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H430" s="428">
         <v>3000</v>
@@ -53146,7 +53175,7 @@
       <c r="E431" s="16"/>
       <c r="F431" s="32"/>
       <c r="G431" s="254" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H431" s="428">
         <v>3000</v>
@@ -55028,57 +55057,57 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1" t="s">
+        <v>461</v>
+      </c>
+      <c r="F1" s="365" t="s">
+        <v>457</v>
+      </c>
+      <c r="I1" t="s">
+        <v>449</v>
+      </c>
+      <c r="J1" t="s">
+        <v>449</v>
+      </c>
+      <c r="K1" t="s">
         <v>462</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>462</v>
-      </c>
-      <c r="D1" t="s">
-        <v>463</v>
-      </c>
-      <c r="E1" t="s">
-        <v>463</v>
-      </c>
-      <c r="F1" s="365" t="s">
-        <v>459</v>
-      </c>
-      <c r="I1" t="s">
-        <v>451</v>
-      </c>
-      <c r="J1" t="s">
-        <v>451</v>
-      </c>
-      <c r="K1" t="s">
-        <v>464</v>
-      </c>
-      <c r="L1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F2" s="365" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J2" t="s">
         <v>88</v>
       </c>
       <c r="K2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="L2" t="s">
         <v>88</v>
@@ -55086,7 +55115,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -55101,7 +55130,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -55118,7 +55147,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -55133,7 +55162,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -55150,7 +55179,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -55165,7 +55194,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -55182,7 +55211,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -55197,7 +55226,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -55214,7 +55243,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -55229,7 +55258,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -55246,7 +55275,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -55261,7 +55290,7 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -55278,7 +55307,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -55293,7 +55322,7 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -55426,7 +55455,7 @@
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -55561,15 +55590,15 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="22" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K9" s="22"/>
       <c r="L9" s="22" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="23"/>
@@ -55618,7 +55647,7 @@
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H11" s="436">
         <v>1</v>
@@ -55652,7 +55681,7 @@
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="33" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H12" s="436">
         <v>1</v>
@@ -55712,7 +55741,7 @@
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
       <c r="G14" s="33" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H14" s="245"/>
       <c r="I14" s="245"/>
@@ -55742,7 +55771,7 @@
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="G15" s="33" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H15" s="245"/>
       <c r="I15" s="245"/>
@@ -55983,7 +56012,7 @@
       <c r="C24" s="11"/>
       <c r="D24" s="12"/>
       <c r="E24" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -56118,15 +56147,15 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="22" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I29" s="22"/>
       <c r="J29" s="22" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="M29" s="22"/>
       <c r="N29" s="23"/>
@@ -56175,7 +56204,7 @@
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
       <c r="G31" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H31" s="245"/>
       <c r="I31" s="245"/>
@@ -56231,7 +56260,7 @@
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
       <c r="G33" s="33" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H33" s="411">
         <v>43511</v>
@@ -56289,7 +56318,7 @@
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
       <c r="G35" s="33" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H35" s="436">
         <v>28</v>
@@ -56506,7 +56535,7 @@
       <c r="C43" s="11"/>
       <c r="D43" s="12"/>
       <c r="E43" s="13" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
@@ -56641,13 +56670,13 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="22" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I48" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="J48" s="22" t="s">
         <v>337</v>
-      </c>
-      <c r="J48" s="22" t="s">
-        <v>339</v>
       </c>
       <c r="K48" s="22"/>
       <c r="L48" s="22"/>
@@ -56672,7 +56701,7 @@
       <c r="E49" s="26"/>
       <c r="F49" s="26"/>
       <c r="G49" s="28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H49" s="436">
         <v>9</v>
@@ -56706,7 +56735,7 @@
       <c r="E50" s="26"/>
       <c r="F50" s="26"/>
       <c r="G50" s="257" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H50" s="436">
         <v>4.5</v>
@@ -56740,7 +56769,7 @@
       <c r="E51" s="30"/>
       <c r="F51" s="30"/>
       <c r="G51" s="258" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H51" s="436">
         <v>10</v>
@@ -56774,7 +56803,7 @@
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
       <c r="G52" s="257" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H52" s="422">
         <v>9</v>
@@ -56834,7 +56863,7 @@
       <c r="E54" s="33"/>
       <c r="F54" s="33"/>
       <c r="G54" s="437" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H54" s="245"/>
       <c r="I54" s="245"/>
@@ -56864,10 +56893,10 @@
       <c r="G55" s="239"/>
       <c r="H55" s="245"/>
       <c r="I55" s="257" t="s">
+        <v>335</v>
+      </c>
+      <c r="J55" s="257" t="s">
         <v>337</v>
-      </c>
-      <c r="J55" s="257" t="s">
-        <v>339</v>
       </c>
       <c r="K55" s="245"/>
       <c r="L55" s="245"/>
@@ -56892,7 +56921,7 @@
       <c r="E56" s="33"/>
       <c r="F56" s="33"/>
       <c r="H56" s="260" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I56" s="436">
         <v>7.0000000000000007E-2</v>
@@ -56923,7 +56952,7 @@
       <c r="E57" s="33"/>
       <c r="F57" s="33"/>
       <c r="H57" s="261" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I57" s="436">
         <v>0.02</v>
@@ -57113,7 +57142,7 @@
       <c r="C64" s="11"/>
       <c r="D64" s="12"/>
       <c r="E64" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
@@ -57145,7 +57174,7 @@
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
       <c r="I65" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J65" s="12"/>
       <c r="K65" s="12"/>
@@ -57222,27 +57251,27 @@
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
       <c r="F68" s="471" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G68" s="472"/>
       <c r="H68" s="22"/>
       <c r="I68" s="22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J68" s="22"/>
       <c r="K68" s="22"/>
       <c r="L68" s="22" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="M68" s="22"/>
       <c r="N68" s="22"/>
       <c r="O68" s="22" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="P68" s="23"/>
       <c r="Q68" s="21"/>
       <c r="R68" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="S68" s="21"/>
       <c r="T68" s="21"/>
@@ -57261,32 +57290,32 @@
         <v>117</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H69" s="22"/>
       <c r="I69" s="22" t="s">
         <v>117</v>
       </c>
       <c r="J69" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K69" s="22"/>
       <c r="L69" s="22" t="s">
         <v>117</v>
       </c>
       <c r="M69" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N69" s="23"/>
       <c r="O69" s="22" t="s">
         <v>117</v>
       </c>
       <c r="P69" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q69" s="21"/>
       <c r="R69" s="21" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="S69" s="21"/>
       <c r="T69" s="21"/>
@@ -57947,7 +57976,7 @@
       <c r="C92" s="11"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
@@ -58002,7 +58031,7 @@
       <c r="D94" s="16"/>
       <c r="E94" s="16"/>
       <c r="F94" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G94" s="21"/>
       <c r="H94" s="21"/>
@@ -58013,7 +58042,7 @@
       <c r="M94" s="21"/>
       <c r="N94" s="21"/>
       <c r="O94" s="21" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="P94" s="21"/>
       <c r="Q94" s="21"/>
@@ -58059,27 +58088,27 @@
       <c r="E96" s="471"/>
       <c r="F96" s="472"/>
       <c r="G96" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H96" s="22"/>
       <c r="I96" s="22"/>
       <c r="J96" s="136" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="K96" s="136"/>
       <c r="L96" s="22"/>
       <c r="M96" s="136" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N96" s="136"/>
       <c r="O96" s="22"/>
       <c r="P96" s="441" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="Q96" s="199"/>
       <c r="R96" s="21"/>
       <c r="S96" s="199" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="T96" s="199"/>
       <c r="U96" s="15"/>
@@ -58093,42 +58122,42 @@
       <c r="C97" s="16"/>
       <c r="D97" s="16"/>
       <c r="E97" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F97" s="16"/>
       <c r="G97" s="22" t="s">
         <v>126</v>
       </c>
       <c r="H97" s="22" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I97" s="22"/>
       <c r="J97" s="22" t="s">
         <v>117</v>
       </c>
       <c r="K97" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="L97" s="22"/>
       <c r="M97" s="22" t="s">
         <v>117</v>
       </c>
       <c r="N97" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="O97" s="22"/>
       <c r="P97" s="22" t="s">
         <v>117</v>
       </c>
       <c r="Q97" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="R97" s="22"/>
       <c r="S97" s="22" t="s">
         <v>117</v>
       </c>
       <c r="T97" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="U97" s="15"/>
       <c r="V97" s="6"/>
@@ -58309,7 +58338,7 @@
       <c r="E102" s="267"/>
       <c r="F102" s="76"/>
       <c r="G102" s="76" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H102" s="440">
         <v>1.2</v>

</xml_diff>

<commit_message>
change fp set from int to 'FP0' and drop space in season set Fix 2 for pyomo run (diff dict function)
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7E6133-A5AB-4CC6-86D9-BC9DDA29EB14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A91E87-16E8-433F-9C87-DD0C1ACF0861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -2954,7 +2954,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="545">
   <si>
     <t>«</t>
   </si>
@@ -4438,9 +4438,6 @@
     <t>Season Types</t>
   </si>
   <si>
-    <t>season 1</t>
-  </si>
-  <si>
     <t>probability</t>
   </si>
   <si>
@@ -4448,9 +4445,6 @@
   </si>
   <si>
     <t>included</t>
-  </si>
-  <si>
-    <t>Do you wan steady state model?</t>
   </si>
   <si>
     <t>Y</t>
@@ -4579,6 +4573,45 @@
   </si>
   <si>
     <t>lmu0</t>
+  </si>
+  <si>
+    <t>FP0</t>
+  </si>
+  <si>
+    <t>FP1</t>
+  </si>
+  <si>
+    <t>FP2</t>
+  </si>
+  <si>
+    <t>FP3</t>
+  </si>
+  <si>
+    <t>FP4</t>
+  </si>
+  <si>
+    <t>FP5</t>
+  </si>
+  <si>
+    <t>FP6</t>
+  </si>
+  <si>
+    <t>FP7</t>
+  </si>
+  <si>
+    <t>FP8</t>
+  </si>
+  <si>
+    <t>FP9</t>
+  </si>
+  <si>
+    <t>FP10</t>
+  </si>
+  <si>
+    <t>Do you want steady state model?</t>
+  </si>
+  <si>
+    <t>season0</t>
   </si>
 </sst>
 </file>
@@ -7416,7 +7449,7 @@
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -7732,7 +7765,7 @@
       <c r="G29" s="241"/>
       <c r="H29" s="241"/>
       <c r="I29" s="241" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="J29" s="442">
         <v>1</v>
@@ -8540,7 +8573,7 @@
         <v>125</v>
       </c>
       <c r="H58" s="242" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I58" s="239"/>
       <c r="J58" s="240"/>
@@ -9587,7 +9620,7 @@
       <c r="K94" s="53"/>
       <c r="L94" s="53"/>
       <c r="M94" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N94" s="33"/>
       <c r="O94" s="55"/>
@@ -9961,7 +9994,7 @@
       <c r="K105" s="53"/>
       <c r="L105" s="53"/>
       <c r="M105" s="33" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="N105" s="33"/>
       <c r="O105" s="55"/>
@@ -10749,7 +10782,7 @@
       <c r="E127" s="16"/>
       <c r="F127" s="25"/>
       <c r="G127" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H127" s="33"/>
       <c r="I127" s="54"/>
@@ -12285,8 +12318,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12314,7 +12347,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="G4" s="74" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H4" s="378">
         <v>0</v>
@@ -12532,7 +12565,7 @@
       <c r="H19" s="281"/>
       <c r="I19" s="281"/>
       <c r="J19" s="281" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K19" s="281"/>
       <c r="L19" s="281"/>
@@ -12676,14 +12709,14 @@
       <c r="H24" s="285"/>
       <c r="I24" s="285"/>
       <c r="J24" s="291" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K24" s="291" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="L24" s="292"/>
       <c r="M24" s="374" t="s">
-        <v>494</v>
+        <v>543</v>
       </c>
       <c r="N24" s="292"/>
       <c r="O24" s="292"/>
@@ -12709,7 +12742,7 @@
       <c r="G25" s="74"/>
       <c r="H25" s="297"/>
       <c r="I25" s="308" t="s">
-        <v>490</v>
+        <v>544</v>
       </c>
       <c r="J25" s="379">
         <v>1</v>
@@ -13905,7 +13938,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13932,8 +13965,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="74">
-        <v>0</v>
+      <c r="A4" s="74" t="s">
+        <v>532</v>
       </c>
       <c r="B4" s="386">
         <v>43579</v>
@@ -13944,8 +13977,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="74">
-        <v>1</v>
+      <c r="A5" s="76" t="s">
+        <v>533</v>
       </c>
       <c r="B5" s="386">
         <v>43600</v>
@@ -13955,12 +13988,12 @@
         <v>28</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="74">
-        <v>2</v>
+      <c r="A6" s="76" t="s">
+        <v>534</v>
       </c>
       <c r="B6" s="386">
         <v>43628</v>
@@ -13971,8 +14004,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="74">
-        <v>3</v>
+      <c r="A7" s="76" t="s">
+        <v>535</v>
       </c>
       <c r="B7" s="386">
         <v>43684</v>
@@ -13983,8 +14016,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="74">
-        <v>4</v>
+      <c r="A8" s="76" t="s">
+        <v>536</v>
       </c>
       <c r="B8" s="386">
         <v>43733</v>
@@ -13995,8 +14028,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="74">
-        <v>5</v>
+      <c r="A9" s="76" t="s">
+        <v>537</v>
       </c>
       <c r="B9" s="386">
         <v>43768</v>
@@ -14007,8 +14040,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="74">
-        <v>6</v>
+      <c r="A10" s="76" t="s">
+        <v>538</v>
       </c>
       <c r="B10" s="386">
         <v>43796</v>
@@ -14019,8 +14052,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="74">
-        <v>7</v>
+      <c r="A11" s="76" t="s">
+        <v>539</v>
       </c>
       <c r="B11" s="386">
         <v>43852</v>
@@ -14031,8 +14064,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="74">
-        <v>8</v>
+      <c r="A12" s="76" t="s">
+        <v>540</v>
       </c>
       <c r="B12" s="386">
         <v>43902</v>
@@ -14043,8 +14076,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="74">
-        <v>9</v>
+      <c r="A13" s="76" t="s">
+        <v>541</v>
       </c>
       <c r="B13" s="386">
         <v>43930</v>
@@ -14055,8 +14088,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="74">
-        <v>10</v>
+      <c r="A14" s="76" t="s">
+        <v>542</v>
       </c>
       <c r="B14" s="386">
         <v>43945</v>
@@ -14066,6 +14099,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -17771,7 +17805,7 @@
       <c r="F50" s="114"/>
       <c r="G50" s="116"/>
       <c r="H50" s="120" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I50" s="120"/>
       <c r="J50" s="118"/>
@@ -17799,7 +17833,7 @@
       <c r="F51" s="114"/>
       <c r="G51" s="116"/>
       <c r="H51" s="468" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I51" s="469"/>
       <c r="J51" s="469"/>
@@ -19043,7 +19077,7 @@
       <c r="J87" s="111"/>
       <c r="K87" s="111"/>
       <c r="L87" s="111" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="M87" s="136" t="s">
         <v>182</v>
@@ -19102,22 +19136,22 @@
         <v>42</v>
       </c>
       <c r="M88" s="111" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="N88" s="111" t="s">
+        <v>523</v>
+      </c>
+      <c r="O88" s="111" t="s">
         <v>525</v>
       </c>
-      <c r="O88" s="111" t="s">
+      <c r="P88" s="111" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q88" s="111" t="s">
         <v>527</v>
       </c>
-      <c r="P88" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="Q88" s="111" t="s">
+      <c r="R88" s="111" t="s">
         <v>529</v>
-      </c>
-      <c r="R88" s="111" t="s">
-        <v>531</v>
       </c>
       <c r="S88" s="111"/>
       <c r="T88" s="111"/>
@@ -20861,7 +20895,7 @@
       <c r="J120" s="179"/>
       <c r="K120" s="179"/>
       <c r="L120" s="180" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="M120" s="181" t="s">
         <v>209</v>
@@ -20920,22 +20954,22 @@
         <v>42</v>
       </c>
       <c r="M121" s="183" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="N121" s="183" t="s">
+        <v>523</v>
+      </c>
+      <c r="O121" s="183" t="s">
         <v>525</v>
       </c>
-      <c r="O121" s="183" t="s">
+      <c r="P121" s="183" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q121" s="183" t="s">
         <v>527</v>
       </c>
-      <c r="P121" s="183" t="s">
-        <v>528</v>
-      </c>
-      <c r="Q121" s="183" t="s">
+      <c r="R121" s="183" t="s">
         <v>529</v>
-      </c>
-      <c r="R121" s="183" t="s">
-        <v>531</v>
       </c>
       <c r="S121" s="123"/>
       <c r="T121" s="123"/>
@@ -22812,7 +22846,7 @@
       <c r="U162" s="111"/>
       <c r="V162" s="111"/>
       <c r="W162" s="136" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="X162" s="136"/>
       <c r="Y162" s="111"/>
@@ -22860,36 +22894,36 @@
       <c r="I163" s="111"/>
       <c r="J163" s="111"/>
       <c r="K163" s="111" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="L163" s="111" t="s">
+        <v>523</v>
+      </c>
+      <c r="M163" s="111" t="s">
         <v>525</v>
       </c>
-      <c r="M163" s="111" t="s">
+      <c r="N163" s="111" t="s">
+        <v>526</v>
+      </c>
+      <c r="O163" s="111" t="s">
         <v>527</v>
-      </c>
-      <c r="N163" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="O163" s="111" t="s">
-        <v>529</v>
       </c>
       <c r="P163" s="111"/>
       <c r="Q163" s="111"/>
       <c r="R163" s="111" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="S163" s="111" t="s">
+        <v>523</v>
+      </c>
+      <c r="T163" s="111" t="s">
         <v>525</v>
       </c>
-      <c r="T163" s="111" t="s">
+      <c r="U163" s="111" t="s">
+        <v>526</v>
+      </c>
+      <c r="V163" s="111" t="s">
         <v>527</v>
-      </c>
-      <c r="U163" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="V163" s="111" t="s">
-        <v>529</v>
       </c>
       <c r="W163" s="111"/>
       <c r="X163" s="111"/>
@@ -22937,7 +22971,7 @@
       <c r="H164" s="116"/>
       <c r="I164" s="139"/>
       <c r="J164" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K164" s="448">
         <f>K188/2</f>
@@ -22961,7 +22995,7 @@
       </c>
       <c r="P164" s="116"/>
       <c r="Q164" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="R164" s="3">
         <f t="shared" ref="R164:V165" si="1">R188*0.6</f>
@@ -24625,7 +24659,7 @@
       <c r="U186" s="111"/>
       <c r="V186" s="111"/>
       <c r="W186" s="136" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="X186" s="136"/>
       <c r="Y186" s="111"/>
@@ -24673,42 +24707,42 @@
       <c r="I187" s="111"/>
       <c r="J187" s="111"/>
       <c r="K187" s="111" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="L187" s="111" t="s">
+        <v>523</v>
+      </c>
+      <c r="M187" s="111" t="s">
         <v>525</v>
       </c>
-      <c r="M187" s="111" t="s">
+      <c r="N187" s="111" t="s">
+        <v>526</v>
+      </c>
+      <c r="O187" s="111" t="s">
         <v>527</v>
-      </c>
-      <c r="N187" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="O187" s="111" t="s">
-        <v>529</v>
       </c>
       <c r="P187" s="111"/>
       <c r="Q187" s="111"/>
       <c r="R187" s="111" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="S187" s="111" t="s">
+        <v>523</v>
+      </c>
+      <c r="T187" s="111" t="s">
         <v>525</v>
       </c>
-      <c r="T187" s="111" t="s">
+      <c r="U187" s="111" t="s">
+        <v>526</v>
+      </c>
+      <c r="V187" s="111" t="s">
         <v>527</v>
       </c>
-      <c r="U187" s="111" t="s">
-        <v>528</v>
-      </c>
-      <c r="V187" s="111" t="s">
-        <v>529</v>
-      </c>
       <c r="W187" s="111" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="X187" s="111" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="Y187" s="111"/>
       <c r="Z187" s="111"/>
@@ -24754,7 +24788,7 @@
       <c r="H188" s="116"/>
       <c r="I188" s="139"/>
       <c r="J188" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K188" s="450">
         <v>200</v>
@@ -24774,7 +24808,7 @@
       </c>
       <c r="P188" s="116"/>
       <c r="Q188" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="R188" s="3">
         <f>0.55*$V188*(K188/$O188)</f>
@@ -24990,7 +25024,7 @@
         <v>50</v>
       </c>
       <c r="Y190" s="116" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="Z190" s="116"/>
       <c r="AA190" s="116"/>
@@ -26577,7 +26611,7 @@
       <c r="G214" s="116"/>
       <c r="H214" s="116"/>
       <c r="I214" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J214" s="116"/>
       <c r="K214" s="134">
@@ -28385,7 +28419,7 @@
       <c r="G246" s="116"/>
       <c r="H246" s="116"/>
       <c r="I246" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J246" s="116"/>
       <c r="K246" s="200">
@@ -29662,7 +29696,7 @@
         <v>200</v>
       </c>
       <c r="K268" s="170" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="L268" s="170" t="s">
         <v>66</v>
@@ -29734,7 +29768,7 @@
       <c r="H269" s="116"/>
       <c r="I269" s="116"/>
       <c r="J269" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K269" s="133">
         <v>0.81</v>
@@ -31420,7 +31454,7 @@
         <v>0.05</v>
       </c>
       <c r="I295" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J295" s="116"/>
       <c r="K295" s="452">
@@ -32867,10 +32901,10 @@
       <c r="J324" s="224"/>
       <c r="K324" s="225"/>
       <c r="L324" s="225" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="M324" s="142" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="N324" s="142" t="s">
         <v>66</v>
@@ -32906,7 +32940,7 @@
         <v>276</v>
       </c>
       <c r="L325" s="139" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="M325" s="451">
         <v>5.5</v>
@@ -34138,7 +34172,7 @@
       <c r="F353" s="156"/>
       <c r="G353" s="120"/>
       <c r="H353" s="229" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="I353" s="120"/>
       <c r="J353" s="133">
@@ -35526,7 +35560,7 @@
         <v>293</v>
       </c>
       <c r="K378" s="111" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="L378" s="111" t="s">
         <v>66</v>
@@ -35587,7 +35621,7 @@
       <c r="H379" s="120"/>
       <c r="I379" s="120"/>
       <c r="J379" s="229" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K379" s="137">
         <v>100</v>
@@ -36760,7 +36794,7 @@
       <c r="E399" s="96"/>
       <c r="F399" s="97"/>
       <c r="G399" s="98" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H399" s="98"/>
       <c r="I399" s="98"/>
@@ -36990,7 +37024,7 @@
       <c r="O403" s="136"/>
       <c r="P403" s="136"/>
       <c r="Q403" s="193" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="R403" s="110"/>
       <c r="S403" s="110"/>
@@ -37042,7 +37076,7 @@
         <v>296</v>
       </c>
       <c r="M404" s="136" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="N404" s="136"/>
       <c r="O404" s="136"/>
@@ -37103,10 +37137,10 @@
         <v>262</v>
       </c>
       <c r="N405" s="170" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="O405" s="170" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="P405" s="170" t="s">
         <v>261</v>
@@ -37158,7 +37192,7 @@
       <c r="I406" s="179"/>
       <c r="J406" s="179"/>
       <c r="K406" s="208" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="L406" s="404">
         <v>0.5</v>
@@ -38436,7 +38470,7 @@
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -41257,7 +41291,7 @@
       <c r="G97" s="16"/>
       <c r="H97" s="16"/>
       <c r="I97" s="22" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J97" s="22" t="s">
         <v>66</v>
@@ -43424,7 +43458,7 @@
       <c r="G156" s="16"/>
       <c r="H156" s="16"/>
       <c r="I156" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J156" s="291" t="s">
         <v>66</v>
@@ -43532,7 +43566,7 @@
       <c r="G159" s="26"/>
       <c r="H159" s="267"/>
       <c r="I159" s="256" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J159" s="256" t="s">
         <v>66</v>
@@ -43853,7 +43887,7 @@
       <c r="J168" s="12"/>
       <c r="K168" s="12"/>
       <c r="L168" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="M168" s="12"/>
       <c r="N168" s="12"/>
@@ -43927,7 +43961,7 @@
       <c r="J170" s="12"/>
       <c r="K170" s="12"/>
       <c r="L170" s="32" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="M170" s="12"/>
       <c r="N170" s="12"/>
@@ -43964,7 +43998,7 @@
       <c r="J171" s="12"/>
       <c r="K171" s="12"/>
       <c r="L171" s="32" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="M171" s="12"/>
       <c r="N171" s="12"/>
@@ -44281,7 +44315,7 @@
       <c r="E177" s="16"/>
       <c r="F177" s="25"/>
       <c r="G177" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H177" s="414" t="s">
         <v>23</v>
@@ -44363,7 +44397,7 @@
         <v>23</v>
       </c>
       <c r="H178" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I178" s="414" t="s">
         <v>23</v>
@@ -44439,10 +44473,10 @@
       <c r="E179" s="16"/>
       <c r="F179" s="25"/>
       <c r="G179" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H179" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I179" s="414" t="s">
         <v>90</v>
@@ -44518,10 +44552,10 @@
       <c r="E180" s="16"/>
       <c r="F180" s="25"/>
       <c r="G180" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H180" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I180" s="414" t="s">
         <v>91</v>
@@ -44597,10 +44631,10 @@
       <c r="E181" s="16"/>
       <c r="F181" s="25"/>
       <c r="G181" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H181" s="414" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I181" s="414" t="s">
         <v>91</v>
@@ -45038,7 +45072,7 @@
       <c r="G193" s="12"/>
       <c r="H193" s="12"/>
       <c r="I193" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="J193" s="12"/>
       <c r="K193" s="12"/>
@@ -46734,7 +46768,7 @@
       <c r="H240" s="16"/>
       <c r="I240" s="16"/>
       <c r="J240" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K240" s="291" t="s">
         <v>66</v>
@@ -47425,7 +47459,7 @@
       </c>
       <c r="F261" s="12"/>
       <c r="G261" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H261" s="12"/>
       <c r="I261" s="12"/>
@@ -47631,7 +47665,7 @@
       <c r="G268" s="16"/>
       <c r="H268" s="16"/>
       <c r="I268" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J268" s="291" t="s">
         <v>66</v>
@@ -49194,7 +49228,7 @@
       <c r="G315" s="16"/>
       <c r="H315" s="16"/>
       <c r="I315" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J315" s="291" t="s">
         <v>66</v>
@@ -49932,7 +49966,7 @@
       <c r="H338" s="16"/>
       <c r="I338" s="16"/>
       <c r="J338" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K338" s="291" t="s">
         <v>66</v>
@@ -51274,7 +51308,7 @@
       <c r="H380" s="471"/>
       <c r="I380" s="16"/>
       <c r="J380" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K380" s="291" t="s">
         <v>66</v>
@@ -54519,7 +54553,7 @@
       <c r="H473" s="16"/>
       <c r="I473" s="16"/>
       <c r="J473" s="291" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K473" s="291" t="s">
         <v>66</v>
@@ -56931,7 +56965,7 @@
       <c r="E54" s="33"/>
       <c r="F54" s="33"/>
       <c r="G54" s="436" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H54" s="244"/>
       <c r="I54" s="244"/>
@@ -57329,7 +57363,7 @@
       <c r="J68" s="22"/>
       <c r="K68" s="22"/>
       <c r="L68" s="22" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="M68" s="22"/>
       <c r="N68" s="22"/>
@@ -58110,7 +58144,7 @@
       <c r="M94" s="21"/>
       <c r="N94" s="21"/>
       <c r="O94" s="21" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="P94" s="21"/>
       <c r="Q94" s="21"/>
@@ -58161,22 +58195,22 @@
       <c r="H96" s="22"/>
       <c r="I96" s="22"/>
       <c r="J96" s="136" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K96" s="136"/>
       <c r="L96" s="22"/>
       <c r="M96" s="136" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="N96" s="136"/>
       <c r="O96" s="22"/>
       <c r="P96" s="440" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="Q96" s="199"/>
       <c r="R96" s="21"/>
       <c r="S96" s="199" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="T96" s="199"/>
       <c r="U96" s="15"/>
@@ -58977,7 +59011,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="74" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B18" s="378">
         <v>1.3</v>
@@ -59023,7 +59057,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="76" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B25" s="378">
         <v>1.2</v>
@@ -59069,7 +59103,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="76" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B32" s="378">
         <v>1</v>

</xml_diff>

<commit_message>
constrain carryover Finance small fix exp1 fix dry pas constraint
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A91E87-16E8-433F-9C87-DD0C1ACF0861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54760EAF-F97A-4006-B2DF-DC1D9DBDE926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <definedName name="approx_hay_yield" localSheetId="8">Mach!$B$42</definedName>
     <definedName name="arable" localSheetId="5">Crop!$H$97:$M$98</definedName>
     <definedName name="ave_pad_distance" localSheetId="8">Mach!$B$7</definedName>
+    <definedName name="bank_bal_start">Finance!$B$4</definedName>
     <definedName name="bas">Labour!$L$69:$M$73</definedName>
     <definedName name="BaseLevelInput" localSheetId="4">Annual!$K$214:$K$223</definedName>
     <definedName name="chem" localSheetId="5">Crop!$N$175:$S$181</definedName>
@@ -2954,7 +2955,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="546">
   <si>
     <t>«</t>
   </si>
@@ -4613,6 +4614,9 @@
   <si>
     <t>season0</t>
   </si>
+  <si>
+    <t>Bank balance at beginning of year</t>
+  </si>
 </sst>
 </file>
 
@@ -5238,7 +5242,7 @@
     <xf numFmtId="0" fontId="23" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="476">
+  <cellXfs count="477">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -6387,6 +6391,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="4" applyBorder="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Calculations" xfId="6" xr:uid="{449B9FA0-BCFF-41FE-A9C5-7F4DFD2D1D3B}"/>
@@ -12288,10 +12295,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17698FFE-A6A0-4C30-BDC9-58F80A4FAF68}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12308,6 +12315,14 @@
         <v>1500000</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="72" t="s">
+        <v>545</v>
+      </c>
+      <c r="B4" s="476">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12318,7 +12333,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -38349,7 +38364,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AU487"/>
   <sheetViews>
-    <sheetView topLeftCell="A445" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J473" sqref="J473:N473"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reporting and survival (not working)
</commit_message>
<xml_diff>
--- a/Property.xlsx
+++ b/Property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783B708-82A1-4CF3-A0AA-B6FA3CBDD0D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4677C5-022C-4B2D-A923-BB38889BEA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{A2ED2E73-F223-47EC-9041-EDA3E1B5327D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="4" r:id="rId1"/>
@@ -24,10 +24,11 @@
     <sheet name="Mach" sheetId="2" r:id="rId9"/>
     <sheet name="Stubble" sheetId="6" r:id="rId10"/>
     <sheet name="Finance" sheetId="3" r:id="rId11"/>
+    <sheet name="Report Settings" sheetId="13" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Annual!$G$139:$O$149</definedName>
@@ -96,6 +97,8 @@
     <definedName name="hay_making_date" localSheetId="5">Crop!$I$77</definedName>
     <definedName name="hay_making_len" localSheetId="5">Crop!$I$79</definedName>
     <definedName name="i_hf">Stubble!$J$29</definedName>
+    <definedName name="i_store_fec_rep">'Report Settings'!$J$18</definedName>
+    <definedName name="i_store_lw_rep">'Report Settings'!$G$18</definedName>
     <definedName name="initial_fungus" localSheetId="5">'[2]Initial conditions'!$M$12:$O$12</definedName>
     <definedName name="initial_nutrients">'[2]Initial conditions'!$R$12</definedName>
     <definedName name="initial_weed" localSheetId="5">'[2]Initial conditions'!$H$11:$J$13</definedName>
@@ -179,10 +182,18 @@
     <definedName name="yield_penalty" localSheetId="5">Crop!$H$43:$J$55</definedName>
     <definedName name="yields" localSheetId="5">Crop!$M$200:$M$205</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2973,7 +2984,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="554">
   <si>
     <t>«</t>
   </si>
@@ -4641,6 +4652,24 @@
   <si>
     <t>inf</t>
   </si>
+  <si>
+    <t>Control variable to be stored for reporting</t>
+  </si>
+  <si>
+    <t>Some arrays used for reporting are vary big so the default is not to store them. This is the default settings which can be overwritten using sensitivity values</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>store lw patterns</t>
+  </si>
+  <si>
+    <t>FEC</t>
+  </si>
+  <si>
+    <t>store fec patterns</t>
+  </si>
 </sst>
 </file>
 
@@ -5279,7 +5308,7 @@
     <xf numFmtId="0" fontId="23" fillId="18" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="477">
+  <cellXfs count="480">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -6370,6 +6399,10 @@
     <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="4" applyBorder="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="14" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -6430,6 +6463,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -7379,7 +7415,7 @@
   <dimension ref="A2:Z160"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="A35" sqref="A35:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -12130,12 +12166,896 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65171DF4-3688-4166-9603-E4B261BE1A52}">
+  <dimension ref="A1:Z31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="274"/>
+      <c r="B1" s="275"/>
+      <c r="C1" s="275"/>
+      <c r="D1" s="275"/>
+      <c r="E1" s="275"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="276"/>
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="276"/>
+      <c r="K1" s="276"/>
+      <c r="L1" s="276"/>
+      <c r="M1" s="276"/>
+      <c r="N1" s="276"/>
+      <c r="O1" s="276"/>
+      <c r="P1" s="276"/>
+      <c r="Q1" s="276"/>
+      <c r="R1" s="276"/>
+      <c r="S1" s="276"/>
+      <c r="T1" s="276"/>
+      <c r="U1" s="276"/>
+      <c r="V1" s="276"/>
+      <c r="W1" s="276"/>
+      <c r="X1" s="276"/>
+      <c r="Y1" s="276"/>
+      <c r="Z1" s="276"/>
+    </row>
+    <row r="2" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="274"/>
+      <c r="B2" s="275"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
+      <c r="G2" s="275"/>
+      <c r="H2" s="276"/>
+      <c r="I2" s="276"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
+      <c r="L2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
+      <c r="O2" s="276"/>
+      <c r="P2" s="276"/>
+      <c r="Q2" s="276"/>
+      <c r="R2" s="276"/>
+      <c r="S2" s="276"/>
+      <c r="T2" s="276"/>
+      <c r="U2" s="276"/>
+      <c r="V2" s="276"/>
+      <c r="W2" s="276"/>
+      <c r="X2" s="275"/>
+      <c r="Y2" s="275"/>
+      <c r="Z2" s="275"/>
+    </row>
+    <row r="3" spans="1:26" s="80" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="274"/>
+      <c r="B3" s="275"/>
+      <c r="C3" s="275"/>
+      <c r="D3" s="275"/>
+      <c r="E3" s="275"/>
+      <c r="F3" s="275"/>
+      <c r="G3" s="275"/>
+      <c r="H3" s="276"/>
+      <c r="I3" s="276"/>
+      <c r="J3" s="276"/>
+      <c r="K3" s="276"/>
+      <c r="L3" s="276"/>
+      <c r="M3" s="276"/>
+      <c r="N3" s="276"/>
+      <c r="O3" s="276"/>
+      <c r="P3" s="276"/>
+      <c r="Q3" s="276"/>
+      <c r="R3" s="276"/>
+      <c r="S3" s="276"/>
+      <c r="T3" s="276"/>
+      <c r="U3" s="276"/>
+      <c r="V3" s="276"/>
+      <c r="W3" s="276"/>
+      <c r="X3" s="275"/>
+      <c r="Y3" s="275"/>
+      <c r="Z3" s="275"/>
+    </row>
+    <row r="4" spans="1:26" s="80" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="274"/>
+      <c r="B4" s="275"/>
+      <c r="C4" s="277"/>
+      <c r="D4" s="277"/>
+      <c r="E4" s="277"/>
+      <c r="F4" s="277"/>
+      <c r="G4" s="277"/>
+      <c r="H4" s="277"/>
+      <c r="I4" s="277"/>
+      <c r="J4" s="277"/>
+      <c r="K4" s="278"/>
+      <c r="L4" s="278"/>
+      <c r="M4" s="278"/>
+      <c r="N4" s="278"/>
+      <c r="O4" s="278"/>
+      <c r="P4" s="278"/>
+      <c r="Q4" s="278"/>
+      <c r="R4" s="278"/>
+      <c r="S4" s="278"/>
+      <c r="T4" s="278"/>
+      <c r="U4" s="278"/>
+      <c r="V4" s="278"/>
+      <c r="W4" s="279"/>
+      <c r="X4" s="276"/>
+      <c r="Y4" s="276"/>
+      <c r="Z4" s="276"/>
+    </row>
+    <row r="5" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="274"/>
+      <c r="B5" s="275"/>
+      <c r="C5" s="280"/>
+      <c r="D5" s="280"/>
+      <c r="E5" s="280"/>
+      <c r="F5" s="281"/>
+      <c r="G5" s="282" t="s">
+        <v>548</v>
+      </c>
+      <c r="H5" s="281"/>
+      <c r="I5" s="281"/>
+      <c r="J5" s="281"/>
+      <c r="K5" s="281"/>
+      <c r="L5" s="281"/>
+      <c r="M5" s="281"/>
+      <c r="N5" s="281"/>
+      <c r="O5" s="281"/>
+      <c r="P5" s="281"/>
+      <c r="Q5" s="281"/>
+      <c r="R5" s="281"/>
+      <c r="S5" s="283"/>
+      <c r="T5" s="281"/>
+      <c r="U5" s="283"/>
+      <c r="V5" s="283"/>
+      <c r="W5" s="284"/>
+      <c r="X5" s="276"/>
+      <c r="Y5" s="276"/>
+      <c r="Z5" s="276"/>
+    </row>
+    <row r="6" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="274"/>
+      <c r="B6" s="275"/>
+      <c r="C6" s="280"/>
+      <c r="D6" s="280"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="281"/>
+      <c r="G6" s="281"/>
+      <c r="H6" s="281"/>
+      <c r="I6" s="281"/>
+      <c r="J6" s="281"/>
+      <c r="K6" s="281"/>
+      <c r="L6" s="281"/>
+      <c r="M6" s="281"/>
+      <c r="N6" s="281"/>
+      <c r="O6" s="281"/>
+      <c r="P6" s="281"/>
+      <c r="Q6" s="281"/>
+      <c r="R6" s="281"/>
+      <c r="S6" s="283"/>
+      <c r="T6" s="286"/>
+      <c r="U6" s="283"/>
+      <c r="V6" s="283"/>
+      <c r="W6" s="284"/>
+      <c r="X6" s="276"/>
+      <c r="Y6" s="276"/>
+      <c r="Z6" s="276"/>
+    </row>
+    <row r="7" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="274"/>
+      <c r="B7" s="275"/>
+      <c r="C7" s="285"/>
+      <c r="D7" s="280"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="281"/>
+      <c r="G7" s="287" t="s">
+        <v>549</v>
+      </c>
+      <c r="H7" s="281"/>
+      <c r="I7" s="281"/>
+      <c r="J7" s="281"/>
+      <c r="K7" s="281"/>
+      <c r="L7" s="281"/>
+      <c r="M7" s="281"/>
+      <c r="N7" s="281"/>
+      <c r="O7" s="281"/>
+      <c r="P7" s="281"/>
+      <c r="Q7" s="281"/>
+      <c r="R7" s="281"/>
+      <c r="S7" s="283"/>
+      <c r="T7" s="286"/>
+      <c r="U7" s="283"/>
+      <c r="V7" s="283"/>
+      <c r="W7" s="284"/>
+      <c r="X7" s="276"/>
+      <c r="Y7" s="276"/>
+      <c r="Z7" s="276"/>
+    </row>
+    <row r="8" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="274"/>
+      <c r="B8" s="275"/>
+      <c r="C8" s="288"/>
+      <c r="D8" s="280"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="281"/>
+      <c r="G8" s="289"/>
+      <c r="H8" s="281"/>
+      <c r="I8" s="281"/>
+      <c r="J8" s="281"/>
+      <c r="K8" s="281"/>
+      <c r="L8" s="281"/>
+      <c r="M8" s="281"/>
+      <c r="N8" s="281"/>
+      <c r="O8" s="281"/>
+      <c r="P8" s="281"/>
+      <c r="Q8" s="281"/>
+      <c r="R8" s="281"/>
+      <c r="S8" s="283"/>
+      <c r="T8" s="286"/>
+      <c r="U8" s="283"/>
+      <c r="V8" s="283"/>
+      <c r="W8" s="284"/>
+      <c r="X8" s="276"/>
+      <c r="Y8" s="276"/>
+      <c r="Z8" s="276"/>
+    </row>
+    <row r="9" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="274"/>
+      <c r="B9" s="275"/>
+      <c r="C9" s="285"/>
+      <c r="D9" s="285"/>
+      <c r="E9" s="285"/>
+      <c r="F9" s="285"/>
+      <c r="G9" s="285"/>
+      <c r="H9" s="285"/>
+      <c r="I9" s="285"/>
+      <c r="J9" s="458"/>
+      <c r="K9" s="458"/>
+      <c r="L9" s="458"/>
+      <c r="M9" s="458"/>
+      <c r="N9" s="458"/>
+      <c r="O9" s="458"/>
+      <c r="P9" s="458"/>
+      <c r="Q9" s="458"/>
+      <c r="R9" s="458"/>
+      <c r="S9" s="458"/>
+      <c r="T9" s="458"/>
+      <c r="U9" s="458"/>
+      <c r="V9" s="458"/>
+      <c r="W9" s="284"/>
+      <c r="X9" s="276"/>
+      <c r="Y9" s="276"/>
+      <c r="Z9" s="276"/>
+    </row>
+    <row r="10" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="274"/>
+      <c r="B10" s="275"/>
+      <c r="C10" s="285"/>
+      <c r="D10" s="285"/>
+      <c r="E10" s="285"/>
+      <c r="F10" s="285"/>
+      <c r="G10" s="285"/>
+      <c r="H10" s="285"/>
+      <c r="I10" s="285"/>
+      <c r="J10" s="285"/>
+      <c r="K10" s="285"/>
+      <c r="L10" s="458"/>
+      <c r="M10" s="458"/>
+      <c r="N10" s="458"/>
+      <c r="O10" s="458"/>
+      <c r="P10" s="458"/>
+      <c r="Q10" s="458"/>
+      <c r="R10" s="458"/>
+      <c r="S10" s="458"/>
+      <c r="T10" s="458"/>
+      <c r="U10" s="458"/>
+      <c r="V10" s="458"/>
+      <c r="W10" s="284"/>
+      <c r="X10" s="276"/>
+      <c r="Y10" s="276"/>
+      <c r="Z10" s="276"/>
+    </row>
+    <row r="11" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="274"/>
+      <c r="B11" s="275"/>
+      <c r="C11" s="285"/>
+      <c r="D11" s="285"/>
+      <c r="E11" s="285"/>
+      <c r="F11" s="285"/>
+      <c r="G11" s="285"/>
+      <c r="H11" s="285"/>
+      <c r="I11" s="285"/>
+      <c r="J11" s="291"/>
+      <c r="K11" s="291"/>
+      <c r="L11" s="291"/>
+      <c r="M11" s="291"/>
+      <c r="N11" s="291"/>
+      <c r="O11" s="291"/>
+      <c r="P11" s="292"/>
+      <c r="Q11" s="292"/>
+      <c r="R11" s="292"/>
+      <c r="S11" s="458"/>
+      <c r="T11" s="458"/>
+      <c r="U11" s="458"/>
+      <c r="V11" s="458"/>
+      <c r="W11" s="284"/>
+      <c r="X11" s="276"/>
+      <c r="Y11" s="276"/>
+      <c r="Z11" s="276"/>
+    </row>
+    <row r="12" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="274"/>
+      <c r="B12" s="275"/>
+      <c r="C12" s="285"/>
+      <c r="D12" s="285"/>
+      <c r="E12" s="285"/>
+      <c r="F12" s="285"/>
+      <c r="G12" s="285"/>
+      <c r="H12" s="285"/>
+      <c r="I12" s="458"/>
+      <c r="J12" s="291"/>
+      <c r="K12" s="291"/>
+      <c r="L12" s="291"/>
+      <c r="M12" s="291"/>
+      <c r="N12" s="291"/>
+      <c r="O12" s="291"/>
+      <c r="P12" s="292"/>
+      <c r="Q12" s="292"/>
+      <c r="R12" s="292"/>
+      <c r="S12" s="458"/>
+      <c r="T12" s="458"/>
+      <c r="U12" s="458"/>
+      <c r="V12" s="458"/>
+      <c r="W12" s="284"/>
+      <c r="X12" s="276"/>
+      <c r="Y12" s="276"/>
+      <c r="Z12" s="276"/>
+    </row>
+    <row r="13" spans="1:26" s="80" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="274"/>
+      <c r="B13" s="275"/>
+      <c r="C13" s="285"/>
+      <c r="D13" s="285"/>
+      <c r="E13" s="285"/>
+      <c r="F13" s="285"/>
+      <c r="G13" s="285"/>
+      <c r="H13" s="285"/>
+      <c r="I13" s="285"/>
+      <c r="J13" s="291"/>
+      <c r="K13" s="291"/>
+      <c r="L13" s="292"/>
+      <c r="M13" s="292"/>
+      <c r="N13" s="292"/>
+      <c r="O13" s="292"/>
+      <c r="P13" s="292"/>
+      <c r="Q13" s="292"/>
+      <c r="R13" s="292"/>
+      <c r="S13" s="458"/>
+      <c r="T13" s="458"/>
+      <c r="U13" s="458"/>
+      <c r="V13" s="458"/>
+      <c r="W13" s="284"/>
+      <c r="X13" s="276"/>
+      <c r="Y13" s="276"/>
+      <c r="Z13" s="276"/>
+    </row>
+    <row r="14" spans="1:26" s="80" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="274"/>
+      <c r="B14" s="275"/>
+      <c r="C14" s="285"/>
+      <c r="D14" s="285"/>
+      <c r="E14" s="285"/>
+      <c r="F14" s="293"/>
+      <c r="G14" s="294"/>
+      <c r="H14" s="294"/>
+      <c r="I14" s="222"/>
+      <c r="J14" s="324"/>
+      <c r="K14" s="324"/>
+      <c r="L14" s="324"/>
+      <c r="M14" s="324"/>
+      <c r="N14" s="324"/>
+      <c r="O14" s="324"/>
+      <c r="P14" s="295"/>
+      <c r="Q14" s="295"/>
+      <c r="R14" s="295"/>
+      <c r="S14" s="295"/>
+      <c r="T14" s="295"/>
+      <c r="U14" s="295"/>
+      <c r="V14" s="296"/>
+      <c r="W14" s="284"/>
+      <c r="X14" s="276"/>
+      <c r="Y14" s="276"/>
+      <c r="Z14" s="276"/>
+    </row>
+    <row r="15" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="274"/>
+      <c r="B15" s="275"/>
+      <c r="C15" s="285"/>
+      <c r="D15" s="285"/>
+      <c r="E15" s="285"/>
+      <c r="F15" s="293"/>
+      <c r="G15" s="242"/>
+      <c r="H15" s="242"/>
+      <c r="I15" s="239"/>
+      <c r="J15" s="240"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="298"/>
+      <c r="Q15" s="298"/>
+      <c r="R15" s="298"/>
+      <c r="S15" s="298"/>
+      <c r="T15" s="298"/>
+      <c r="U15" s="298"/>
+      <c r="V15" s="296"/>
+      <c r="W15" s="284"/>
+      <c r="X15" s="276"/>
+      <c r="Y15" s="276"/>
+      <c r="Z15" s="276"/>
+    </row>
+    <row r="16" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="274"/>
+      <c r="B16" s="275"/>
+      <c r="C16" s="285"/>
+      <c r="D16" s="285"/>
+      <c r="E16" s="285"/>
+      <c r="F16" s="293"/>
+      <c r="G16" s="459" t="s">
+        <v>550</v>
+      </c>
+      <c r="H16" s="242"/>
+      <c r="I16" s="239"/>
+      <c r="J16" s="479" t="s">
+        <v>552</v>
+      </c>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="298"/>
+      <c r="Q16" s="298"/>
+      <c r="R16" s="298"/>
+      <c r="S16" s="298"/>
+      <c r="T16" s="298"/>
+      <c r="U16" s="298"/>
+      <c r="V16" s="296"/>
+      <c r="W16" s="284"/>
+      <c r="X16" s="276"/>
+      <c r="Y16" s="276"/>
+      <c r="Z16" s="276"/>
+    </row>
+    <row r="17" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="274"/>
+      <c r="B17" s="275"/>
+      <c r="C17" s="285"/>
+      <c r="D17" s="285"/>
+      <c r="E17" s="285"/>
+      <c r="F17" s="293"/>
+      <c r="G17" s="242" t="s">
+        <v>551</v>
+      </c>
+      <c r="H17" s="242"/>
+      <c r="I17" s="239"/>
+      <c r="J17" s="242" t="s">
+        <v>553</v>
+      </c>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="298"/>
+      <c r="Q17" s="298"/>
+      <c r="R17" s="298"/>
+      <c r="S17" s="298"/>
+      <c r="T17" s="298"/>
+      <c r="U17" s="298"/>
+      <c r="V17" s="296"/>
+      <c r="W17" s="284"/>
+      <c r="X17" s="276"/>
+      <c r="Y17" s="276"/>
+      <c r="Z17" s="276"/>
+    </row>
+    <row r="18" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="274"/>
+      <c r="B18" s="275"/>
+      <c r="C18" s="285"/>
+      <c r="D18" s="285"/>
+      <c r="E18" s="285"/>
+      <c r="F18" s="293"/>
+      <c r="G18" s="416" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="242"/>
+      <c r="I18" s="239"/>
+      <c r="J18" s="416" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="298"/>
+      <c r="Q18" s="298"/>
+      <c r="R18" s="298"/>
+      <c r="S18" s="298"/>
+      <c r="T18" s="298"/>
+      <c r="U18" s="298"/>
+      <c r="V18" s="296"/>
+      <c r="W18" s="284"/>
+      <c r="X18" s="276"/>
+      <c r="Y18" s="276"/>
+      <c r="Z18" s="276"/>
+    </row>
+    <row r="19" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="274"/>
+      <c r="B19" s="275"/>
+      <c r="C19" s="285"/>
+      <c r="D19" s="285"/>
+      <c r="E19" s="285"/>
+      <c r="F19" s="293"/>
+      <c r="G19" s="242"/>
+      <c r="H19" s="242"/>
+      <c r="I19" s="239"/>
+      <c r="J19" s="241"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="298"/>
+      <c r="Q19" s="298"/>
+      <c r="R19" s="298"/>
+      <c r="S19" s="298"/>
+      <c r="T19" s="298"/>
+      <c r="U19" s="298"/>
+      <c r="V19" s="296"/>
+      <c r="W19" s="284"/>
+      <c r="X19" s="276"/>
+      <c r="Y19" s="276"/>
+      <c r="Z19" s="276"/>
+    </row>
+    <row r="20" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="274"/>
+      <c r="B20" s="275"/>
+      <c r="C20" s="285"/>
+      <c r="D20" s="285"/>
+      <c r="E20" s="285"/>
+      <c r="F20" s="293"/>
+      <c r="G20" s="242"/>
+      <c r="H20" s="242"/>
+      <c r="I20" s="239"/>
+      <c r="J20" s="241"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="298"/>
+      <c r="Q20" s="298"/>
+      <c r="R20" s="298"/>
+      <c r="S20" s="298"/>
+      <c r="T20" s="298"/>
+      <c r="U20" s="298"/>
+      <c r="V20" s="296"/>
+      <c r="W20" s="284"/>
+      <c r="X20" s="276"/>
+      <c r="Y20" s="276"/>
+      <c r="Z20" s="276"/>
+    </row>
+    <row r="21" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="274"/>
+      <c r="B21" s="275"/>
+      <c r="C21" s="285"/>
+      <c r="D21" s="285"/>
+      <c r="E21" s="285"/>
+      <c r="F21" s="293"/>
+      <c r="G21" s="242"/>
+      <c r="H21" s="242"/>
+      <c r="I21" s="239"/>
+      <c r="J21" s="241"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="298"/>
+      <c r="Q21" s="298"/>
+      <c r="R21" s="298"/>
+      <c r="S21" s="298"/>
+      <c r="T21" s="298"/>
+      <c r="U21" s="298"/>
+      <c r="V21" s="296"/>
+      <c r="W21" s="284"/>
+      <c r="X21" s="276"/>
+      <c r="Y21" s="276"/>
+      <c r="Z21" s="276"/>
+    </row>
+    <row r="22" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="274"/>
+      <c r="B22" s="275"/>
+      <c r="C22" s="285"/>
+      <c r="D22" s="285"/>
+      <c r="E22" s="285"/>
+      <c r="F22" s="293"/>
+      <c r="G22" s="242"/>
+      <c r="H22" s="242"/>
+      <c r="I22" s="239"/>
+      <c r="J22" s="241"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="298"/>
+      <c r="Q22" s="298"/>
+      <c r="R22" s="298"/>
+      <c r="S22" s="298"/>
+      <c r="T22" s="298"/>
+      <c r="U22" s="298"/>
+      <c r="V22" s="296"/>
+      <c r="W22" s="284"/>
+      <c r="X22" s="276"/>
+      <c r="Y22" s="276"/>
+      <c r="Z22" s="276"/>
+    </row>
+    <row r="23" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="274"/>
+      <c r="B23" s="275"/>
+      <c r="C23" s="285"/>
+      <c r="D23" s="285"/>
+      <c r="E23" s="285"/>
+      <c r="F23" s="293"/>
+      <c r="G23" s="242"/>
+      <c r="H23" s="242"/>
+      <c r="I23" s="239"/>
+      <c r="J23" s="240"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="298"/>
+      <c r="Q23" s="298"/>
+      <c r="R23" s="298"/>
+      <c r="S23" s="298"/>
+      <c r="T23" s="298"/>
+      <c r="U23" s="298"/>
+      <c r="V23" s="296"/>
+      <c r="W23" s="284"/>
+      <c r="X23" s="276"/>
+      <c r="Y23" s="276"/>
+      <c r="Z23" s="276"/>
+    </row>
+    <row r="24" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="274"/>
+      <c r="B24" s="275"/>
+      <c r="C24" s="285"/>
+      <c r="D24" s="285"/>
+      <c r="E24" s="285"/>
+      <c r="F24" s="293"/>
+      <c r="G24" s="242"/>
+      <c r="H24" s="242"/>
+      <c r="I24" s="239"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="O24" s="53"/>
+      <c r="P24" s="298"/>
+      <c r="Q24" s="298"/>
+      <c r="R24" s="298"/>
+      <c r="S24" s="298"/>
+      <c r="T24" s="298"/>
+      <c r="U24" s="298"/>
+      <c r="V24" s="296"/>
+      <c r="W24" s="284"/>
+      <c r="X24" s="276"/>
+      <c r="Y24" s="276"/>
+      <c r="Z24" s="276"/>
+    </row>
+    <row r="25" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="274"/>
+      <c r="B25" s="275"/>
+      <c r="C25" s="285"/>
+      <c r="D25" s="285"/>
+      <c r="E25" s="285"/>
+      <c r="F25" s="293"/>
+      <c r="G25" s="242"/>
+      <c r="H25" s="242"/>
+      <c r="I25" s="239"/>
+      <c r="J25" s="241"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="298"/>
+      <c r="Q25" s="298"/>
+      <c r="R25" s="298"/>
+      <c r="S25" s="298"/>
+      <c r="T25" s="298"/>
+      <c r="U25" s="298"/>
+      <c r="V25" s="296"/>
+      <c r="W25" s="284"/>
+      <c r="X25" s="276"/>
+      <c r="Y25" s="276"/>
+      <c r="Z25" s="276"/>
+    </row>
+    <row r="26" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="274"/>
+      <c r="B26" s="275"/>
+      <c r="C26" s="285"/>
+      <c r="D26" s="285"/>
+      <c r="E26" s="285"/>
+      <c r="F26" s="293"/>
+      <c r="G26" s="242"/>
+      <c r="H26" s="242"/>
+      <c r="I26" s="239"/>
+      <c r="J26" s="241"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="298"/>
+      <c r="Q26" s="298"/>
+      <c r="R26" s="298"/>
+      <c r="S26" s="298"/>
+      <c r="T26" s="298"/>
+      <c r="U26" s="298"/>
+      <c r="V26" s="296"/>
+      <c r="W26" s="284"/>
+      <c r="X26" s="276"/>
+      <c r="Y26" s="276"/>
+      <c r="Z26" s="276"/>
+    </row>
+    <row r="27" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="274"/>
+      <c r="B27" s="275"/>
+      <c r="C27" s="285"/>
+      <c r="D27" s="285"/>
+      <c r="E27" s="285"/>
+      <c r="F27" s="293"/>
+      <c r="G27" s="238"/>
+      <c r="H27" s="242"/>
+      <c r="I27" s="239"/>
+      <c r="J27" s="241"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="298"/>
+      <c r="Q27" s="298"/>
+      <c r="R27" s="298"/>
+      <c r="S27" s="298"/>
+      <c r="T27" s="298"/>
+      <c r="U27" s="298"/>
+      <c r="V27" s="296"/>
+      <c r="W27" s="284"/>
+      <c r="X27" s="276"/>
+      <c r="Y27" s="276"/>
+      <c r="Z27" s="276"/>
+    </row>
+    <row r="28" spans="1:26" s="80" customFormat="1" ht="5.0999999999999996" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="274"/>
+      <c r="B28" s="275"/>
+      <c r="C28" s="285"/>
+      <c r="D28" s="285"/>
+      <c r="E28" s="285"/>
+      <c r="F28" s="300"/>
+      <c r="G28" s="303"/>
+      <c r="H28" s="303"/>
+      <c r="I28" s="303"/>
+      <c r="J28" s="304"/>
+      <c r="K28" s="304"/>
+      <c r="L28" s="304"/>
+      <c r="M28" s="304"/>
+      <c r="N28" s="304"/>
+      <c r="O28" s="304"/>
+      <c r="P28" s="304"/>
+      <c r="Q28" s="304"/>
+      <c r="R28" s="304"/>
+      <c r="S28" s="304"/>
+      <c r="T28" s="304"/>
+      <c r="U28" s="304"/>
+      <c r="V28" s="296"/>
+      <c r="W28" s="284"/>
+      <c r="X28" s="276"/>
+      <c r="Y28" s="276"/>
+      <c r="Z28" s="276"/>
+    </row>
+    <row r="29" spans="1:26" s="80" customFormat="1" ht="24.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="274"/>
+      <c r="B29" s="275"/>
+      <c r="C29" s="305"/>
+      <c r="D29" s="305"/>
+      <c r="E29" s="305"/>
+      <c r="F29" s="305"/>
+      <c r="G29" s="306"/>
+      <c r="H29" s="305"/>
+      <c r="I29" s="305"/>
+      <c r="J29" s="305"/>
+      <c r="K29" s="305"/>
+      <c r="L29" s="305"/>
+      <c r="M29" s="305"/>
+      <c r="N29" s="305"/>
+      <c r="O29" s="305"/>
+      <c r="P29" s="305"/>
+      <c r="Q29" s="305"/>
+      <c r="R29" s="305"/>
+      <c r="S29" s="305"/>
+      <c r="T29" s="305"/>
+      <c r="U29" s="305"/>
+      <c r="V29" s="305"/>
+      <c r="W29" s="307"/>
+      <c r="X29" s="276"/>
+      <c r="Y29" s="276"/>
+      <c r="Z29" s="276"/>
+    </row>
+    <row r="30" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="274"/>
+      <c r="B30" s="275"/>
+      <c r="C30" s="275"/>
+      <c r="D30" s="275"/>
+      <c r="E30" s="275"/>
+      <c r="F30" s="276"/>
+      <c r="G30" s="276"/>
+      <c r="H30" s="276"/>
+      <c r="I30" s="276"/>
+      <c r="J30" s="276"/>
+      <c r="K30" s="276"/>
+      <c r="L30" s="276"/>
+      <c r="M30" s="276"/>
+      <c r="N30" s="276"/>
+      <c r="O30" s="276"/>
+      <c r="P30" s="276"/>
+      <c r="Q30" s="276"/>
+      <c r="R30" s="276"/>
+      <c r="S30" s="276"/>
+      <c r="T30" s="276"/>
+      <c r="U30" s="276"/>
+      <c r="V30" s="276"/>
+      <c r="W30" s="276"/>
+      <c r="X30" s="276"/>
+      <c r="Y30" s="276"/>
+      <c r="Z30" s="276"/>
+    </row>
+    <row r="31" spans="1:26" s="80" customFormat="1" ht="12" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="274"/>
+      <c r="B31" s="275"/>
+      <c r="C31" s="275"/>
+      <c r="D31" s="275"/>
+      <c r="E31" s="275"/>
+      <c r="F31" s="276"/>
+      <c r="G31" s="276"/>
+      <c r="H31" s="276"/>
+      <c r="I31" s="276"/>
+      <c r="J31" s="276"/>
+      <c r="K31" s="276"/>
+      <c r="L31" s="276"/>
+      <c r="M31" s="276"/>
+      <c r="N31" s="276"/>
+      <c r="O31" s="276"/>
+      <c r="P31" s="276"/>
+      <c r="Q31" s="276"/>
+      <c r="R31" s="276"/>
+      <c r="S31" s="276"/>
+      <c r="T31" s="276"/>
+      <c r="U31" s="276"/>
+      <c r="V31" s="276"/>
+      <c r="W31" s="276"/>
+      <c r="X31" s="276"/>
+      <c r="Y31" s="276"/>
+      <c r="Z31" s="276"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AB1FD0-C06F-43E2-AD4D-7EBD7CDF886A}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -17515,21 +18435,21 @@
       <c r="E46" s="112"/>
       <c r="F46" s="114"/>
       <c r="G46" s="123"/>
-      <c r="H46" s="458" t="s">
+      <c r="H46" s="460" t="s">
         <v>161</v>
       </c>
-      <c r="I46" s="459"/>
-      <c r="J46" s="459"/>
-      <c r="K46" s="459"/>
-      <c r="L46" s="459"/>
-      <c r="M46" s="459"/>
-      <c r="N46" s="459"/>
-      <c r="O46" s="459"/>
-      <c r="P46" s="459"/>
-      <c r="Q46" s="459"/>
-      <c r="R46" s="459"/>
-      <c r="S46" s="459"/>
-      <c r="T46" s="460"/>
+      <c r="I46" s="461"/>
+      <c r="J46" s="461"/>
+      <c r="K46" s="461"/>
+      <c r="L46" s="461"/>
+      <c r="M46" s="461"/>
+      <c r="N46" s="461"/>
+      <c r="O46" s="461"/>
+      <c r="P46" s="461"/>
+      <c r="Q46" s="461"/>
+      <c r="R46" s="461"/>
+      <c r="S46" s="461"/>
+      <c r="T46" s="462"/>
       <c r="U46" s="123"/>
       <c r="V46" s="114"/>
       <c r="W46" s="94"/>
@@ -17543,19 +18463,19 @@
       <c r="E47" s="112"/>
       <c r="F47" s="114"/>
       <c r="G47" s="123"/>
-      <c r="H47" s="461"/>
-      <c r="I47" s="462"/>
-      <c r="J47" s="462"/>
-      <c r="K47" s="462"/>
-      <c r="L47" s="462"/>
-      <c r="M47" s="462"/>
-      <c r="N47" s="462"/>
-      <c r="O47" s="462"/>
-      <c r="P47" s="462"/>
-      <c r="Q47" s="462"/>
-      <c r="R47" s="462"/>
-      <c r="S47" s="462"/>
-      <c r="T47" s="463"/>
+      <c r="H47" s="463"/>
+      <c r="I47" s="464"/>
+      <c r="J47" s="464"/>
+      <c r="K47" s="464"/>
+      <c r="L47" s="464"/>
+      <c r="M47" s="464"/>
+      <c r="N47" s="464"/>
+      <c r="O47" s="464"/>
+      <c r="P47" s="464"/>
+      <c r="Q47" s="464"/>
+      <c r="R47" s="464"/>
+      <c r="S47" s="464"/>
+      <c r="T47" s="465"/>
       <c r="U47" s="123"/>
       <c r="V47" s="114"/>
       <c r="W47" s="94"/>
@@ -17569,19 +18489,19 @@
       <c r="E48" s="112"/>
       <c r="F48" s="114"/>
       <c r="G48" s="123"/>
-      <c r="H48" s="461"/>
-      <c r="I48" s="462"/>
-      <c r="J48" s="462"/>
-      <c r="K48" s="462"/>
-      <c r="L48" s="462"/>
-      <c r="M48" s="462"/>
-      <c r="N48" s="462"/>
-      <c r="O48" s="462"/>
-      <c r="P48" s="462"/>
-      <c r="Q48" s="462"/>
-      <c r="R48" s="462"/>
-      <c r="S48" s="462"/>
-      <c r="T48" s="463"/>
+      <c r="H48" s="463"/>
+      <c r="I48" s="464"/>
+      <c r="J48" s="464"/>
+      <c r="K48" s="464"/>
+      <c r="L48" s="464"/>
+      <c r="M48" s="464"/>
+      <c r="N48" s="464"/>
+      <c r="O48" s="464"/>
+      <c r="P48" s="464"/>
+      <c r="Q48" s="464"/>
+      <c r="R48" s="464"/>
+      <c r="S48" s="464"/>
+      <c r="T48" s="465"/>
       <c r="U48" s="123"/>
       <c r="V48" s="114"/>
       <c r="W48" s="94"/>
@@ -17595,19 +18515,19 @@
       <c r="E49" s="112"/>
       <c r="F49" s="114"/>
       <c r="G49" s="123"/>
-      <c r="H49" s="464"/>
-      <c r="I49" s="465"/>
-      <c r="J49" s="465"/>
-      <c r="K49" s="465"/>
-      <c r="L49" s="465"/>
-      <c r="M49" s="465"/>
-      <c r="N49" s="465"/>
-      <c r="O49" s="465"/>
-      <c r="P49" s="465"/>
-      <c r="Q49" s="465"/>
-      <c r="R49" s="465"/>
-      <c r="S49" s="465"/>
-      <c r="T49" s="466"/>
+      <c r="H49" s="466"/>
+      <c r="I49" s="467"/>
+      <c r="J49" s="467"/>
+      <c r="K49" s="467"/>
+      <c r="L49" s="467"/>
+      <c r="M49" s="467"/>
+      <c r="N49" s="467"/>
+      <c r="O49" s="467"/>
+      <c r="P49" s="467"/>
+      <c r="Q49" s="467"/>
+      <c r="R49" s="467"/>
+      <c r="S49" s="467"/>
+      <c r="T49" s="468"/>
       <c r="U49" s="123"/>
       <c r="V49" s="114"/>
       <c r="W49" s="94"/>
@@ -17649,21 +18569,21 @@
       <c r="E51" s="112"/>
       <c r="F51" s="114"/>
       <c r="G51" s="116"/>
-      <c r="H51" s="469" t="s">
+      <c r="H51" s="471" t="s">
         <v>521</v>
       </c>
-      <c r="I51" s="470"/>
-      <c r="J51" s="470"/>
-      <c r="K51" s="470"/>
-      <c r="L51" s="470"/>
-      <c r="M51" s="470"/>
-      <c r="N51" s="470"/>
-      <c r="O51" s="470"/>
-      <c r="P51" s="470"/>
-      <c r="Q51" s="470"/>
-      <c r="R51" s="470"/>
-      <c r="S51" s="470"/>
-      <c r="T51" s="471"/>
+      <c r="I51" s="472"/>
+      <c r="J51" s="472"/>
+      <c r="K51" s="472"/>
+      <c r="L51" s="472"/>
+      <c r="M51" s="472"/>
+      <c r="N51" s="472"/>
+      <c r="O51" s="472"/>
+      <c r="P51" s="472"/>
+      <c r="Q51" s="472"/>
+      <c r="R51" s="472"/>
+      <c r="S51" s="472"/>
+      <c r="T51" s="473"/>
       <c r="U51" s="116"/>
       <c r="V51" s="114"/>
       <c r="W51" s="284"/>
@@ -32607,9 +33527,9 @@
       <c r="I320" s="219"/>
       <c r="J320" s="219"/>
       <c r="K320" s="111"/>
-      <c r="L320" s="467"/>
-      <c r="M320" s="468"/>
-      <c r="N320" s="468"/>
+      <c r="L320" s="469"/>
+      <c r="M320" s="470"/>
+      <c r="N320" s="470"/>
       <c r="O320" s="111"/>
       <c r="P320" s="111"/>
       <c r="Q320" s="111"/>
@@ -41581,18 +42501,18 @@
       <c r="E112" s="16"/>
       <c r="F112" s="16"/>
       <c r="G112" s="16"/>
-      <c r="H112" s="474" t="s">
+      <c r="H112" s="476" t="s">
         <v>487</v>
       </c>
-      <c r="I112" s="474"/>
-      <c r="J112" s="474"/>
+      <c r="I112" s="476"/>
+      <c r="J112" s="476"/>
       <c r="K112" s="348"/>
       <c r="L112" s="365"/>
-      <c r="M112" s="473" t="s">
+      <c r="M112" s="475" t="s">
         <v>357</v>
       </c>
-      <c r="N112" s="473"/>
-      <c r="O112" s="473"/>
+      <c r="N112" s="475"/>
+      <c r="O112" s="475"/>
       <c r="P112" s="365"/>
       <c r="Q112" s="365"/>
       <c r="R112" s="365"/>
@@ -52084,7 +53004,7 @@
       <c r="E402" s="16"/>
       <c r="F402" s="16"/>
       <c r="G402" s="16"/>
-      <c r="H402" s="472"/>
+      <c r="H402" s="474"/>
       <c r="I402" s="16"/>
       <c r="J402" s="16"/>
       <c r="K402" s="21"/>
@@ -52112,7 +53032,7 @@
       <c r="E403" s="16"/>
       <c r="F403" s="16"/>
       <c r="G403" s="16"/>
-      <c r="H403" s="472"/>
+      <c r="H403" s="474"/>
       <c r="I403" s="16"/>
       <c r="J403" s="22" t="s">
         <v>41</v>
@@ -52146,7 +53066,7 @@
       <c r="G404" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="H404" s="472"/>
+      <c r="H404" s="474"/>
       <c r="I404" s="16"/>
       <c r="J404" s="291" t="s">
         <v>531</v>
@@ -58199,10 +59119,10 @@
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
-      <c r="F68" s="475" t="s">
+      <c r="F68" s="477" t="s">
         <v>347</v>
       </c>
-      <c r="G68" s="476"/>
+      <c r="G68" s="478"/>
       <c r="H68" s="22"/>
       <c r="I68" s="22" t="s">
         <v>348</v>
@@ -59034,8 +59954,8 @@
       <c r="B96" s="5"/>
       <c r="C96" s="16"/>
       <c r="D96" s="16"/>
-      <c r="E96" s="475"/>
-      <c r="F96" s="476"/>
+      <c r="E96" s="477"/>
+      <c r="F96" s="478"/>
       <c r="G96" s="22" t="s">
         <v>354</v>
       </c>

</xml_diff>